<commit_message>
Changes to database to make it work.
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni-my.sharepoint.com/personal/prana001_student_otago_ac_nz/Documents/Year 3/COSC345/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\Downloads\COSC345\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="884" documentId="8_{EFA227FA-5189-4934-925A-773C6139C4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FEE6C26-2A83-4DFC-A668-138482A50FCF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88357CA3-329D-4286-9175-88C79487136A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
   <sheets>
     <sheet name="COSC345_Recipes" sheetId="1" r:id="rId1"/>
@@ -928,7 +928,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,31 +963,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF374151"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF374151"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1003,7 +985,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1026,14 +1008,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1372,20 +1348,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
   <dimension ref="A1:CM229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="53" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="79.5703125" customWidth="1"/>
-    <col min="5" max="5" width="74.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="79.5546875" customWidth="1"/>
+    <col min="5" max="5" width="74.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="57.75">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1431,7 +1407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="332.25">
+    <row r="3" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -1454,7 +1430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="87">
+    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1477,7 +1453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="201.75">
+    <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="318">
+    <row r="6" spans="1:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1523,7 +1499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="260.25">
+    <row r="7" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1546,7 +1522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="390">
+    <row r="8" spans="1:7" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -1569,7 +1545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="245.25">
+    <row r="9" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
@@ -1592,7 +1568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="361.5">
+    <row r="10" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
@@ -1615,7 +1591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="216.75">
+    <row r="11" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>53</v>
       </c>
@@ -1638,7 +1614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="332.25">
+    <row r="12" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
@@ -1661,7 +1637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="318">
+    <row r="13" spans="1:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
@@ -1684,7 +1660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="361.5">
+    <row r="14" spans="1:7" ht="360" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>66</v>
       </c>
@@ -1707,7 +1683,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="216.75">
+    <row r="15" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>70</v>
       </c>
@@ -1730,7 +1706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="409.6">
+    <row r="16" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -1753,7 +1729,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:91" ht="144.75">
+    <row r="17" spans="1:91" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>80</v>
       </c>
@@ -1776,7 +1752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:91" ht="332.25">
+    <row r="18" spans="1:91" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>84</v>
       </c>
@@ -1799,7 +1775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:91" ht="332.25">
+    <row r="19" spans="1:91" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>89</v>
       </c>
@@ -1822,7 +1798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:91" ht="29.25">
+    <row r="20" spans="1:91" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>94</v>
       </c>
@@ -1845,7 +1821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:91" ht="154.5" customHeight="1">
+    <row r="21" spans="1:91" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>99</v>
       </c>
@@ -1868,7 +1844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:91" ht="169.5" customHeight="1">
+    <row r="22" spans="1:91" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>103</v>
       </c>
@@ -1891,20 +1867,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:91" ht="237" customHeight="1">
+    <row r="23" spans="1:91" ht="237" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>112</v>
       </c>
       <c r="F23" s="3">
@@ -1914,7 +1890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:91" ht="236.25" customHeight="1">
+    <row r="24" spans="1:91" ht="236.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>113</v>
       </c>
@@ -1927,7 +1903,7 @@
       <c r="D24" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="3" t="s">
         <v>117</v>
       </c>
       <c r="F24" s="6">
@@ -1962,7 +1938,7 @@
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
     </row>
-    <row r="25" spans="1:91" ht="201.75">
+    <row r="25" spans="1:91" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>118</v>
       </c>
@@ -1975,7 +1951,7 @@
       <c r="D25" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="3" t="s">
         <v>122</v>
       </c>
       <c r="F25" s="1">
@@ -2010,7 +1986,7 @@
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
     </row>
-    <row r="26" spans="1:91" ht="153.75" customHeight="1">
+    <row r="26" spans="1:91" ht="153.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>123</v>
       </c>
@@ -2023,7 +1999,7 @@
       <c r="D26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F26" s="1">
@@ -2117,7 +2093,7 @@
       <c r="CL26" s="1"/>
       <c r="CM26" s="1"/>
     </row>
-    <row r="27" spans="1:91" ht="72.75">
+    <row r="27" spans="1:91" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>128</v>
       </c>
@@ -2130,7 +2106,7 @@
       <c r="D27" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F27" s="1">
@@ -2224,7 +2200,7 @@
       <c r="CL27" s="1"/>
       <c r="CM27" s="1"/>
     </row>
-    <row r="28" spans="1:91" ht="260.25">
+    <row r="28" spans="1:91" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>133</v>
       </c>
@@ -2237,7 +2213,7 @@
       <c r="D28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F28" s="1">
@@ -2331,7 +2307,7 @@
       <c r="CL28" s="1"/>
       <c r="CM28" s="1"/>
     </row>
-    <row r="29" spans="1:91" ht="130.5">
+    <row r="29" spans="1:91" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>138</v>
       </c>
@@ -2344,7 +2320,7 @@
       <c r="D29" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="3" t="s">
         <v>142</v>
       </c>
       <c r="F29" s="1">
@@ -2438,7 +2414,7 @@
       <c r="CL29" s="1"/>
       <c r="CM29" s="1"/>
     </row>
-    <row r="30" spans="1:91" ht="115.5">
+    <row r="30" spans="1:91" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>143</v>
       </c>
@@ -2451,7 +2427,7 @@
       <c r="D30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="3" t="s">
         <v>146</v>
       </c>
       <c r="F30" s="1">
@@ -2545,7 +2521,7 @@
       <c r="CL30" s="1"/>
       <c r="CM30" s="1"/>
     </row>
-    <row r="31" spans="1:91" ht="57.75">
+    <row r="31" spans="1:91" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>147</v>
       </c>
@@ -2558,7 +2534,7 @@
       <c r="D31" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F31" s="1">
@@ -2652,7 +2628,7 @@
       <c r="CL31" s="1"/>
       <c r="CM31" s="1"/>
     </row>
-    <row r="32" spans="1:91" ht="225" customHeight="1">
+    <row r="32" spans="1:91" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>152</v>
       </c>
@@ -2665,7 +2641,7 @@
       <c r="D32" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="3" t="s">
         <v>156</v>
       </c>
       <c r="F32" s="1">
@@ -2759,7 +2735,7 @@
       <c r="CL32" s="1"/>
       <c r="CM32" s="1"/>
     </row>
-    <row r="33" spans="1:91" ht="216.75">
+    <row r="33" spans="1:91" ht="216" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>157</v>
       </c>
@@ -2772,7 +2748,7 @@
       <c r="D33" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="3" t="s">
         <v>160</v>
       </c>
       <c r="F33" s="1">
@@ -2866,7 +2842,7 @@
       <c r="CL33" s="1"/>
       <c r="CM33" s="1"/>
     </row>
-    <row r="34" spans="1:91" ht="231">
+    <row r="34" spans="1:91" ht="216" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>161</v>
       </c>
@@ -2879,7 +2855,7 @@
       <c r="D34" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="3" t="s">
         <v>164</v>
       </c>
       <c r="F34" s="1">
@@ -2973,7 +2949,7 @@
       <c r="CL34" s="1"/>
       <c r="CM34" s="1"/>
     </row>
-    <row r="35" spans="1:91" ht="57.75">
+    <row r="35" spans="1:91" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>165</v>
       </c>
@@ -2986,7 +2962,7 @@
       <c r="D35" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="3" t="s">
         <v>169</v>
       </c>
       <c r="F35" s="1">
@@ -3080,7 +3056,7 @@
       <c r="CL35" s="1"/>
       <c r="CM35" s="1"/>
     </row>
-    <row r="36" spans="1:91" ht="57.75">
+    <row r="36" spans="1:91" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>170</v>
       </c>
@@ -3093,7 +3069,7 @@
       <c r="D36" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="3" t="s">
         <v>172</v>
       </c>
       <c r="F36" s="1">
@@ -3187,7 +3163,7 @@
       <c r="CL36" s="1"/>
       <c r="CM36" s="1"/>
     </row>
-    <row r="37" spans="1:91" ht="274.5">
+    <row r="37" spans="1:91" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>173</v>
       </c>
@@ -3200,7 +3176,7 @@
       <c r="D37" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="3" t="s">
         <v>177</v>
       </c>
       <c r="F37" s="1">
@@ -3294,7 +3270,7 @@
       <c r="CL37" s="1"/>
       <c r="CM37" s="1"/>
     </row>
-    <row r="38" spans="1:91" ht="188.25">
+    <row r="38" spans="1:91" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>178</v>
       </c>
@@ -3307,7 +3283,7 @@
       <c r="D38" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="3" t="s">
         <v>181</v>
       </c>
       <c r="F38" s="1">
@@ -3401,7 +3377,7 @@
       <c r="CL38" s="1"/>
       <c r="CM38" s="1"/>
     </row>
-    <row r="39" spans="1:91" ht="159">
+    <row r="39" spans="1:91" ht="144" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>182</v>
       </c>
@@ -3414,7 +3390,7 @@
       <c r="D39" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="3" t="s">
         <v>185</v>
       </c>
       <c r="F39" s="1">
@@ -3508,7 +3484,7 @@
       <c r="CL39" s="1"/>
       <c r="CM39" s="1"/>
     </row>
-    <row r="40" spans="1:91" ht="144.75">
+    <row r="40" spans="1:91" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>186</v>
       </c>
@@ -3521,7 +3497,7 @@
       <c r="D40" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="3" t="s">
         <v>190</v>
       </c>
       <c r="F40" s="1">
@@ -3615,7 +3591,7 @@
       <c r="CL40" s="1"/>
       <c r="CM40" s="1"/>
     </row>
-    <row r="41" spans="1:91" ht="130.5">
+    <row r="41" spans="1:91" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>191</v>
       </c>
@@ -3628,7 +3604,7 @@
       <c r="D41" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="3" t="s">
         <v>195</v>
       </c>
       <c r="F41" s="1">
@@ -3722,7 +3698,7 @@
       <c r="CL41" s="1"/>
       <c r="CM41" s="1"/>
     </row>
-    <row r="42" spans="1:91" ht="57.75">
+    <row r="42" spans="1:91" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>196</v>
       </c>
@@ -3735,7 +3711,7 @@
       <c r="D42" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="3" t="s">
         <v>200</v>
       </c>
       <c r="F42" s="1">
@@ -3829,7 +3805,7 @@
       <c r="CL42" s="1"/>
       <c r="CM42" s="1"/>
     </row>
-    <row r="43" spans="1:91" ht="260.25">
+    <row r="43" spans="1:91" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>201</v>
       </c>
@@ -3842,7 +3818,7 @@
       <c r="D43" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="3" t="s">
         <v>205</v>
       </c>
       <c r="F43" s="1">
@@ -3936,7 +3912,7 @@
       <c r="CL43" s="1"/>
       <c r="CM43" s="1"/>
     </row>
-    <row r="44" spans="1:91" ht="260.25">
+    <row r="44" spans="1:91" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>206</v>
       </c>
@@ -3949,7 +3925,7 @@
       <c r="D44" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="3" t="s">
         <v>209</v>
       </c>
       <c r="F44" s="1">
@@ -4043,7 +4019,7 @@
       <c r="CL44" s="1"/>
       <c r="CM44" s="1"/>
     </row>
-    <row r="45" spans="1:91" ht="409.6">
+    <row r="45" spans="1:91" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>210</v>
       </c>
@@ -4056,7 +4032,7 @@
       <c r="D45" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F45" s="1">
@@ -4150,7 +4126,7 @@
       <c r="CL45" s="1"/>
       <c r="CM45" s="1"/>
     </row>
-    <row r="46" spans="1:91" ht="288.75">
+    <row r="46" spans="1:91" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>214</v>
       </c>
@@ -4163,7 +4139,7 @@
       <c r="D46" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="3" t="s">
         <v>217</v>
       </c>
       <c r="F46" s="1">
@@ -4257,7 +4233,7 @@
       <c r="CL46" s="1"/>
       <c r="CM46" s="1"/>
     </row>
-    <row r="47" spans="1:91" ht="231">
+    <row r="47" spans="1:91" ht="216" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>218</v>
       </c>
@@ -4270,7 +4246,7 @@
       <c r="D47" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="3" t="s">
         <v>221</v>
       </c>
       <c r="F47" s="1">
@@ -4364,7 +4340,7 @@
       <c r="CL47" s="1"/>
       <c r="CM47" s="1"/>
     </row>
-    <row r="48" spans="1:91" ht="409.6">
+    <row r="48" spans="1:91" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>222</v>
       </c>
@@ -4377,7 +4353,7 @@
       <c r="D48" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="3" t="s">
         <v>225</v>
       </c>
       <c r="F48" s="1">
@@ -4471,7 +4447,7 @@
       <c r="CL48" s="1"/>
       <c r="CM48" s="1"/>
     </row>
-    <row r="49" spans="1:91" ht="332.25">
+    <row r="49" spans="1:91" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>226</v>
       </c>
@@ -4484,7 +4460,7 @@
       <c r="D49" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="3" t="s">
         <v>229</v>
       </c>
       <c r="F49" s="1">
@@ -4578,7 +4554,7 @@
       <c r="CL49" s="1"/>
       <c r="CM49" s="1"/>
     </row>
-    <row r="50" spans="1:91" ht="409.6">
+    <row r="50" spans="1:91" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>230</v>
       </c>
@@ -4591,7 +4567,7 @@
       <c r="D50" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="3" t="s">
         <v>233</v>
       </c>
       <c r="F50" s="1">
@@ -4685,7 +4661,7 @@
       <c r="CL50" s="1"/>
       <c r="CM50" s="1"/>
     </row>
-    <row r="51" spans="1:91" ht="346.5">
+    <row r="51" spans="1:91" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>234</v>
       </c>
@@ -4698,7 +4674,7 @@
       <c r="D51" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="3" t="s">
         <v>237</v>
       </c>
       <c r="F51" s="1">
@@ -4792,7 +4768,7 @@
       <c r="CL51" s="1"/>
       <c r="CM51" s="1"/>
     </row>
-    <row r="52" spans="1:91" ht="201.75">
+    <row r="52" spans="1:91" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>238</v>
       </c>
@@ -4805,7 +4781,7 @@
       <c r="D52" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="3" t="s">
         <v>241</v>
       </c>
       <c r="F52" s="1">
@@ -4899,7 +4875,7 @@
       <c r="CL52" s="1"/>
       <c r="CM52" s="1"/>
     </row>
-    <row r="53" spans="1:91" ht="361.5">
+    <row r="53" spans="1:91" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>242</v>
       </c>
@@ -4912,7 +4888,7 @@
       <c r="D53" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="3" t="s">
         <v>245</v>
       </c>
       <c r="F53" s="1">
@@ -5006,7 +4982,7 @@
       <c r="CL53" s="1"/>
       <c r="CM53" s="1"/>
     </row>
-    <row r="54" spans="1:91" ht="409.6">
+    <row r="54" spans="1:91" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>246</v>
       </c>
@@ -5019,7 +4995,7 @@
       <c r="D54" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="3" t="s">
         <v>249</v>
       </c>
       <c r="F54" s="1">
@@ -5113,7 +5089,7 @@
       <c r="CL54" s="1"/>
       <c r="CM54" s="1"/>
     </row>
-    <row r="55" spans="1:91" ht="409.6">
+    <row r="55" spans="1:91" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>250</v>
       </c>
@@ -5126,7 +5102,7 @@
       <c r="D55" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" s="3" t="s">
         <v>253</v>
       </c>
       <c r="F55" s="1">
@@ -5220,7 +5196,7 @@
       <c r="CL55" s="1"/>
       <c r="CM55" s="1"/>
     </row>
-    <row r="56" spans="1:91" ht="288.75">
+    <row r="56" spans="1:91" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>254</v>
       </c>
@@ -5233,7 +5209,7 @@
       <c r="D56" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="3" t="s">
         <v>257</v>
       </c>
       <c r="F56" s="1">
@@ -5327,7 +5303,7 @@
       <c r="CL56" s="1"/>
       <c r="CM56" s="1"/>
     </row>
-    <row r="57" spans="1:91" ht="288.75">
+    <row r="57" spans="1:91" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>258</v>
       </c>
@@ -5340,7 +5316,7 @@
       <c r="D57" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" s="3" t="s">
         <v>261</v>
       </c>
       <c r="F57" s="1">
@@ -5434,7 +5410,7 @@
       <c r="CL57" s="1"/>
       <c r="CM57" s="1"/>
     </row>
-    <row r="58" spans="1:91" ht="409.6">
+    <row r="58" spans="1:91" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>262</v>
       </c>
@@ -5447,7 +5423,7 @@
       <c r="D58" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="3" t="s">
         <v>265</v>
       </c>
       <c r="F58" s="1">
@@ -5541,7 +5517,7 @@
       <c r="CL58" s="1"/>
       <c r="CM58" s="1"/>
     </row>
-    <row r="59" spans="1:91" ht="144.75">
+    <row r="59" spans="1:91" ht="144" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>266</v>
       </c>
@@ -5554,7 +5530,7 @@
       <c r="D59" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" s="3" t="s">
         <v>269</v>
       </c>
       <c r="F59" s="1">
@@ -5648,7 +5624,7 @@
       <c r="CL59" s="1"/>
       <c r="CM59" s="1"/>
     </row>
-    <row r="60" spans="1:91" ht="245.25">
+    <row r="60" spans="1:91" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>270</v>
       </c>
@@ -5661,7 +5637,7 @@
       <c r="D60" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" s="3" t="s">
         <v>273</v>
       </c>
       <c r="F60" s="1">
@@ -5755,7 +5731,7 @@
       <c r="CL60" s="1"/>
       <c r="CM60" s="1"/>
     </row>
-    <row r="61" spans="1:91" ht="332.25">
+    <row r="61" spans="1:91" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>274</v>
       </c>
@@ -5768,7 +5744,7 @@
       <c r="D61" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" s="3" t="s">
         <v>277</v>
       </c>
       <c r="F61" s="1">
@@ -5862,7 +5838,7 @@
       <c r="CL61" s="1"/>
       <c r="CM61" s="1"/>
     </row>
-    <row r="62" spans="1:91" ht="188.25">
+    <row r="62" spans="1:91" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>278</v>
       </c>
@@ -5875,7 +5851,7 @@
       <c r="D62" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="3" t="s">
         <v>281</v>
       </c>
       <c r="F62" s="1">
@@ -5969,12 +5945,11 @@
       <c r="CL62" s="1"/>
       <c r="CM62" s="1"/>
     </row>
-    <row r="63" spans="1:91" ht="15">
+    <row r="63" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -6062,12 +6037,11 @@
       <c r="CL63" s="1"/>
       <c r="CM63" s="1"/>
     </row>
-    <row r="64" spans="1:91" ht="15">
+    <row r="64" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -6155,12 +6129,11 @@
       <c r="CL64" s="1"/>
       <c r="CM64" s="1"/>
     </row>
-    <row r="65" spans="1:91" ht="15">
+    <row r="65" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -6248,12 +6221,11 @@
       <c r="CL65" s="1"/>
       <c r="CM65" s="1"/>
     </row>
-    <row r="66" spans="1:91" ht="15">
+    <row r="66" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -6341,12 +6313,11 @@
       <c r="CL66" s="1"/>
       <c r="CM66" s="1"/>
     </row>
-    <row r="67" spans="1:91" ht="15">
+    <row r="67" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -6434,12 +6405,11 @@
       <c r="CL67" s="1"/>
       <c r="CM67" s="1"/>
     </row>
-    <row r="68" spans="1:91" ht="15">
+    <row r="68" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -6527,12 +6497,11 @@
       <c r="CL68" s="1"/>
       <c r="CM68" s="1"/>
     </row>
-    <row r="69" spans="1:91" ht="15">
+    <row r="69" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -6620,12 +6589,11 @@
       <c r="CL69" s="1"/>
       <c r="CM69" s="1"/>
     </row>
-    <row r="70" spans="1:91" ht="15">
+    <row r="70" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -6713,12 +6681,11 @@
       <c r="CL70" s="1"/>
       <c r="CM70" s="1"/>
     </row>
-    <row r="71" spans="1:91" ht="15">
+    <row r="71" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -6806,12 +6773,11 @@
       <c r="CL71" s="1"/>
       <c r="CM71" s="1"/>
     </row>
-    <row r="72" spans="1:91" ht="15">
+    <row r="72" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -6899,12 +6865,11 @@
       <c r="CL72" s="1"/>
       <c r="CM72" s="1"/>
     </row>
-    <row r="73" spans="1:91" ht="15">
+    <row r="73" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
@@ -6992,12 +6957,11 @@
       <c r="CL73" s="1"/>
       <c r="CM73" s="1"/>
     </row>
-    <row r="74" spans="1:91" ht="15">
+    <row r="74" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -7085,12 +7049,11 @@
       <c r="CL74" s="1"/>
       <c r="CM74" s="1"/>
     </row>
-    <row r="75" spans="1:91" ht="15">
+    <row r="75" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -7178,12 +7141,11 @@
       <c r="CL75" s="1"/>
       <c r="CM75" s="1"/>
     </row>
-    <row r="76" spans="1:91" ht="15">
+    <row r="76" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
@@ -7271,12 +7233,11 @@
       <c r="CL76" s="1"/>
       <c r="CM76" s="1"/>
     </row>
-    <row r="77" spans="1:91" ht="15">
+    <row r="77" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -7364,12 +7325,11 @@
       <c r="CL77" s="1"/>
       <c r="CM77" s="1"/>
     </row>
-    <row r="78" spans="1:91" ht="15">
+    <row r="78" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -7457,12 +7417,11 @@
       <c r="CL78" s="1"/>
       <c r="CM78" s="1"/>
     </row>
-    <row r="79" spans="1:91" ht="15">
+    <row r="79" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -7550,12 +7509,11 @@
       <c r="CL79" s="1"/>
       <c r="CM79" s="1"/>
     </row>
-    <row r="80" spans="1:91" ht="15">
+    <row r="80" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
@@ -7643,12 +7601,11 @@
       <c r="CL80" s="1"/>
       <c r="CM80" s="1"/>
     </row>
-    <row r="81" spans="1:91" ht="15">
+    <row r="81" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
@@ -7736,12 +7693,11 @@
       <c r="CL81" s="1"/>
       <c r="CM81" s="1"/>
     </row>
-    <row r="82" spans="1:91" ht="15">
+    <row r="82" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
@@ -7829,12 +7785,11 @@
       <c r="CL82" s="1"/>
       <c r="CM82" s="1"/>
     </row>
-    <row r="83" spans="1:91" ht="15">
+    <row r="83" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -7922,12 +7877,11 @@
       <c r="CL83" s="1"/>
       <c r="CM83" s="1"/>
     </row>
-    <row r="84" spans="1:91" ht="15">
+    <row r="84" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -8015,12 +7969,11 @@
       <c r="CL84" s="1"/>
       <c r="CM84" s="1"/>
     </row>
-    <row r="85" spans="1:91" ht="15">
+    <row r="85" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
@@ -8108,12 +8061,11 @@
       <c r="CL85" s="1"/>
       <c r="CM85" s="1"/>
     </row>
-    <row r="86" spans="1:91" ht="15">
+    <row r="86" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -8201,12 +8153,11 @@
       <c r="CL86" s="1"/>
       <c r="CM86" s="1"/>
     </row>
-    <row r="87" spans="1:91" ht="15">
+    <row r="87" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
@@ -8294,12 +8245,11 @@
       <c r="CL87" s="1"/>
       <c r="CM87" s="1"/>
     </row>
-    <row r="88" spans="1:91" ht="15">
+    <row r="88" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
@@ -8387,12 +8337,11 @@
       <c r="CL88" s="1"/>
       <c r="CM88" s="1"/>
     </row>
-    <row r="89" spans="1:91" ht="15">
+    <row r="89" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -8480,12 +8429,11 @@
       <c r="CL89" s="1"/>
       <c r="CM89" s="1"/>
     </row>
-    <row r="90" spans="1:91" ht="15">
+    <row r="90" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -8573,12 +8521,11 @@
       <c r="CL90" s="1"/>
       <c r="CM90" s="1"/>
     </row>
-    <row r="91" spans="1:91" ht="15">
+    <row r="91" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -8666,12 +8613,11 @@
       <c r="CL91" s="1"/>
       <c r="CM91" s="1"/>
     </row>
-    <row r="92" spans="1:91" ht="15">
+    <row r="92" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
@@ -8759,12 +8705,11 @@
       <c r="CL92" s="1"/>
       <c r="CM92" s="1"/>
     </row>
-    <row r="93" spans="1:91" ht="15">
+    <row r="93" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
@@ -8852,12 +8797,11 @@
       <c r="CL93" s="1"/>
       <c r="CM93" s="1"/>
     </row>
-    <row r="94" spans="1:91" ht="15">
+    <row r="94" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
@@ -8945,12 +8889,11 @@
       <c r="CL94" s="1"/>
       <c r="CM94" s="1"/>
     </row>
-    <row r="95" spans="1:91" ht="15">
+    <row r="95" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -9038,12 +8981,11 @@
       <c r="CL95" s="1"/>
       <c r="CM95" s="1"/>
     </row>
-    <row r="96" spans="1:91" ht="15">
+    <row r="96" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -9131,12 +9073,11 @@
       <c r="CL96" s="1"/>
       <c r="CM96" s="1"/>
     </row>
-    <row r="97" spans="1:91" ht="15">
+    <row r="97" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
@@ -9224,12 +9165,11 @@
       <c r="CL97" s="1"/>
       <c r="CM97" s="1"/>
     </row>
-    <row r="98" spans="1:91" ht="15">
+    <row r="98" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
@@ -9317,12 +9257,11 @@
       <c r="CL98" s="1"/>
       <c r="CM98" s="1"/>
     </row>
-    <row r="99" spans="1:91" ht="15">
+    <row r="99" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
@@ -9410,12 +9349,11 @@
       <c r="CL99" s="1"/>
       <c r="CM99" s="1"/>
     </row>
-    <row r="100" spans="1:91" ht="15">
+    <row r="100" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
@@ -9503,12 +9441,11 @@
       <c r="CL100" s="1"/>
       <c r="CM100" s="1"/>
     </row>
-    <row r="101" spans="1:91" ht="15">
+    <row r="101" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
@@ -9596,12 +9533,11 @@
       <c r="CL101" s="1"/>
       <c r="CM101" s="1"/>
     </row>
-    <row r="102" spans="1:91" ht="15">
+    <row r="102" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
@@ -9689,12 +9625,11 @@
       <c r="CL102" s="1"/>
       <c r="CM102" s="1"/>
     </row>
-    <row r="103" spans="1:91" ht="15">
+    <row r="103" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
@@ -9782,12 +9717,11 @@
       <c r="CL103" s="1"/>
       <c r="CM103" s="1"/>
     </row>
-    <row r="104" spans="1:91" ht="15">
+    <row r="104" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
@@ -9875,12 +9809,11 @@
       <c r="CL104" s="1"/>
       <c r="CM104" s="1"/>
     </row>
-    <row r="105" spans="1:91" ht="15">
+    <row r="105" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
@@ -9968,12 +9901,11 @@
       <c r="CL105" s="1"/>
       <c r="CM105" s="1"/>
     </row>
-    <row r="106" spans="1:91" ht="15">
+    <row r="106" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
@@ -10061,12 +9993,11 @@
       <c r="CL106" s="1"/>
       <c r="CM106" s="1"/>
     </row>
-    <row r="107" spans="1:91" ht="15">
+    <row r="107" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
@@ -10154,12 +10085,11 @@
       <c r="CL107" s="1"/>
       <c r="CM107" s="1"/>
     </row>
-    <row r="108" spans="1:91" ht="15">
+    <row r="108" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
@@ -10247,12 +10177,11 @@
       <c r="CL108" s="1"/>
       <c r="CM108" s="1"/>
     </row>
-    <row r="109" spans="1:91" ht="15">
+    <row r="109" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
@@ -10340,12 +10269,11 @@
       <c r="CL109" s="1"/>
       <c r="CM109" s="1"/>
     </row>
-    <row r="110" spans="1:91" ht="15">
+    <row r="110" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
@@ -10433,12 +10361,11 @@
       <c r="CL110" s="1"/>
       <c r="CM110" s="1"/>
     </row>
-    <row r="111" spans="1:91" ht="15">
+    <row r="111" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -10526,12 +10453,11 @@
       <c r="CL111" s="1"/>
       <c r="CM111" s="1"/>
     </row>
-    <row r="112" spans="1:91" ht="15">
+    <row r="112" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
@@ -10619,12 +10545,11 @@
       <c r="CL112" s="1"/>
       <c r="CM112" s="1"/>
     </row>
-    <row r="113" spans="1:91" ht="15">
+    <row r="113" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
@@ -10712,12 +10637,11 @@
       <c r="CL113" s="1"/>
       <c r="CM113" s="1"/>
     </row>
-    <row r="114" spans="1:91" ht="15">
+    <row r="114" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
@@ -10805,12 +10729,11 @@
       <c r="CL114" s="1"/>
       <c r="CM114" s="1"/>
     </row>
-    <row r="115" spans="1:91" ht="15">
+    <row r="115" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
@@ -10898,12 +10821,11 @@
       <c r="CL115" s="1"/>
       <c r="CM115" s="1"/>
     </row>
-    <row r="116" spans="1:91" ht="15">
+    <row r="116" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
@@ -10991,12 +10913,11 @@
       <c r="CL116" s="1"/>
       <c r="CM116" s="1"/>
     </row>
-    <row r="117" spans="1:91" ht="15">
+    <row r="117" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -11084,12 +11005,11 @@
       <c r="CL117" s="1"/>
       <c r="CM117" s="1"/>
     </row>
-    <row r="118" spans="1:91" ht="15">
+    <row r="118" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
@@ -11177,12 +11097,11 @@
       <c r="CL118" s="1"/>
       <c r="CM118" s="1"/>
     </row>
-    <row r="119" spans="1:91" ht="15">
+    <row r="119" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
@@ -11270,12 +11189,11 @@
       <c r="CL119" s="1"/>
       <c r="CM119" s="1"/>
     </row>
-    <row r="120" spans="1:91" ht="15">
+    <row r="120" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
@@ -11363,12 +11281,11 @@
       <c r="CL120" s="1"/>
       <c r="CM120" s="1"/>
     </row>
-    <row r="121" spans="1:91" ht="15">
+    <row r="121" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
@@ -11456,12 +11373,11 @@
       <c r="CL121" s="1"/>
       <c r="CM121" s="1"/>
     </row>
-    <row r="122" spans="1:91" ht="15">
+    <row r="122" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -11549,12 +11465,11 @@
       <c r="CL122" s="1"/>
       <c r="CM122" s="1"/>
     </row>
-    <row r="123" spans="1:91" ht="15">
+    <row r="123" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -11642,12 +11557,11 @@
       <c r="CL123" s="1"/>
       <c r="CM123" s="1"/>
     </row>
-    <row r="124" spans="1:91" ht="15">
+    <row r="124" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
@@ -11735,12 +11649,11 @@
       <c r="CL124" s="1"/>
       <c r="CM124" s="1"/>
     </row>
-    <row r="125" spans="1:91" ht="15">
+    <row r="125" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
@@ -11828,12 +11741,11 @@
       <c r="CL125" s="1"/>
       <c r="CM125" s="1"/>
     </row>
-    <row r="126" spans="1:91" ht="15">
+    <row r="126" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
-      <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -11921,12 +11833,11 @@
       <c r="CL126" s="1"/>
       <c r="CM126" s="1"/>
     </row>
-    <row r="127" spans="1:91" ht="15">
+    <row r="127" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
@@ -12014,12 +11925,11 @@
       <c r="CL127" s="1"/>
       <c r="CM127" s="1"/>
     </row>
-    <row r="128" spans="1:91" ht="15">
+    <row r="128" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
@@ -12107,12 +12017,11 @@
       <c r="CL128" s="1"/>
       <c r="CM128" s="1"/>
     </row>
-    <row r="129" spans="1:91" ht="15">
+    <row r="129" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
@@ -12200,12 +12109,11 @@
       <c r="CL129" s="1"/>
       <c r="CM129" s="1"/>
     </row>
-    <row r="130" spans="1:91" ht="15">
+    <row r="130" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
@@ -12293,12 +12201,11 @@
       <c r="CL130" s="1"/>
       <c r="CM130" s="1"/>
     </row>
-    <row r="131" spans="1:91" ht="15">
+    <row r="131" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
-      <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
@@ -12386,12 +12293,11 @@
       <c r="CL131" s="1"/>
       <c r="CM131" s="1"/>
     </row>
-    <row r="132" spans="1:91" ht="15">
+    <row r="132" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
-      <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -12479,12 +12385,11 @@
       <c r="CL132" s="1"/>
       <c r="CM132" s="1"/>
     </row>
-    <row r="133" spans="1:91" ht="15">
+    <row r="133" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
-      <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
@@ -12572,12 +12477,11 @@
       <c r="CL133" s="1"/>
       <c r="CM133" s="1"/>
     </row>
-    <row r="134" spans="1:91" ht="15">
+    <row r="134" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
@@ -12665,12 +12569,11 @@
       <c r="CL134" s="1"/>
       <c r="CM134" s="1"/>
     </row>
-    <row r="135" spans="1:91" ht="15">
+    <row r="135" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
@@ -12758,12 +12661,11 @@
       <c r="CL135" s="1"/>
       <c r="CM135" s="1"/>
     </row>
-    <row r="136" spans="1:91" ht="15">
+    <row r="136" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
@@ -12851,12 +12753,11 @@
       <c r="CL136" s="1"/>
       <c r="CM136" s="1"/>
     </row>
-    <row r="137" spans="1:91" ht="15">
+    <row r="137" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
-      <c r="E137" s="1"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -12944,12 +12845,11 @@
       <c r="CL137" s="1"/>
       <c r="CM137" s="1"/>
     </row>
-    <row r="138" spans="1:91" ht="15">
+    <row r="138" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
-      <c r="E138" s="1"/>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
@@ -13037,12 +12937,11 @@
       <c r="CL138" s="1"/>
       <c r="CM138" s="1"/>
     </row>
-    <row r="139" spans="1:91" ht="15">
+    <row r="139" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
-      <c r="E139" s="1"/>
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
@@ -13130,12 +13029,11 @@
       <c r="CL139" s="1"/>
       <c r="CM139" s="1"/>
     </row>
-    <row r="140" spans="1:91" ht="15">
+    <row r="140" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
-      <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
@@ -13223,12 +13121,11 @@
       <c r="CL140" s="1"/>
       <c r="CM140" s="1"/>
     </row>
-    <row r="141" spans="1:91" ht="15">
+    <row r="141" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
@@ -13316,12 +13213,11 @@
       <c r="CL141" s="1"/>
       <c r="CM141" s="1"/>
     </row>
-    <row r="142" spans="1:91" ht="15">
+    <row r="142" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
-      <c r="E142" s="1"/>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
@@ -13409,12 +13305,11 @@
       <c r="CL142" s="1"/>
       <c r="CM142" s="1"/>
     </row>
-    <row r="143" spans="1:91" ht="15">
+    <row r="143" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
-      <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
@@ -13502,12 +13397,11 @@
       <c r="CL143" s="1"/>
       <c r="CM143" s="1"/>
     </row>
-    <row r="144" spans="1:91" ht="15">
+    <row r="144" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
-      <c r="E144" s="1"/>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
@@ -13595,12 +13489,11 @@
       <c r="CL144" s="1"/>
       <c r="CM144" s="1"/>
     </row>
-    <row r="145" spans="1:91" ht="15">
+    <row r="145" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
@@ -13688,12 +13581,11 @@
       <c r="CL145" s="1"/>
       <c r="CM145" s="1"/>
     </row>
-    <row r="146" spans="1:91" ht="15">
+    <row r="146" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
@@ -13781,12 +13673,11 @@
       <c r="CL146" s="1"/>
       <c r="CM146" s="1"/>
     </row>
-    <row r="147" spans="1:91" ht="15">
+    <row r="147" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
@@ -13874,12 +13765,11 @@
       <c r="CL147" s="1"/>
       <c r="CM147" s="1"/>
     </row>
-    <row r="148" spans="1:91" ht="15">
+    <row r="148" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
@@ -13967,12 +13857,11 @@
       <c r="CL148" s="1"/>
       <c r="CM148" s="1"/>
     </row>
-    <row r="149" spans="1:91" ht="15">
+    <row r="149" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
@@ -14060,12 +13949,11 @@
       <c r="CL149" s="1"/>
       <c r="CM149" s="1"/>
     </row>
-    <row r="150" spans="1:91" ht="15">
+    <row r="150" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
@@ -14153,12 +14041,11 @@
       <c r="CL150" s="1"/>
       <c r="CM150" s="1"/>
     </row>
-    <row r="151" spans="1:91" ht="15">
+    <row r="151" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
@@ -14246,12 +14133,11 @@
       <c r="CL151" s="1"/>
       <c r="CM151" s="1"/>
     </row>
-    <row r="152" spans="1:91" ht="15">
+    <row r="152" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
@@ -14339,12 +14225,11 @@
       <c r="CL152" s="1"/>
       <c r="CM152" s="1"/>
     </row>
-    <row r="153" spans="1:91" ht="15">
+    <row r="153" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
@@ -14432,12 +14317,11 @@
       <c r="CL153" s="1"/>
       <c r="CM153" s="1"/>
     </row>
-    <row r="154" spans="1:91" ht="15">
+    <row r="154" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
-      <c r="E154" s="1"/>
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
@@ -14525,12 +14409,11 @@
       <c r="CL154" s="1"/>
       <c r="CM154" s="1"/>
     </row>
-    <row r="155" spans="1:91" ht="15">
+    <row r="155" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
-      <c r="E155" s="1"/>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
@@ -14618,12 +14501,11 @@
       <c r="CL155" s="1"/>
       <c r="CM155" s="1"/>
     </row>
-    <row r="156" spans="1:91" ht="15">
+    <row r="156" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
-      <c r="E156" s="1"/>
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
@@ -14711,12 +14593,11 @@
       <c r="CL156" s="1"/>
       <c r="CM156" s="1"/>
     </row>
-    <row r="157" spans="1:91" ht="15">
+    <row r="157" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
@@ -14804,12 +14685,11 @@
       <c r="CL157" s="1"/>
       <c r="CM157" s="1"/>
     </row>
-    <row r="158" spans="1:91" ht="15">
+    <row r="158" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
@@ -14897,12 +14777,11 @@
       <c r="CL158" s="1"/>
       <c r="CM158" s="1"/>
     </row>
-    <row r="159" spans="1:91" ht="15">
+    <row r="159" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
@@ -14990,12 +14869,11 @@
       <c r="CL159" s="1"/>
       <c r="CM159" s="1"/>
     </row>
-    <row r="160" spans="1:91" ht="15">
+    <row r="160" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
-      <c r="E160" s="1"/>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
@@ -15083,12 +14961,11 @@
       <c r="CL160" s="1"/>
       <c r="CM160" s="1"/>
     </row>
-    <row r="161" spans="1:91" ht="15">
+    <row r="161" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
-      <c r="E161" s="1"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
@@ -15176,12 +15053,11 @@
       <c r="CL161" s="1"/>
       <c r="CM161" s="1"/>
     </row>
-    <row r="162" spans="1:91" ht="15">
+    <row r="162" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
-      <c r="E162" s="1"/>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
@@ -15269,12 +15145,11 @@
       <c r="CL162" s="1"/>
       <c r="CM162" s="1"/>
     </row>
-    <row r="163" spans="1:91" ht="15">
+    <row r="163" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
-      <c r="E163" s="1"/>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
@@ -15362,12 +15237,11 @@
       <c r="CL163" s="1"/>
       <c r="CM163" s="1"/>
     </row>
-    <row r="164" spans="1:91" ht="15">
+    <row r="164" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
@@ -15455,12 +15329,11 @@
       <c r="CL164" s="1"/>
       <c r="CM164" s="1"/>
     </row>
-    <row r="165" spans="1:91" ht="15">
+    <row r="165" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
@@ -15548,12 +15421,11 @@
       <c r="CL165" s="1"/>
       <c r="CM165" s="1"/>
     </row>
-    <row r="166" spans="1:91" ht="15">
+    <row r="166" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
@@ -15641,12 +15513,11 @@
       <c r="CL166" s="1"/>
       <c r="CM166" s="1"/>
     </row>
-    <row r="167" spans="1:91" ht="15">
+    <row r="167" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
@@ -15734,12 +15605,11 @@
       <c r="CL167" s="1"/>
       <c r="CM167" s="1"/>
     </row>
-    <row r="168" spans="1:91" ht="15">
+    <row r="168" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
-      <c r="E168" s="1"/>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
@@ -15827,12 +15697,11 @@
       <c r="CL168" s="1"/>
       <c r="CM168" s="1"/>
     </row>
-    <row r="169" spans="1:91" ht="15">
+    <row r="169" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
-      <c r="E169" s="1"/>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
@@ -15920,12 +15789,11 @@
       <c r="CL169" s="1"/>
       <c r="CM169" s="1"/>
     </row>
-    <row r="170" spans="1:91" ht="15">
+    <row r="170" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
-      <c r="E170" s="1"/>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
@@ -16013,12 +15881,11 @@
       <c r="CL170" s="1"/>
       <c r="CM170" s="1"/>
     </row>
-    <row r="171" spans="1:91" ht="15">
+    <row r="171" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
@@ -16106,12 +15973,11 @@
       <c r="CL171" s="1"/>
       <c r="CM171" s="1"/>
     </row>
-    <row r="172" spans="1:91" ht="15">
+    <row r="172" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
-      <c r="E172" s="1"/>
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
@@ -16199,12 +16065,11 @@
       <c r="CL172" s="1"/>
       <c r="CM172" s="1"/>
     </row>
-    <row r="173" spans="1:91" ht="15">
+    <row r="173" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
-      <c r="E173" s="1"/>
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
@@ -16292,12 +16157,11 @@
       <c r="CL173" s="1"/>
       <c r="CM173" s="1"/>
     </row>
-    <row r="174" spans="1:91" ht="15">
+    <row r="174" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
-      <c r="E174" s="1"/>
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
@@ -16385,12 +16249,11 @@
       <c r="CL174" s="1"/>
       <c r="CM174" s="1"/>
     </row>
-    <row r="175" spans="1:91" ht="15">
+    <row r="175" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
-      <c r="E175" s="1"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
@@ -16478,12 +16341,11 @@
       <c r="CL175" s="1"/>
       <c r="CM175" s="1"/>
     </row>
-    <row r="176" spans="1:91" ht="15">
+    <row r="176" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
-      <c r="E176" s="1"/>
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
@@ -16571,12 +16433,11 @@
       <c r="CL176" s="1"/>
       <c r="CM176" s="1"/>
     </row>
-    <row r="177" spans="1:91" ht="15">
+    <row r="177" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
-      <c r="E177" s="1"/>
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
@@ -16664,12 +16525,11 @@
       <c r="CL177" s="1"/>
       <c r="CM177" s="1"/>
     </row>
-    <row r="178" spans="1:91" ht="15">
+    <row r="178" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
-      <c r="E178" s="1"/>
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
@@ -16757,12 +16617,11 @@
       <c r="CL178" s="1"/>
       <c r="CM178" s="1"/>
     </row>
-    <row r="179" spans="1:91" ht="15">
+    <row r="179" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
-      <c r="E179" s="1"/>
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
@@ -16850,12 +16709,11 @@
       <c r="CL179" s="1"/>
       <c r="CM179" s="1"/>
     </row>
-    <row r="180" spans="1:91" ht="15">
+    <row r="180" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
-      <c r="E180" s="1"/>
       <c r="F180" s="1"/>
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
@@ -16943,12 +16801,11 @@
       <c r="CL180" s="1"/>
       <c r="CM180" s="1"/>
     </row>
-    <row r="181" spans="1:91" ht="15">
+    <row r="181" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
-      <c r="E181" s="1"/>
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
@@ -17036,12 +16893,11 @@
       <c r="CL181" s="1"/>
       <c r="CM181" s="1"/>
     </row>
-    <row r="182" spans="1:91" ht="15">
+    <row r="182" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
-      <c r="E182" s="1"/>
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
@@ -17129,12 +16985,11 @@
       <c r="CL182" s="1"/>
       <c r="CM182" s="1"/>
     </row>
-    <row r="183" spans="1:91" ht="15">
+    <row r="183" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
-      <c r="E183" s="1"/>
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
@@ -17222,12 +17077,11 @@
       <c r="CL183" s="1"/>
       <c r="CM183" s="1"/>
     </row>
-    <row r="184" spans="1:91" ht="15">
+    <row r="184" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
-      <c r="E184" s="1"/>
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
@@ -17315,12 +17169,11 @@
       <c r="CL184" s="1"/>
       <c r="CM184" s="1"/>
     </row>
-    <row r="185" spans="1:91" ht="15">
+    <row r="185" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
-      <c r="E185" s="1"/>
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
@@ -17408,12 +17261,11 @@
       <c r="CL185" s="1"/>
       <c r="CM185" s="1"/>
     </row>
-    <row r="186" spans="1:91" ht="15">
+    <row r="186" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
-      <c r="E186" s="1"/>
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
@@ -17501,12 +17353,11 @@
       <c r="CL186" s="1"/>
       <c r="CM186" s="1"/>
     </row>
-    <row r="187" spans="1:91" ht="15">
+    <row r="187" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
-      <c r="E187" s="1"/>
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
@@ -17594,12 +17445,11 @@
       <c r="CL187" s="1"/>
       <c r="CM187" s="1"/>
     </row>
-    <row r="188" spans="1:91" ht="15">
+    <row r="188" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
-      <c r="E188" s="1"/>
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
@@ -17687,12 +17537,11 @@
       <c r="CL188" s="1"/>
       <c r="CM188" s="1"/>
     </row>
-    <row r="189" spans="1:91" ht="15">
+    <row r="189" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
-      <c r="E189" s="1"/>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
@@ -17780,12 +17629,11 @@
       <c r="CL189" s="1"/>
       <c r="CM189" s="1"/>
     </row>
-    <row r="190" spans="1:91" ht="15">
+    <row r="190" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
-      <c r="E190" s="1"/>
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
@@ -17873,12 +17721,11 @@
       <c r="CL190" s="1"/>
       <c r="CM190" s="1"/>
     </row>
-    <row r="191" spans="1:91" ht="15">
+    <row r="191" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
-      <c r="E191" s="1"/>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
@@ -17966,12 +17813,11 @@
       <c r="CL191" s="1"/>
       <c r="CM191" s="1"/>
     </row>
-    <row r="192" spans="1:91" ht="15">
+    <row r="192" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
-      <c r="E192" s="1"/>
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
@@ -18059,12 +17905,11 @@
       <c r="CL192" s="1"/>
       <c r="CM192" s="1"/>
     </row>
-    <row r="193" spans="1:91" ht="15">
+    <row r="193" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
-      <c r="E193" s="1"/>
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
@@ -18152,12 +17997,11 @@
       <c r="CL193" s="1"/>
       <c r="CM193" s="1"/>
     </row>
-    <row r="194" spans="1:91" ht="15">
+    <row r="194" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
-      <c r="E194" s="1"/>
       <c r="F194" s="1"/>
       <c r="G194" s="1"/>
       <c r="H194" s="1"/>
@@ -18245,12 +18089,11 @@
       <c r="CL194" s="1"/>
       <c r="CM194" s="1"/>
     </row>
-    <row r="195" spans="1:91" ht="15">
+    <row r="195" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
-      <c r="E195" s="1"/>
       <c r="F195" s="1"/>
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
@@ -18338,12 +18181,11 @@
       <c r="CL195" s="1"/>
       <c r="CM195" s="1"/>
     </row>
-    <row r="196" spans="1:91" ht="15">
+    <row r="196" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
-      <c r="E196" s="1"/>
       <c r="F196" s="1"/>
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
@@ -18431,12 +18273,11 @@
       <c r="CL196" s="1"/>
       <c r="CM196" s="1"/>
     </row>
-    <row r="197" spans="1:91" ht="15">
+    <row r="197" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
-      <c r="E197" s="1"/>
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
@@ -18524,12 +18365,11 @@
       <c r="CL197" s="1"/>
       <c r="CM197" s="1"/>
     </row>
-    <row r="198" spans="1:91" ht="15">
+    <row r="198" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
-      <c r="E198" s="1"/>
       <c r="F198" s="1"/>
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
@@ -18617,12 +18457,11 @@
       <c r="CL198" s="1"/>
       <c r="CM198" s="1"/>
     </row>
-    <row r="199" spans="1:91" ht="15">
+    <row r="199" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
-      <c r="E199" s="1"/>
       <c r="F199" s="1"/>
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
@@ -18710,12 +18549,11 @@
       <c r="CL199" s="1"/>
       <c r="CM199" s="1"/>
     </row>
-    <row r="200" spans="1:91" ht="15">
+    <row r="200" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
-      <c r="E200" s="1"/>
       <c r="F200" s="1"/>
       <c r="G200" s="1"/>
       <c r="H200" s="1"/>
@@ -18803,12 +18641,11 @@
       <c r="CL200" s="1"/>
       <c r="CM200" s="1"/>
     </row>
-    <row r="201" spans="1:91" ht="15">
+    <row r="201" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
-      <c r="E201" s="1"/>
       <c r="F201" s="1"/>
       <c r="G201" s="1"/>
       <c r="H201" s="1"/>
@@ -18896,12 +18733,11 @@
       <c r="CL201" s="1"/>
       <c r="CM201" s="1"/>
     </row>
-    <row r="202" spans="1:91" ht="15">
+    <row r="202" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
-      <c r="E202" s="1"/>
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
       <c r="H202" s="1"/>
@@ -18989,12 +18825,11 @@
       <c r="CL202" s="1"/>
       <c r="CM202" s="1"/>
     </row>
-    <row r="203" spans="1:91" ht="15">
+    <row r="203" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
-      <c r="E203" s="1"/>
       <c r="F203" s="1"/>
       <c r="G203" s="1"/>
       <c r="H203" s="1"/>
@@ -19082,12 +18917,11 @@
       <c r="CL203" s="1"/>
       <c r="CM203" s="1"/>
     </row>
-    <row r="204" spans="1:91" ht="15">
+    <row r="204" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
-      <c r="E204" s="1"/>
       <c r="F204" s="1"/>
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
@@ -19175,12 +19009,11 @@
       <c r="CL204" s="1"/>
       <c r="CM204" s="1"/>
     </row>
-    <row r="205" spans="1:91" ht="15">
+    <row r="205" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
-      <c r="E205" s="1"/>
       <c r="F205" s="1"/>
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
@@ -19268,12 +19101,11 @@
       <c r="CL205" s="1"/>
       <c r="CM205" s="1"/>
     </row>
-    <row r="206" spans="1:91" ht="15">
+    <row r="206" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
-      <c r="E206" s="1"/>
       <c r="F206" s="1"/>
       <c r="G206" s="1"/>
       <c r="H206" s="1"/>
@@ -19361,12 +19193,11 @@
       <c r="CL206" s="1"/>
       <c r="CM206" s="1"/>
     </row>
-    <row r="207" spans="1:91" ht="15">
+    <row r="207" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
-      <c r="E207" s="1"/>
       <c r="F207" s="1"/>
       <c r="G207" s="1"/>
       <c r="H207" s="1"/>
@@ -19454,12 +19285,11 @@
       <c r="CL207" s="1"/>
       <c r="CM207" s="1"/>
     </row>
-    <row r="208" spans="1:91" ht="15">
+    <row r="208" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
-      <c r="E208" s="1"/>
       <c r="F208" s="1"/>
       <c r="G208" s="1"/>
       <c r="H208" s="1"/>
@@ -19547,12 +19377,11 @@
       <c r="CL208" s="1"/>
       <c r="CM208" s="1"/>
     </row>
-    <row r="209" spans="1:91" ht="15">
+    <row r="209" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
-      <c r="E209" s="1"/>
       <c r="F209" s="1"/>
       <c r="G209" s="1"/>
       <c r="H209" s="1"/>
@@ -19640,12 +19469,11 @@
       <c r="CL209" s="1"/>
       <c r="CM209" s="1"/>
     </row>
-    <row r="210" spans="1:91" ht="15">
+    <row r="210" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
       <c r="F210" s="1"/>
       <c r="G210" s="1"/>
       <c r="H210" s="1"/>
@@ -19733,12 +19561,11 @@
       <c r="CL210" s="1"/>
       <c r="CM210" s="1"/>
     </row>
-    <row r="211" spans="1:91" ht="15">
+    <row r="211" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
-      <c r="E211" s="1"/>
       <c r="F211" s="1"/>
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
@@ -19826,12 +19653,11 @@
       <c r="CL211" s="1"/>
       <c r="CM211" s="1"/>
     </row>
-    <row r="212" spans="1:91" ht="15">
+    <row r="212" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
-      <c r="E212" s="1"/>
       <c r="F212" s="1"/>
       <c r="G212" s="1"/>
       <c r="H212" s="1"/>
@@ -19919,12 +19745,11 @@
       <c r="CL212" s="1"/>
       <c r="CM212" s="1"/>
     </row>
-    <row r="213" spans="1:91" ht="15">
+    <row r="213" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
-      <c r="E213" s="1"/>
       <c r="F213" s="1"/>
       <c r="G213" s="1"/>
       <c r="H213" s="1"/>
@@ -20012,12 +19837,11 @@
       <c r="CL213" s="1"/>
       <c r="CM213" s="1"/>
     </row>
-    <row r="214" spans="1:91" ht="15">
+    <row r="214" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
-      <c r="E214" s="1"/>
       <c r="F214" s="1"/>
       <c r="G214" s="1"/>
       <c r="H214" s="1"/>
@@ -20105,12 +19929,11 @@
       <c r="CL214" s="1"/>
       <c r="CM214" s="1"/>
     </row>
-    <row r="215" spans="1:91" ht="15">
+    <row r="215" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
-      <c r="E215" s="1"/>
       <c r="F215" s="1"/>
       <c r="G215" s="1"/>
       <c r="H215" s="1"/>
@@ -20198,12 +20021,11 @@
       <c r="CL215" s="1"/>
       <c r="CM215" s="1"/>
     </row>
-    <row r="216" spans="1:91" ht="15">
+    <row r="216" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
-      <c r="E216" s="1"/>
       <c r="F216" s="1"/>
       <c r="G216" s="1"/>
       <c r="H216" s="1"/>
@@ -20291,12 +20113,11 @@
       <c r="CL216" s="1"/>
       <c r="CM216" s="1"/>
     </row>
-    <row r="217" spans="1:91" ht="15">
+    <row r="217" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
-      <c r="E217" s="1"/>
       <c r="F217" s="1"/>
       <c r="G217" s="1"/>
       <c r="H217" s="1"/>
@@ -20384,12 +20205,11 @@
       <c r="CL217" s="1"/>
       <c r="CM217" s="1"/>
     </row>
-    <row r="218" spans="1:91" ht="15">
+    <row r="218" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
-      <c r="E218" s="1"/>
       <c r="F218" s="1"/>
       <c r="G218" s="1"/>
       <c r="H218" s="1"/>
@@ -20477,12 +20297,11 @@
       <c r="CL218" s="1"/>
       <c r="CM218" s="1"/>
     </row>
-    <row r="219" spans="1:91" ht="15">
+    <row r="219" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
-      <c r="E219" s="1"/>
       <c r="F219" s="1"/>
       <c r="G219" s="1"/>
       <c r="H219" s="1"/>
@@ -20570,12 +20389,11 @@
       <c r="CL219" s="1"/>
       <c r="CM219" s="1"/>
     </row>
-    <row r="220" spans="1:91" ht="15">
+    <row r="220" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
-      <c r="E220" s="1"/>
       <c r="F220" s="1"/>
       <c r="G220" s="1"/>
       <c r="H220" s="1"/>
@@ -20663,12 +20481,11 @@
       <c r="CL220" s="1"/>
       <c r="CM220" s="1"/>
     </row>
-    <row r="221" spans="1:91" ht="15">
+    <row r="221" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
-      <c r="E221" s="1"/>
       <c r="F221" s="1"/>
       <c r="G221" s="1"/>
       <c r="H221" s="1"/>
@@ -20756,12 +20573,11 @@
       <c r="CL221" s="1"/>
       <c r="CM221" s="1"/>
     </row>
-    <row r="222" spans="1:91" ht="15">
+    <row r="222" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
-      <c r="E222" s="1"/>
       <c r="F222" s="1"/>
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
@@ -20849,12 +20665,11 @@
       <c r="CL222" s="1"/>
       <c r="CM222" s="1"/>
     </row>
-    <row r="223" spans="1:91" ht="15">
+    <row r="223" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="1"/>
       <c r="F223" s="1"/>
       <c r="G223" s="1"/>
       <c r="H223" s="1"/>
@@ -20942,12 +20757,11 @@
       <c r="CL223" s="1"/>
       <c r="CM223" s="1"/>
     </row>
-    <row r="224" spans="1:91" ht="15">
+    <row r="224" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
-      <c r="E224" s="1"/>
       <c r="F224" s="1"/>
       <c r="G224" s="1"/>
       <c r="H224" s="1"/>
@@ -21035,12 +20849,11 @@
       <c r="CL224" s="1"/>
       <c r="CM224" s="1"/>
     </row>
-    <row r="225" spans="1:91" ht="15">
+    <row r="225" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
-      <c r="E225" s="1"/>
       <c r="F225" s="1"/>
       <c r="G225" s="1"/>
       <c r="H225" s="1"/>
@@ -21128,12 +20941,11 @@
       <c r="CL225" s="1"/>
       <c r="CM225" s="1"/>
     </row>
-    <row r="226" spans="1:91" ht="15">
+    <row r="226" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
-      <c r="E226" s="1"/>
       <c r="F226" s="1"/>
       <c r="G226" s="1"/>
       <c r="H226" s="1"/>
@@ -21221,12 +21033,11 @@
       <c r="CL226" s="1"/>
       <c r="CM226" s="1"/>
     </row>
-    <row r="227" spans="1:91" ht="15">
+    <row r="227" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
-      <c r="E227" s="1"/>
       <c r="F227" s="1"/>
       <c r="G227" s="1"/>
       <c r="H227" s="1"/>
@@ -21314,12 +21125,11 @@
       <c r="CL227" s="1"/>
       <c r="CM227" s="1"/>
     </row>
-    <row r="228" spans="1:91" ht="15">
+    <row r="228" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
-      <c r="E228" s="1"/>
       <c r="F228" s="1"/>
       <c r="G228" s="1"/>
       <c r="H228" s="1"/>
@@ -21407,12 +21217,11 @@
       <c r="CL228" s="1"/>
       <c r="CM228" s="1"/>
     </row>
-    <row r="229" spans="1:91" ht="15">
+    <row r="229" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
-      <c r="E229" s="1"/>
       <c r="F229" s="1"/>
       <c r="G229" s="1"/>
       <c r="H229" s="1"/>

</xml_diff>

<commit_message>
Added some one piece recipes
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\Downloads\COSC345\Realm-of-Feasts\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkish\Downloads\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB967377-800A-483F-AA4C-0CEBFDFEF105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B016B0B7-B48A-4935-A34A-2D5DFFDFBBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
   <sheets>
     <sheet name="RecipesTest" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="307">
   <si>
     <t>Name</t>
   </si>
@@ -882,13 +882,88 @@
   </si>
   <si>
     <t>1*tablespoon*Butter,1*cup*Bulgur Wheat,1*cup*Whole Milk,1*cups*Water,100*milliliters*Whole Cream,50*grams*Dried Cherries,50*grams*Currants,2*null*Egg Yolks (beaten),4*strands*Saffron,50*grams*Brown Sugar,0.5*tablespoon*Butter (topping),1*tablespoon*Pine Nuts,100*grams*Flaked Almonds,100*milliliter*Whole Cream (topping)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fried Rice </t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Piece </t>
+  </si>
+  <si>
+    <t>Fried Rice with corned beef you can cook in one frying pan</t>
+  </si>
+  <si>
+    <t>2*cups*Rice (cooked),2*large*Eggs (beaten),50*grams*Corned Beef,1*quarter*Onion,4*small*Brown Mushrooms*1*tablespoon*Vegetable Oil,0.5*teaspoon*Salt,1*sprinkle*Black Pepper,1.5*tablespoon*Soy Sauce,2*null*Green Onions</t>
+  </si>
+  <si>
+    <t>1. Mince the onion, finely slice the mushrooms, and chop the green onions.||2. Oil the frying pan and fry half the minced onion and all the mushrooms, then add the corned beef. ||3. Push the fried ingredients to one side of the pan and apply more oil to the empty space, then pour in the beaten eggs. (A) Add the rice before the egg firms up and mix everything in the pan. Sprinkle salt and pepper, and then add the remaining onion, Drizzle in soy sauce from the side of the pan (B) and mix briefly. When cooked, divide between plates and scatter the chopped green onions on top.</t>
+  </si>
+  <si>
+    <t>Really Really Bad (Good) Staff Soup</t>
+  </si>
+  <si>
+    <t>A Western-style clear soup made with sea bream and kombu kelp</t>
+  </si>
+  <si>
+    <t>1*null*Sea Bream Head,1*sheet*Kombu,2*null*turnips,6*null*Asparagus (pencil spears),0.5*null*Lemon,5*cups*Water,2*teaspoons*Salt,1*dash*Soy Sauce</t>
+  </si>
+  <si>
+    <t>1. Soak the kombu in water for at least 30 minutes. Slice the sea bream head into pieces if necessary and place it in a separate pot of boiling water deep enough to cover the fish head. When the surface becomes white, remove and place in another bowl of cold water, then scrub clean to remove blood and stains ©.||2. Cut turnips into wedges and slice greens finely. Peel the bottom third of asparagus and slice into 2inch (5 cm) pieces. Slice lemon into wheels.|| 3. Pour water from step 1 and sea bream into the same pot and bring to a boil. Skim the scum off the top and lower heat to medium, Add turnip wedges(D) and let simmer, skimming regularly.|| 4. After 10 minutes, add asparagus and simmer for 5 minutes. Add salt, and soy sauce to taste. Transfer to bowls, add lemon slices, and scatter turnip greens on top.</t>
+  </si>
+  <si>
+    <t>Pirate Box Lunches for Crossing the Desert</t>
+  </si>
+  <si>
+    <t>Lightly Breaded Fried Chicken</t>
+  </si>
+  <si>
+    <t>2*boneless*Chicken Thighs (skinless),1*clove*Garlic ( grated),1*teaspoon*Salt,1*tablespoon*sake,1*sprinkle*Black Pepper,4*tablespoons*Flour,4*tablespoons*Vegetable Oil,4*null*Sausages,4*hard-boiled*Eggs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treasure Splitting Sandwiches </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg and Crab Sandwiches </t>
+  </si>
+  <si>
+    <t>6*Slices*Bread,3*null*Eggs,2*oz*Crab Meat (boiled),2*tablespoons*Mayonnaise*1*stick*Butter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monstrous Grilled Giant Sandora Dragon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roast Beef cooked in the frying pan </t>
+  </si>
+  <si>
+    <t>500*grams*Steak (prime whole),0.5*clove*Garlic,1*teaspoon*Salt,1*sprinkle*Black Pepper,1*tablespoon*Vegetable Oil,0.5*null*Onion ,0.6*clove*Garlic (for sauce),3*tablespoons*Sake,2*tablespoons*Soy Sauce,0.5*tablespoons*Butter,1*tablespoon*Vinegar</t>
+  </si>
+  <si>
+    <t>1. Boil eggs whole for 12 minutes until hard-boiled. Let cool. Peel off shells and cut them into thick slices. Tear crab meat by hand. Mince onion, then soak in water, remove, and press the liquid out. Put egg, crab, and onion into a bowl, then mix with mayonnaise (A), Spread butter on the bread slices, then divide the mix to make three sandwiches.</t>
+  </si>
+  <si>
+    <t>1. Trim fat and sinew from the chicken thighs and cut into bite-size pieces—grate garlic. Put the chicken into a bowl, add mix garlic, salt, pepper and sake then marinate for 20-30 minutes.||2. Sprinkle flour over the thighs. Heat vegetable oil in a pan on medium heat, then fry chicken in batches for 4-5 minutes undisturbed on each side.</t>
+  </si>
+  <si>
+    <t>1. Let the beef sit at room temperature for 30 minutes, and grate onion and garlic for sauce. Just before cooking, rub the other garlic half against meat( C), then rub on salt and pepper. Pour oil on a heated frying pan and cook the meat surface on medium heat (D). Cover and heat on low for 6-8 minutes, then turn over and heat for another 4-5 minutes.||2. Remove from pan, wrap in aluminum foil, and let sit for 15 minutes to heat through (E).||3. Add onions, garlic and saké to the meat juice in the frying pan. Once bubbling, mix in soy sauce and butter. Once mixed in, turn off the heat, add vinegar and mix again.||4. Slice meat thinly and transfer to plate, then drizzle sauce from pan, Add mustard or wasabi as desired.</t>
+  </si>
+  <si>
+    <t>Luffy's Favorite Meat on the Bone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Scotch Egg made with Chicken </t>
+  </si>
+  <si>
+    <t>4*null*Chicken Drumsticks,4*null*Eggs (hard-boiled),0.25*cup*Breadcrumbs,3*tablespoons*Milk,500*grams*Chicken,1*teaspoon*Salt,1*dash*Black Pepper,1*null*Egg,1*spalsh*Vegetable Oil</t>
+  </si>
+  <si>
+    <t>1. Make chicken drumstick “tulips.” Use kitchen scissors to cut the meat loose from the handle end of the drumstick (A). Roll the meat down the bone until it is fully inside-out at the end.||2. Soak the breadcrumbs in milk. Knead ground chicken, salt, pepper and egg in a bowl, then add breadcrumbs and knead again.||3.  Fold the meaty end of the drumstick around a hard-boiled egg (B). If the meat doesn't cover well enough, add cuts to loosen it up. Oil hands lightly and cover drumstick and egg with the breadcrumb mixture from the previous step.||4. Bake at 400 degrees Fahrenheit  (200 degrees Celsius) for 15-20 minutes, watching carefully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -923,6 +998,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -945,7 +1026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -970,6 +1051,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1306,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2747,6 +2834,144 @@
         <v>12</v>
       </c>
     </row>
+    <row r="63" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F63" s="1">
+        <v>30</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F64" s="1">
+        <v>60</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F65" s="1">
+        <v>50</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="F66" s="1">
+        <v>30</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F67" s="1">
+        <v>70</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F68" s="1">
+        <v>40</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished One Piece Recipes
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkish\Downloads\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B016B0B7-B48A-4935-A34A-2D5DFFDFBBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEFA7CD-4F85-44BE-A0F7-01D8ED3F4C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
   <sheets>
     <sheet name="RecipesTest" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="383">
   <si>
     <t>Name</t>
   </si>
@@ -957,6 +957,236 @@
   </si>
   <si>
     <t>1. Make chicken drumstick “tulips.” Use kitchen scissors to cut the meat loose from the handle end of the drumstick (A). Roll the meat down the bone until it is fully inside-out at the end.||2. Soak the breadcrumbs in milk. Knead ground chicken, salt, pepper and egg in a bowl, then add breadcrumbs and knead again.||3.  Fold the meaty end of the drumstick around a hard-boiled egg (B). If the meat doesn't cover well enough, add cuts to loosen it up. Oil hands lightly and cover drumstick and egg with the breadcrumb mixture from the previous step.||4. Bake at 400 degrees Fahrenheit  (200 degrees Celsius) for 15-20 minutes, watching carefully</t>
+  </si>
+  <si>
+    <t>Yagara Bull's Favourite Steamed Water-Water Meat</t>
+  </si>
+  <si>
+    <t>A steamed spare rib dish</t>
+  </si>
+  <si>
+    <t>500*grams*Pork Spare Ribs,0.5*teaspoon*Salt,1*dash*Black Pepper,1*null*Celery Stalk,0.5*null*Carrot,0.25*null*Daikon Radish (cut lengthwise),0.5*head*Lettuce,0.5*null*Green Onion,1*tablespoon*Sesame Oil,7*tablespoons*Ponzu,1*sprinkle*Garlic (grated)</t>
+  </si>
+  <si>
+    <t>1. Pat spare ribs, salt, and pepper into a plastic bag knead well, and let sit for one hour (A). Peel celery, carrot, and daikon into ribbons (B). Tear lettuce into reasonably-sized pieces.||2. Mince green onion for the tare sauce. Heat sesame oil in a frying pan, then pour over spring onion in a heat-resistant bowl, add ponzu, and mix.||3. Place spare ribs into a steam cooker and steam for 20 minutes, When the meat is tender, add vegetables to steamer (C), and once heated, remove and serve. Drizzle tare sauce as you eat and add grated garlic as desired.</t>
+  </si>
+  <si>
+    <t>Impel Down's Roast Hummingbird</t>
+  </si>
+  <si>
+    <t>Roasted chicken stuffed with special rice pilaf</t>
+  </si>
+  <si>
+    <t>1*large*Chicken,2*teaspoon*Salt,2*sprinkles*Black Pepper,0.5*null*Onion,1*tablespoon*Vegetable Oil,0.25*cup*Water,1.5*null*Cooked Rice,0.5*null*Tomato,1*tablespoon*Parsley (chopped)</t>
+  </si>
+  <si>
+    <t>1. Remove neck and organs if present, and rinse chicken clean. Dry excess liquid and rub salt and pepper onto the exterior and interior.||2. Slice onion thinly and cube tomato. Mix rice, tomato, parsley,1 teaspoon of salt and 1 sprinkle of pepper and stuff chicken (A). Use a large toothpick to pin rear shut so stuffing doesn't spill.Rub vegetable oil onto exterior of chicken.||3. Spread out onion onto a large oven tray and rest chicken on top (C). Add water and chicken neck, split in two. Put into the oven at 400 degrees F (200 degrees C) for 40-50 minutes, rotating the tray partway and occasionally scooping juices back onto the chicken. Once cooked to an internal temperature of 165 degrees F (74 degrees C), extending cook time as needed, turn off the heat and leave in the oven for another 10-15 minutes.||4. Strain juice from the tray and use it as gravy. If the onions are dry and there is little juice, transfer to a small pot, add water (2-3 02./50-80 ml) and boil, then strain. Cut the chicken into servings, then add gravy and sprinkle salt and pepper to taste.</t>
+  </si>
+  <si>
+    <t>Lakeside Campsite Hot Rock Stew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A rich pork stew, no roux required </t>
+  </si>
+  <si>
+    <t>600*grams*Pork Butt,1*teaspoon*Salt,1*dash*Black Pepper,1*clove*Garlic,6*null*Mushrooms,0.5*null*White Onion (peeled),1*tablespoon*Vegetable Oil,2*tablespoons*Butter,0.25*cup*Flour,400*ml*Red Wine,400*ml*Chicken Stock,2*null*Bay Leaves,30*grams*Raisins,5*tablespoons*Ketchup</t>
+  </si>
+  <si>
+    <t>1. Cut pork into half-inch (1.5 cm) pieces and place on a tray, then coat with salt, pepper, and flour (A). Cut garlic in half, remove germ, and crush with the flat of your knife. Halve mushrooms and cut onion into 4 wedges.||2. Put vegetable oil and garlic into a pot and cook on medium heat. When fragrant, remove the garlic and add half of butter. When butter is melted, add meat and all the flour from the tray. Cook both sides until you see it start to sear.||3. Add red wine. Once the alcohol has been brought to a boil, add chicken stock (B) cooked garlic from the previous step, and bay leaves. When it boils again and a froth starts to build, remove bay leaves and skim the top (C). Add raisins and ketchup. Cover with pot lid ajar and simmer on low heat for 40 minutes||4. Place the other half of the butter into a heated frying pan. Once melted, add mushrooms and onions to fry until browned, then add to the main pot and cook for another 20 minutes. Add salt to taste.</t>
+  </si>
+  <si>
+    <t>Absalom's Croquettes</t>
+  </si>
+  <si>
+    <t>Potato croquettes, packed with beef</t>
+  </si>
+  <si>
+    <t>4*small*Potatoes,200*grams*Mixed Beef,0.5*null*Onion,1*cup*Vegetable Oil,1*teaspoon*Salt,1*sprinkle*Black Pepper,1*tablespoon*Butter,0.5*cup*Flour,2*large*Eggs,1.5*cups*Panko,1*null*Cabbage (jullienne-cut),1*splat*Worcestershire Sauce</t>
+  </si>
+  <si>
+    <t>1. Steam potatoes in a steam cooker for about 40 minutes until they soften. Cut beef into 3-quarter  inch (2 cm) strips (A) and mince the onion.||2. Pour vegetable oil into a heated frying pan and cook beef on medium heat. Once adequately heated, add onions and cook for 3-4 minutes until translucent, then flavour with salt (half tsp.) and black pepper. Transfer food to a tray to cool.||3. While the potatoes are still hot, peel them and place them in a bowl. Mash with a ladle or spatula, add butter and salt half tsp.) and mix (B). Add beef and onions, mix, then transfer to a tray to cool.||4. Separate the mixture into 10 equal parts and mould it into an oval shape (C). Dip into flour, beaten egg yolks, and panko in that order, then frying oil heated to 360 degrees F (180 degrees C) for three minutes, turning over partway.||5. Remove and place on a cooling rack over a baking sheet with paper towels beneath to catch oil. Transfer to serving plate with cabbage and drizzle sauce over.</t>
+  </si>
+  <si>
+    <t>Davy Back Fight Frankfurters</t>
+  </si>
+  <si>
+    <t>A rich pot-au-feu where the infused oil is the key</t>
+  </si>
+  <si>
+    <t>8*null*Frankfurters,2*large*Idaho Potatoes,1*null*Carrot,0.5*head*Cabbage,2*small*Onions,8*cups*Chicken Stock,2*teaspoon*Salt,1*clove*Garlic,1*tablespoon*Olive Oil,1*sprinkle*Parmesan Cheese,1*dash*Black Pepper</t>
+  </si>
+  <si>
+    <t>1. Lightly split frankfurters to allow flavour to blend. Peel potatoes and cut in half. Peel the carrot and cut it into bite-size quarters. Cut cabbage into four equal wedges and use toothpicks or skewers to hold in place. Peel onions and use whole. Mince garlic.||2. Heat chicken stock, salt, carrots, and onions in a pot. Bring to a boil, then reduce heat to low and let simmer for 20 minutes, Add cabbage and potatoes and simmer for 20 more minutes. When vegetables are soft, add frankfurters and simmer for 10 more minutes.||3. Cook mix garlic and olive oil in a frying pan on medium heat: When garlic begins to brown, add to pot. If flavor is lacking, add extra salt, Parmesan cheese, and black pepper to taste, Once served, remove toothpicks from the cabbage and enjoy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sky Seafood Extravaganza </t>
+  </si>
+  <si>
+    <t>Shrimp and Scallop Marinade</t>
+  </si>
+  <si>
+    <t>6*fresh*Scallops,10*null*Shrimp (shell on),1*null*Grapefruit,1*null*Celery Stalk (with leaves),0.5*null*Red Onion,1*knob*Ginger Root,1*null*Limes Juice,1*sprinkle*White Pepper,0.5*teaspoon*Salt,1*splash*Olive Oil</t>
+  </si>
+  <si>
+    <t>1. Place scallops in boiling water for 30 seconds, then remove and wash in cold water (A), Cut in half to make coins. Remove the shrimp heads and back vein, then boil with the shell on until they turn pink and pour into a strainer. When they are cool enough to touch, peel off the shell (B) and cut in half if too large. Remove peel and rind from grapefruit, then slice into wedges. Remove strings from celery, then slice diagonally. Slice red onion thinly and peel and cut ginger into julienne strips.||2. Place shrimp and scallops into a bowl. Add lime juice, salt, and white pepper, and mix. Add red onion, celery, and ginger, and mix again. Add grapefruit pieces and chill in refrigerator.||3. After mixing again, transfer to the serving dish and garnish with celery leaves. Add olive oil if desired.</t>
+  </si>
+  <si>
+    <t>Elephant True Bluefin Saute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooked Blue Marlin with a Special Sweet Sauce </t>
+  </si>
+  <si>
+    <t>4*fillets*Blue Marlin,1*dash*Salt,1*sprinkle*White Pepper,1*tablespoon*Olive Oil,0.5*null*Onion,2*tablespoons*Olive Oil (sauce),1*teaspoon*Garlic (grated),2*tablespoons*Water,2*teaspoons*Honey,0.6*teaspoon*Salt (sauce),1*teaspoon*Soy Sauce,3*tablespoons*White Sesame seeds (hulled)</t>
+  </si>
+  <si>
+    <t>1. Sprinkle salt and white pepper on the marlin and mince onion for sauce. Add olive oil to a heated frying pan and cook marlin pieces on both sides. Remove once cooked to 125 degrees F, roughly 5-7 minutes per side for a 1-and-a-half-inch thick steak (A).||2. Using the same frying pan, heat the olive oil for the sauce, then fry the onions until translucent. Add garlic, water, honey, salt, soy sauce, and ground sesame (B).||3. Serve marlin on a plate and drizzle the sauce over it.</t>
+  </si>
+  <si>
+    <t>Sky Fish Saute</t>
+  </si>
+  <si>
+    <t>Fried Horse Mackerel with Melted Cheese</t>
+  </si>
+  <si>
+    <t>4*whole*Horse Mackerel,1*ball*Mozzarella Cheese,1*dash*Salt,1*sprinkle*White Pepper,4*teaspoons*Flour,1*null*Egg,6*tablespoons*Panko,1*splash*Vegetable Oil,1*null*Tomato,0.25*null*Onion,6*tablespoons*Ketchup,2*teaspoons*Vinegar,2*teaspoons*Olive Oil,1*dash*Hot Sauce,1*null*Red Onion,1*bits*Basil</t>
+  </si>
+  <si>
+    <t>1. Split the horse mackerel for frying, leaving a hinge. Cut the mozzarella into halves and third-inch (8 mm) slices.||2. Mince the tomato and onion for the sauce and mix with ketchup, vinegar, olive oil and hot sauce.||3. Sprinkle salt and white pepper on the mackerel, then place mozzarella slices in between the fillets (A). Dip into flour, beaten egg, and panko in order.||4. Fill the frying pan with about half an inch (1 cm) of vegetable oil and heat to 320 degrees F (160 degrees C). Add breaded mackerel (B). Fry for about five minutes total, turning over once. Remove and place on a cooling rack over a paper towel-lined tray to drain oil.||5. Slice red onion thinly and garnish fish with sauce mixture and basil.</t>
+  </si>
+  <si>
+    <t>Roasted Sky Shark</t>
+  </si>
+  <si>
+    <t>Sanji's take on steam-fried Salmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3*fillets*Salmon,1*dash*Salt,1*dash*White Pepper,0.25*head*Cabbage,0.5*null*Onion,0.5*null*Carrot,1*splash*Vegetable Oil,1*tablespoon*Sake,1.5*tablespoon*Sugar,3*tablespoons*Miso,1.5*tablespoon*Butter,0.5*tablespoon*Soy Sauce </t>
+  </si>
+  <si>
+    <t>1. Lightly sprinkle salt and white pepper on the salmon. Roughly cut the cabbage, slice the onion into 4-inch (1 cm) pieces, and cut the carrot into short strips.||2.  Pour oil onto a heated frying pan and cook salmon, skin side down, on medium heat for 2-3 minutes, until browned.||3. Turn over the salmon, then add cabbage, onion, and carrot. Swirl in saké, Sprinkle sugar and miso here and there and add dabs of butter on top of the miso clumps (A). Carefully cover with aluminum foil and steam for 6-7 minutes (B).||4. Remove foil, tear salmon into chunks, and mix contents. Add soy sauce and turn off heat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sliced Octopus </t>
+  </si>
+  <si>
+    <t>Delicious Clams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nice Savory Octopus Snacks </t>
+  </si>
+  <si>
+    <t>Creamy and steamed clams in wine</t>
+  </si>
+  <si>
+    <t>150*grams*Fresh Octopus (sushi-grade),0.25*null*Onion,0.5*tablespoon*Vinegar,2*pinches*Salt,1*tablespoon*Olive Oil,1*dash*Paprika</t>
+  </si>
+  <si>
+    <t>1. Mince onion and soak in water. Slice the octopus diagonally and arrange it on a plate.||2. Mix salt into vinegar, then mix in olive oil.||3. Pour the sauce on octopus. Dry out the onions and scatter over the octopus. Sprinkle paprika.</t>
+  </si>
+  <si>
+    <t>500*grams*Clams (in shell),0.25*null*Onion*1*clove*Garlic,100*ml*White Wine,1*sprinkle*White Pepper,1*tablespoon*Butter,50*ml*Heavy Cream,1*flat-leaf*Parsley</t>
+  </si>
+  <si>
+    <t>1. Place clams in a bowl of salted water at roughly seawater salinity. Cover with aluminium foil and put in a dark place for 2-3 hours until they have purged grit.||2. Mince onions. Cut garlic in half vertically, remove the stem, and crush with the flat of the knife. Chop parsley roughly.||3. Place clams, onions, garlic, and white wine in a frying pan, turn on the heat and cover. Once the clams open, sprinkle white pepper, add butter, and pour heavy cream. Transfer to a dish and sprinkle parsley. Cook leftover liquid and pour over rice for a risotto if desired.</t>
+  </si>
+  <si>
+    <t>Water-Water Cabbage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japanese style bagna cuada </t>
+  </si>
+  <si>
+    <t>4*leaves*Napa Cabbage,0.5*null*Carrot,0.5*null*Yellow Bell Pepper,6*tablespoons*Mayonnaise,2*tablespoons*Miso Paste,2*tablespoons*Milk,1*sprinkle*Chilli Powder</t>
+  </si>
+  <si>
+    <t>1. Place cabbage, carrot, and bell pepper into a bowl of cold water until they are firm.||2. Dry off cabbage and separate the leaf from the stalk. Cut leaf to bite size, and slice stalk into sticks. Slice carrot into long wedges with the skin on, Remove stem and seeds from bell pepper and cut into long, thin pieces.||3. Mix mayonnaise, miso paste, milk and chilli powder to make a sauce. Then use it as a dip for the vegetables.</t>
+  </si>
+  <si>
+    <t>Laughing Mushrooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mushrooms packed with fragrant herbs </t>
+  </si>
+  <si>
+    <t>6*null*Shiitake Mushrooms,1*pack*Shimeji Mushrooms,2*null*King Oyster Mushrooms,3*pieces*Bacon,1*tablespoon*Vegetable Oil,2*sprigs*Rosemary,1*teaspoon*Salt,1*sprinkle*Black Pepper,1*pat*Butter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Remove the shiitake mushrooms from their base and cut them into half-inch (1 cm) slices. Remove the shimeji mushrooms from their base and separate them into small bunches. Trim king oyster mushrooms to a length of 1 and a half inches (3cm) and slice thinly. Cut bacon into quarter-inch (7 mm) slices.||2. Put vegetable oil and rosemary into a frying pan and heat on medium. When oil is fragrant, fry bacon briefly, then add all mushrooms and mix. Cover and steam on low heat for 4 minutes.||3. Remove the lid, add salt, and mix again. Cover again and continue steaming for 4-5 minutes, stirring occasionally, until the liquid is gone and the bacon is fried and no longer appears pink. If needed, add more salt and pepper for flavour, then add butter, mix, and turn off heat.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stir-fried Bean Sprouts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A stir fry with anchovies and garlic </t>
+  </si>
+  <si>
+    <t>2*bags*Bean Sprouts,2*cloves*Garlic (peeled),6*null*Anchovies,1*splash*Olive Oil,1*sprinkle*Black Pepper,1*sprinkle*Salt</t>
+  </si>
+  <si>
+    <t>1. Mince garlic and chop anchovies finely.||2. Put olive oil and garlic into a frying pan on medium heat. When garlic is golden, add bean sprouts and cook on high heat.||3. When bean sprouts are translucent, add anchovies and black pepper and mix. Taste test and add more salt if needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pommed Paille </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crispy Shoestring Potatoes </t>
+  </si>
+  <si>
+    <t>3*null*Potatoes (peeled),60*grams*Shredded Cheese,1*splash*Vegetable Oil,1*sprinkle*Salt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Place finely cut shoestring potatoes using a mandoline at a one-third-inch setting if available, and mix with cheese.||2. Pour a generous amount (around a quarter cup) of oil into a frying pan. Pack a quarter of the potatoes tightly and fry on low heat for 7-8 minutes. Turn over and fry another 7-8 minutes, until both sides are crispy. Be careful not to prod too much while frying, as it will come apart. Once cooked, dab dry with paper towels, then sprinkle with salt.||3. Repeat for the other three portions.
+</t>
+  </si>
+  <si>
+    <t>Neptunian Penne Gorgonzola</t>
+  </si>
+  <si>
+    <t>Rich pasta made with two kinds of cheese</t>
+  </si>
+  <si>
+    <t>180*grams*Penne,2*slices*Ham,100*ml*Milk,100*ml*Heavy Cream,50*grams*Blue Cheese,3*tablespoons*Parmesan Cheese (grated),1*dash*Black Pepper,1*flat-leaf*Parsley,7*cups*Water,1*tablespoon*Salt</t>
+  </si>
+  <si>
+    <t>1. Boil about 6-7 cups (1,500 ml) of water, and add 1 tbsp. (15 g) of salt, and boil penne for 1 minute less than indicated on the package. Slice ham into quarter-inch (5 mm) pieces.||2. Starting with a third cup of milk and adding more as needed, heat milk and cream in a pan on medium heat for about 2 minutes before the penne is cooked. Mix in crumbled blue cheese. When it has half melted, add penne and ham and simmer for 1 minute or until sauce has thickened, Add parmesan and mix.||3. Lastly, add pepper to taste, and sprinkle chopped parsley on top.</t>
+  </si>
+  <si>
+    <t>Luffy and Zoro Bread Crusts</t>
+  </si>
+  <si>
+    <t>Stylish Fried Bread Crusts</t>
+  </si>
+  <si>
+    <t>6*slices*Bread (crusts),1*heap*Cinnamon Sugar,1*can*Condensed Milk,1*splash*Frying Oil</t>
+  </si>
+  <si>
+    <t>1. Heat frying oil to 340 degrees F (170 degrees C). Place bread crusts in the pan, frying for about 90 seconds until golden brown. Remove and place on a drying rack over a cooking sheet lined with paper towels to remove oil.||2. Dust with cinnamon sugar as desired, and dip into condensed milk to eat.</t>
+  </si>
+  <si>
+    <t>Exploding Apples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baked Apples you can make in the toaster oven </t>
+  </si>
+  <si>
+    <t>2*null*Apples,2*null*Cinnamon Sticks,2*teaspoons*Lemon Juice,4*null*Cardamon Pods,1.5*tablespoon*Butter,4*teaspoons*Granulated Sugar</t>
+  </si>
+  <si>
+    <t>1. Slice apples in half lengthwise and scoop out seeds and core with a spoon. Break cinnamon sticks into 1-inch (3 cm) pieces and dampen them with water to keep them from burning.||2. Add lemon juice, cardamom, and butter to the apple surface and stick cinnamon into the centre.||3. Scatter granulated sugar on surface liberally, then cover skin side of apple in foil and bake in toaster oven with a sheet pan underneath for 20 minutes.</t>
+  </si>
+  <si>
+    <t>Oda's Favourite Sea Chicken Onigiri</t>
+  </si>
+  <si>
+    <t>The secret treasure of rice balls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5*cups*Rice (cooked and warm),1*can* Sea Chicken Tuna,1*tablespoon*Miso Paste,0.5*teaspoon*Sugar,2*null*Green Onion,1*heap*Dried Seaweed Sheets,1*sprinkle*Salt </t>
+  </si>
+  <si>
+    <t>1. Mince green onion, Drain oil briefly from tuna can, then fry in a pan on medium heat, mixing in miso and sugar. Add green onion and mix briefly, then turn off the heat. ||2. Wet hands with water, sprinkle with salt and surround a dab of tuna mixture with the cooked rice to form an onigiri. Cut nori sheet to the appropriate size and wrap it.</t>
   </si>
 </sst>
 </file>
@@ -1393,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2972,6 +3202,443 @@
         <v>78</v>
       </c>
     </row>
+    <row r="69" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F69" s="1">
+        <v>100</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F70" s="1">
+        <v>115</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="F71" s="1">
+        <v>90</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F72" s="1">
+        <v>80</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F73" s="1">
+        <v>95</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="F74" s="1">
+        <v>40</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F75" s="1">
+        <v>30</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="F76" s="1">
+        <v>25</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F77" s="1">
+        <v>25</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="F78" s="1">
+        <v>10</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="F79" s="1">
+        <v>210</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F80" s="1">
+        <v>20</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="F81" s="1">
+        <v>35</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F82" s="1">
+        <v>10</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="F83" s="1">
+        <v>80</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="F84" s="1">
+        <v>30</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="F85" s="1">
+        <v>7</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="F86" s="1">
+        <v>35</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="F87" s="1">
+        <v>20</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished the recipes for Genshin
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkish\Downloads\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C66FD7-9952-4078-8122-E1CEDFBC7BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FADF47-F3C9-49E6-B80A-BE6174A05E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="562">
   <si>
     <t>Name</t>
   </si>
@@ -1456,6 +1456,276 @@
   </si>
   <si>
     <t>1. To make the cupcakes: Preheat the oven to 350 degrees F (177 degrees C). Prep a cupcake pan with paper liners.||2. In a medium bowl, whisk together the cake flour, baking powder, and salt.||3. In the bowl of an electric mixer, cream the butter and sugar until fluffy.||4. Add the eggs and vanilla, stirring until just combined. Stir in the flour mixture, alternating with buttermilk. Spoon the batter into the prepped cupcake pan.||5. Bake for 16 to 17 minutes, or until a toothpick inserted in the center comes out clean.||6. Let cool on a wire rack.||7. To make the frosting: In a large bowl with a handheld mixer on low, cream the butter while slowly adding the confectioners’ sugar. Stir in the heavy whipping cream, vanilla, and salt.Add food coloring and stir, until the frosting becomes a light pink color.||8. Turn the mixer up to medium-high and whip for 10 to 15 seconds, until light and fluffy.||9. To assemble: Pipe the frosting onto the cupcakes to serve.</t>
+  </si>
+  <si>
+    <t>Grilled Chicken Skewers</t>
+  </si>
+  <si>
+    <t>Genshin</t>
+  </si>
+  <si>
+    <t>Simple to make chicken skewers</t>
+  </si>
+  <si>
+    <t>1*tablespoon*Dried Oregano,1*tablespoon*Dijon Mustard,0.5*teaspoon*Dried Thyme,1*null*Lemon Juice,3*cloves*Garlic (minced),2*tablespoons*Olive Oil,1*tablespoon*Smoked Paprika,0.25*cup*Soy Sauce,1*tablespoon*Maple Syrup,3*tablespoons*Orange Juice,0.25*cup*Chicken Stock,0.5*teaspoon*Pepper,2*null*Chicken Breasts (boneless and skinless),1*pound*Cremini Mushrooms (whole)</t>
+  </si>
+  <si>
+    <t>1.. In a large bowl, mix together all the ingredients except the chicken and mushrooms to create a marinade.||2. Cut the chicken breasts into bite-size pieces. Place the chicken and mushrooms in the bowl of marinade and stir until thoroughly coated. Cover and refrigerate for 4 to 10 hours, stirring occasionally.||3. If you’re using bamboo skewers, soak them in water for a few minutes right before the chicken and mushrooms are done marinating to keep them from burning when it comes time to cook. Then pat dry.||4. Thread the chicken and mushrooms on the skewers, discarding any remaining marinade. Grill on high heat until cooked, 5 to 7 minutes, or bake in the oven at 430 degrees F for 8 to 10 minutes. Enjoy!</t>
+  </si>
+  <si>
+    <t>Fried Radish on a Stick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The delicious yet subtle flavour of radishes </t>
+  </si>
+  <si>
+    <t>1*large*Daikon Radish (white),1*pinch*Salt,2*large*Eggs,0.75*cup*Flour,1*null*Green Onion (thinly sliced),1*teaspoon*Vegetable Stock Powder,1*teaspoon*Ginger ( minced),1*teaspoon*Garlic Powder,1*teaspoon*Onion Powder,1*teaspoon*Paprika,1*pinch*Pepper,1*splash*Vegetable Oil</t>
+  </si>
+  <si>
+    <t>1. Using a vegetable peeler, remove the skin from the radish. Then use a grater to shred the radish into a large bowl.||2. Sprinkle the grated radish with a pinch of salt and let sit for a few minutes to draw out the water from the radish. Drain the excess water and use a paper towel to squeeze out any remaining water fromthe radish.||3. Add the eggs, flour, green onion, vegetable stock, ginger, and remaining seasonings. Mix well.||4. Shape the radish mixture into balls. (The smaller the balls, the faster they will cook.)||5. Add vegetable oil to a skillet over medium heat. Gently place the radish balls in the oil and fry all together for 5 minutes or until golden brown, turning them occasionally to ensure all sides are frying evenly. Serve with an aioli or your favorite sauce.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crispy Potato-Shrimp Balls </t>
+  </si>
+  <si>
+    <t>These cute and compact balls of fried goodness make this dish the perfect appetizer for your next gathering with friends!</t>
+  </si>
+  <si>
+    <t>20*raw*Shrimp,3*medium*Russet Potatoes (peeled and cut into 1-inch cubes),1*tablespoon*Unsalted Butter,1*null*egg Yolk,1*large*Egg,2*teaspoons*Salt,1.5*teaspoon*Pepper,2*teaspoons*Paprika,0.25*teaspoon*Dried Thyme,2*teaspoons*Garlic Powder,1*cup*Flour,1*cup*Panko Breadcrumbs,1*splash*Vegetable Oil</t>
+  </si>
+  <si>
+    <t>1. Peel off the shrimp shells, leaving the tails on. Season with a pinch of salt and pepper and set aside.||2. Boil the potatoes in water over medium-high heat for 15 to 20 minutes, or until fork tender. Mash them using a potato masher, then add in the unsalted butter and egg yolk. Mix until smooth. Your potatoes should be creamy but not soupy. If they are too soupy, add a little flour until the potatoes are thickened to a creamy texture.||3. Add the 1 and a half teaspoons salt, 1 teaspoon pepper, paprika, thyme, and garlic powder. Mix well.||4. Scoop out a third cup of the potato mixture and use your hands to form it into a ball. Using your thumb, poke a hole in the top of the ball, place a shrimp in the hole, then cover the shrimp with the potatoes until just the shrimp tail is sticking out. Squeeze slightly to tighten everything and make sure the shrimp stays locked inside.||5. Pour 1 cup flour into a shallow dish. Then crack the egg into a separate dish and whisk to combine the yolk and egg white. Add the panko crumbs to another shallow dish.||6. Carefully roll a potato-shrimp ball into the flour, shaking off any excess. Then roll in the egg wash and then the bread crumbs. Make sure the ball is fully covered with all three ingredients. Set aside on a large plate or tray and repeat for the remaining potato-shrimp balls.||7. Fill a medium frying pan halfway with vegetable oil and heat to between 350 degrees F to 375 degrees F over medium heat. Fry the shrimp balls together until the outside is golden brown, about 4 minutes, turning occasionally to ensure all shrimp balls are frying evenly.||8. Remove from the oil and let the potato-shrimp balls cool for a few minutes. Enjoy by themselves or serve with an aioli or your favorite sauce.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Cold Cuts </t>
+  </si>
+  <si>
+    <t>A platter of delicious meats</t>
+  </si>
+  <si>
+    <t>1*package*Prosciutto,7*slices*Deli Ham,2*links*Cured Chorizo,1*scoop*Cherry Tomatoes,1*heap*Lettuce Leaves</t>
+  </si>
+  <si>
+    <t>1. On a flat platter or board, arrange the prosciutto slices as light and airy ribbons covering a third of the serving plate.||2. On another third of the platter, fan the ham pieces out like a deck of cards, or fold each piece in half twice so they are easy to grab.||3. Cut the sausages into round slices and arrange on the last third of the platter.||4. Place some cherry tomatoes and a few leaves of lettuce in the middle of the platter. You can also tuck a few lettuce leaves under the meat slices and along the edge of the platter.</t>
+  </si>
+  <si>
+    <t>Elegant Egg Roll</t>
+  </si>
+  <si>
+    <t>Eggs to fluffy perfection and rolling them into a rectangular loaf</t>
+  </si>
+  <si>
+    <t>8*null*Eggs,2.5*tablepoons*Water,1*tablespoon*Soy Sauce,0.75*teaspoon*Sugar,1*tablespoon*Olive Oil</t>
+  </si>
+  <si>
+    <t>1. In a medium bowl, combine the eggs, water, soy sauce, and sugar. Using a whisk, beat until well combined.||2. Heat a tamagoyaki pan (rectangular Japanese omelet pan) or a small frying pan over medium heat. Using a pastry brush, lightly coat the bottom of the pan with olive oil.||3. Pour a thin layer of the egg mixture to cover the surface of the pan. When it’s about 80 percent cooked but still wet on the surface, use chopsticks or wooden tongs to start gently rolling in the edges to form a rolled omelet. Move the rolled omelet to one side of the pan.||4. Brush the pan with oil again and pour in another thin layer of the egg mixture. Using a spoon, gently lift the previously made omelet and spread some of the uncooked egg mixture underneath. This willhelp both omelets stick together. When this next layer of eggs is 80 percent cooked but the surface is still wet, start with the previously made omelet and gently roll it up with the new layer. Set to one side of the pan. Repeat this process until the egg mixture is gone. Your omelet will have 3 to 4 layers.||5. Transfer the rolled omelet onto a cutting board and allow to rest for several minutes. Cut into even 2-inch slices and serve.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loaded Baked Potato </t>
+  </si>
+  <si>
+    <t>One-of-a-kind baked potato side dish!</t>
+  </si>
+  <si>
+    <t>3*large*Baking Potatoes,1*teaspoon*Olive Oil,4*tablespoons*Unsalted Butter (cut into cubes),0.5*cup*Green Onions (chopped),5*null*Cremini Mushrooms (chopped),0.5*cup*Half and Half,0.5*cup*Sour Cream,1*sprinkle*Salt,1*spinkle*Pepper,1*cup*Cheddar Cheesew (shredded)</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 400 degrees F. Pierce the potatoes several times with a fork and rub with olive oil. Bake until tender, 50 to 75 minutes. While baking, you can check if the potatoes are done by sticking a skewer or a fork into them; if soft, they are ready.||2. Remove the potatoes from the oven. When cool enough to handle, slice the top off each potato horizontally (about 1 inch). Scoop out the potato pulp and transfer it to a large mixing bowl, leaving thin potato shells. Set the potato skins aside and reduce the oven temperature to 375 degrees F.||3. In a small skillet, melt the butter over medium-high heat, then add the onions and mushrooms and sauté until tender, about 5 minutes.||4. In the mixing bowl, using a potato masher, mash the potato pulp. Stir in the sauteed onions and mushrooms, half-and-half, sour cream, salt, and pepper. Stuff this mixture into the 3 potato shells and top with cheddar cheese.||5. Place the stuffed potatoes on a baking sheet and bake until heated through, about 20 minutes. Top with extra chopped green onions to serve.</t>
+  </si>
+  <si>
+    <t>Crispy Baked HashBrowns</t>
+  </si>
+  <si>
+    <t>Crispy Baked Hash Browns</t>
+  </si>
+  <si>
+    <t>1*package*Hashbrown Potatoes (frozen,shredded and thawed),2*null*Eggs,1*cup*Cheddar Cheese (shredded),1*pinch*Salt,1*pinch*Pepper,1*teaspoon*Ground Cumin,1*teaspoon*Dried Mint,0.5*teaspoon*Garlic Powder,0.5*teaspoon*Onion Powder,0.5*cup*Unsalted Butter (melted)</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 400 degrees F. Line a baking sheet with parchment paper and set aside.||2. Pour the shredded potatoes into a large bowl. In a small separate bowl, whisk the eggs. Add the eggs to the potatoes along with the shredded cheese and all the seasonings. Toss to coat everything evenly. Pour the melted butter over the top and toss once again to coat.||3. Spread the potato mixture evenly over the parchment-lined baking sheet. Bake for 40 minutes, or until the potatoes turn a light golden-brown color.||4. Remove from the oven. Using a round cookie cutter, cut the potatoes into individual hash brown circles to serve.</t>
+  </si>
+  <si>
+    <t>Afternoon Tea Pancakes</t>
+  </si>
+  <si>
+    <t>Afternoon Tea Pancakes make the perfect breakfast for your average adventurer</t>
+  </si>
+  <si>
+    <t>2*cups*Flour,0.25*cup*Granulated Sugar,4*teaspoons*Baking Powder,0.25*teaspoon*Baking Soda,0.5*teaspoon*Salt,1.75*cups*Whole Milk,4*tablespoons*Unsalted Butter (melted),2*teaspoons*Pure Vanilla Extract,1*null*Egg,1*dash*Honey,1*bunch*Golden Coloured Berries</t>
+  </si>
+  <si>
+    <t>1. In a large mixing bowl, combine the flour, sugar, baking powder, baking soda, and salt. Mix thoroughly, using a wire whisk.||2. Make a well in the center of your dry ingredients and add the milk, butter, vanilla, and egg. Whisk the wet ingredients together in the well first before slowly folding them into the dry ingredients. Combine until smooth.||3. Heat a nonstick pan over medium-low heat and add a small dollop of butter to lightly grease the pan.||4. Using a ladle, pour about a quarter cup of batter onto the pan and gently spread with the back of the ladle to create a round shape.||5. Cook until bubbles begin to appear on the surface of the pancake and the underside is golden, about 4 minutes. Then flip with a spatula and cook until the other side is golden. Repeat with the remaining batter.||6. Drizzle with honey or maple syrup and decorate with a golden-colored berry on top, if you wish.</t>
+  </si>
+  <si>
+    <t>Jade Dumplings</t>
+  </si>
+  <si>
+    <t>Pork Dumplings</t>
+  </si>
+  <si>
+    <t>1*teaspoon*Salt,1*pound*Ground Pork,1*null*Egg (beaten),13*null*Green Onions,1*tablespoon*Ginger (fresh and minced),2*cloves*Garlic (minced),2*tablespoons*Soy Sauce,1*tablespoon*Sesame Oil,0.25*teapoon*Black pepper,1*tablespoon*Paprika,10*large*Cabbage Leaves (root ends trimmed),2*cups*Pork Bone Broth,1*null*Red Chili Pepper (sliced)</t>
+  </si>
+  <si>
+    <t>1. Fill a large saucepan a third full with water, add a pinch of salt, and bring to a boil over high heat.||2. While the water is coming to a boil, in a large mixing bowl, combine the ground pork, beaten egg, 3 chopped green onions, ginger, garlic, soy sauce, 1 tablespoon toasted sesame oil, crushed red pepper flakes, half a teaspoon salt, pepper, and paprika. Mix to combine thoroughly, then set aside.||3. Place the cabbage leaves and 10 whole green onions in the boiling water for 3 minutes to soften them. Meanwhile, line a baking sheet with paper towels. Transfer the softened leaves and onions to the baking sheet and let cool.||4. Use the paper towels to pat off any excess water. Then spread out a cabbage leaf and place about 1 ½ tablespoons of the pork mixture in the middle of the leaf. Gather the leaf edges together and gently tie with a softened green onion. Repeat until all the cabbage leaves are filled with pork and tied shut.||5. In a pot that can hold a steamer basket, combine the 2 cups broth, the remaining 1 teaspoon sesame oil, and the chili slices. Set the steamer basket on top of the pot. (The pot should be filled to just below your basket so that the broth doesn’t touch the dumplings.)||6. Place the dumplings in the steamer basket and bring the broth to a boil. Then cover with the pot lid and let steam until the pork is cooked through, about 15 minutes. To test, cut a dumpling open and make sure the pork has browned so no pink coloring remains.||7. Using tongs, carefully transfer the dumplings to a serving plate. Pour the chili broth you used for the steaming over the dumplings until they’re sitting in a thin layer of the broth, then serve.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cherry Blossom Tempura </t>
+  </si>
+  <si>
+    <t>The subtle floral flavor of cherry blossoms will serve to elevate this classic tempura dish.</t>
+  </si>
+  <si>
+    <t>1*purple*Eggplant (sliced in rounds),10*null*Okra Pods,10*null*Raw Shrimp (peeled and tails on),4*null*Cauliflower Florets,2*null*Button Mushrooms (sliced),1*cup*Cherry Blossom Petals,4*cups*Vegetable Oil,1*cup*Flour,1*cup*Ice Water,1*null*Egg,1*teaspoon*Salt,1*splash*Soy Sauce,1*dash*Wasabi</t>
+  </si>
+  <si>
+    <t>1. Pat all the vegetables and shrimp dry with a paper towel and set aside.||2. Add the oil to a deep fryer or a medium pot on the stovetop and heat to 320 degrees F. (Use a thermometer to check the temperature, or dip the tip of a wooden or bamboo chopstick in the oil. If small bubbles appear around the chopstick, the oil is ready.)||3. While the oil is heating, prepare the tempura batter. Place the all-purpose flour in a large bowl. In a smaller bowl, whisk together the ice water and egg until fully combined. Scoop up and discard any surface foam.||4. Slowly pour the egg mixture into the flour while mixing with chopsticks or a wire whisk. Once all the egg mixture is in, continue whisking gently for about 15 seconds. Be careful not to overmix; it’s okay to leave some lumps in your batter. It’s important to keep the tempura batter cold, so set your bowl of batter inside a larger bowl filled with about 1 inch of ice water.||5. When the oil reaches the right temperature, start by dipping an eggplant slice in the cold batter, letting any excess batter drip off for a few seconds before very gently placing the eggplant in the hot oil. Repeat this with each individual ingredient you’re going to deep fry, but make sure you don’t overcrowd the deep fryer or cooking pot. The ingredients should take up only half of the surface area at any time. (Having too many ingredients in the pot at once will cause the oil temperature to drop.)||6. Deep-fry the vegetables and shrimp for 1 to 2 minutes each and the sakura petals or nettle leaves for 15 to 20 seconds, or until golden. Continue frying in batches until all the ingredients have been cooked, transferring each batch to a baking sheet or plate lined with paper towels to absorb excess oil. Between batches, skim any leftover tempura crumbs from the top of the oil so they don’t burn and change the flavor of the oil.||7. Serve the tempura immediately with wasabi and/or soy sauce for dipping.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cold Soba Noodles </t>
+  </si>
+  <si>
+    <t>The subtle buckwheat flavor of the noodles dunked in a cold soy sauce dip will refresh you in no time and get you ready to travel on to your next quest.</t>
+  </si>
+  <si>
+    <t>1*package*Soba Noodles,2*tablespoons*Sesame Oil,1*null*Nori Sheet (cut into thin strips)1*sprinkle*Pepper,1*splash*Soy Sauce</t>
+  </si>
+  <si>
+    <t>1. Over high heat, bring a medium pot of water to boil. Add the soba noodles and cook until they are chewy but still a little firm, about 4 to 5 minutes.||2. While the noodles are cooking, fill a large bowl with ice water.||3. Once the noodles are done cooking, strain them and place in the prepared ice water. Chill until the noodles are cold, about 3 minutes. Then strain again and toss with the sesame oil.||4. Place equal portions of noodles on serving plates and sprinkle with nori strips and a bit of pepper. Serve with soy sauce for dipping.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pork Cutlet Sandwich </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pork Cutlet Sandwich, with its fluffy bread surrounding the crispiest pork cutlet, is the perfect lunch to munch on as you traverse snowy mountains or arid deserts.</t>
+  </si>
+  <si>
+    <t>12*ounce*Boneless Pork Loin (fat trimmed),0.3*cup*Shio Koji Seasoning,2.5*teaspoons*Salt,1*cup*Water,0.5*head*Green Cabbage (core removed and thinly sliced),2*null*Lemons,2*null*Eggs,1*cup*Flour,2*cups*Panko Bread Crumbs,6*cups*Vegetable Oil,2*tablespoons*Japanese Kewpie Mayonnaise,1*splash*Tonkatsu Sauce,8*sliced*Japanaese Milk Bread</t>
+  </si>
+  <si>
+    <t>1. To prepare the pork cutlets, slice the pork loin into 4 equal pieces. Place each slice in a sealed plastic bag with all the air removed or between 2 sheets of plastic wrap. Using a meat tenderizer, gently pound each slice until it is about 6 inches wide and half aninch thick.||2. In a medium bowl, combine the shio koji, 2 teaspoons salt, and 1 cup water; stir well until the salt is fully dissolved. Add the pork pieces, then cover and chill in the refrigerator for 8 hours or overnight.||3. Just before the pork is done chilling, place the cabbage in a medium bowl. Zest both lemons over the cabbage and then add the juice from the lemons. Season with a half teaspoon salt and toss with your hands until the cabbage is fully coated and slightly wilted. Cover and chill until ready to use.||4. After the pork has chilled, remove it from the refrigerator, drain, and set aside. Line a rimmed baking sheet with paper towels, set a wire rack on top, and place near the stovetop.||5. In a shallow dish, whisk together the eggs and 2 tablespoons water. Place the flour and the bread crumbs in 2 more shallow dishes. Working with a single pork cutlet at a time, first coat it in the flour, shaking off any excess. Then dip it in the eggs and finally in the bread crumbs, pressing firmly into the crumbs on both sides to make sure they stick. Transfer to another rimmed baking sheet or a platter.||6. Pour oil into a medium-deep pot so that it comes about 2 inches up the side. Heat over medium-high heat until an instant-read thermometer reads between 350 degrees F and 365 degrees F. Using chopsticks or tongs, lower a cutlet vertically into the pan, letting it slide away into the oil until it lies flat. Use the chopsticks or tongs to keep the pork fully submerged in the oil until the underside is golden brown, about 1 minute. Gently flip and cook the other side until it is also golden brown, about 1 more minute. Then transfer the cutlet to the prepared wire rack over the paper towel–lined baking sheet. Repeat with the remaining pork cutlets.||7. Drizzle tonkatsu sauce over the cutlets and let rest for a few minutes. Then spread Kewpie mayonnaise on half of the bread slices and add a few cabbage leaves. Top with a pork cutlet and a second slice of bread, then cut each sandwich in half.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warming Goulash </t>
+  </si>
+  <si>
+    <t>A medley of hearty vegetables, meat, and spices create a phenomenally flavorful dish</t>
+  </si>
+  <si>
+    <t>3*pounds*Boneless Beef Chuck Roast (cut into 1inch cubes),2*teaspoons*Salt,1*teaspoon*Pepper,2*tablespoons*Vegetable Oil,5*cups*Beef Stock,3*large*Carrots (peeled and chopped),2*cups*Fresh Okra Pods,2*null*Onions (diced),2*stalks*Celery (diced),1*null*Red Bell Pepper (diced),1*null*Yellow Bell Pepper (diced),0.25*null*Paprika,4*cloves*Garlic (minced),1*can*Tomato Sauce,1*null*Roma Tomato (diced),1*tablespoon*Soy Sauce,2*null*Bay Leaves,2*sprigs*Fresh Thyme,3*large*Russet Potatoes (peeled and cubed),2*tablespoons*FLour,0.25*cup*Water,1.5*tablespoons*Apple Cider Vinegar</t>
+  </si>
+  <si>
+    <t>1. Move an oven rack to the lower third of the oven. Preheat the oven to 300 degrees F.||2. In a large bowl, season the beef chunks generously with the 2 teaspoons salt and 1 teaspoon pepper and set aside. Add the oil to a Dutch oven or oven-safe stockpot and heat on the stovetop over medium-high heat. Add the seasoned meat and cook until the beef cubes are browning around the edges, about 10 minutes. Transfer the beef back to the bowl and set aside.||3. Reduce the heat to medium-low. Add the sliced carrots and okra to the Dutch oven or stockpot and season to taste with salt and pepper. Cook for about 4 minutes, then transfer to a bowl and set aside. Add the onion, celery, and bell peppers to the pot and cook, stirring occasionally, until the onion and peppers are soft and starting to brown, about 8 minutes.||4. Add the paprika and minced garlic and cook about 1 more minute, until the garlic is fragrant. Pour in the stock, tomato sauce, diced tomatoes, and soy sauce. Sprinkle on the bay leaves and thyme and stir to combine.||5. Add the beef chunks back into the cooking pot and turn the heat up to medium. Stirring well, bring everything to a simmer.||6. Once the mixture is simmering, transfer the pot to the oven, cover it with a lid set slightly off the top, and cook for 1 hour. Adjust the oven temperature if necessary to maintain a low simmer.||7. Remove the goulash from the oven and add the potatoes and the reserved carrots and okra. Return to the oven with the lid partially covering the pot again. Cook until the broth has thickened and the beef and potatoes are fork tender, about 45 minutes. Remove the lid. Using a ladle, skim any excess fat from the surface and discard.||8. In a small bowl, mix together the 2 tablespoons flour and quarter cup water. Pour over the goulash and stir gently until well combined. Cook in the oven for another 5 minutes.||9. Remove from the oven, stir in the vinegar, and season to taste with salt and pepper, if necessary.||10. Serve in individual bowls and top with fresh parsley or cilantro.</t>
+  </si>
+  <si>
+    <t>Honey Glazed Roast</t>
+  </si>
+  <si>
+    <t>Succulent pork roast covered with a sweet-and-savory glaze and accompanied by perfectly seasoned veggies—a superb meal.</t>
+  </si>
+  <si>
+    <t>1*cup*Soy Sauce,0.25*cup*Light Brown Sugar (packed),2.5*tablespoons*Garlic (minced),1*teaspoon*Onion Powder,1*teaspoon*Paprika,0.5*teaspoon*Dried Oregano,2*null*Scallions (chopped),2*pounds*Boneless Pork Shoulder (skin on),5*medium*Yukon Gold Potatoes (chopped into half inch chunks),2*null*Carrots (peeled and sliced),10*cloves*Garlic,2*tablespoon*Olive Oil,1*sprinkle*Salt,1*sprinkle*Pepper,1*cup*Dark Brown Sugar (packed),0.5*cup*Honey</t>
+  </si>
+  <si>
+    <t>1. In a large bowl, combine the 3 quarters of a cup soy sauce with the light brown sugar, minced garlic, onion powder, paprika, oregano, and chopped scallions.||2. Using a sharp knife, score the fat layer of the pork in diamond shapes.||3. Place the pork in the soy sauce marinade and turn to coat evenly. Cover with plastic wrap and place in the fridge to marinate for 1 hour.||4. Preheat the oven to 275 degrees F. Place the potatoes, carrots, and garlic cloves on a rimmed baking sheet and toss with the 2 tablespoons oil, salt, and pepper. Place the marinated pork on top of the veggies in the middle of the baking sheet. Bake for 1 hour, then remove from the oven.||5. Increase the oven temperature to 500 degrees F. In a small bowl, combine the dark brown sugar, honey, and remaining eiighth of a cup soy sauce, stirring until smooth.||6. Spoon the honey glaze over the top of the pork. Return to the oven and bake for 15 to 20 minutes, until the sugar is caramelized and the top of the pork is crispy.||7. Transfer the pork and vegetables to a serving plate. Spoon the reserved pan juices on top of the pork to serve.</t>
+  </si>
+  <si>
+    <t>Fish and Noodle Stir Fry</t>
+  </si>
+  <si>
+    <t>The springy rice noodles add a balance of texture when paired with pieces of soft, flaky tilapia</t>
+  </si>
+  <si>
+    <t>1*package*Rice Tagliatelle Noodles,3*tablespoons*Olive Oil,0.5*null*Onion (sliced),1*null*Green Bell Pepper (sliced),1*null*Red Bell Pepper (sliced),3*cloves*Garlic (minced),1*teaspoon*Hoisin sauce,2*tablespoons*Soy sauce,1*Tilapia Filet (cut into 1inch pieces),1*sprinkle*Salt,1*sprinkle*Pepper</t>
+  </si>
+  <si>
+    <t>1. Cook the rice noodles according to the package instructions. Drain and set aside.||2. Add the oil to a wok or large frying pan over medium-high heat. Heat for about 2 minutes and then add the onion and bell peppers slices. Sauté for 3 minutes, stirring frequently.||3. Stir in the garlic, hoisin sauce, and soy sauce and cook for 1 minute.||4. Season the tilapia pieces with salt and pepper and add to the pan. Cook for 2 to 3 minutes, stirring frequently so the fish doesn’t burn.||5. Add the rice noodles and toss gently so the noodles are thoroughly coated and mixed with the veggies. Serve immediately!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grilled Steak </t>
+  </si>
+  <si>
+    <t>A simple, juicy steak.</t>
+  </si>
+  <si>
+    <t>1*teaspoon*Salt,0.5*teaspoon*Pepper,1*teaspoon*Dried Thyme,1*teaspoon*Garlic Powder,2*null*Boneless Strip steaks (1.5 inches thick),1*tablespoon*Olive Oil</t>
+  </si>
+  <si>
+    <t>1. Combine the dried seasonings in a small bowl. Rub both sides of each steak with olive oil, then generously season all over with your seasoning mixture.||2. Light two of the grill burners and heat on high for 10 minutes, or until the temperature reaches 500 degrees F. Add the steaks to the lit burners, close the grill lid, and sear for 1 to 2 minutes. Then flip the steaks, close the grill lid again, and sear for 1 more minute.||3. Open the grill lid and move the steaks to the unlit portion of the grill. Continue cooking for 7 more minutes, grill lid closed, until the steaks reach medium-rare doneness.||4. Transfer the steaks to a large plate and let rest for at least 5 minutes. Sprinkle with salt and black pepper, if desired, and serve.</t>
+  </si>
+  <si>
+    <t>Fruit Manju</t>
+  </si>
+  <si>
+    <t>Springtime Mochi</t>
+  </si>
+  <si>
+    <t>Colorful Dango</t>
+  </si>
+  <si>
+    <t>Fragrant Rose Custard</t>
+  </si>
+  <si>
+    <t>Sticky Rice Pudding</t>
+  </si>
+  <si>
+    <t>Crispy Lotus Flowers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fresh fruit encased in a sweet gelatin makes for the perfect bite every time. </t>
+  </si>
+  <si>
+    <t>2*tablespoons*Potato Starch,1*tablespoon*Sugar,0.75*cup*Water,1*null*Banana (sliced)</t>
+  </si>
+  <si>
+    <t>1. In a saucepan over medium-low heat, combine the potato starch, sugar, and 3 quarters of cup water. Using a wire whisk, stir frequently until the liquid becomes a translucent jelly, about 5 minutes.||2. Spoon the warm jelly into a silicone or nonstick mini muffin tin until the cups are about 2 thirds full. Add the sliced banana, then spoon more warm jelly on top. Make sure that no parts of the banana are poking up through the jelly.||3. Refrigerate for 1 hour, then gently pop the manju onto a plate to serve.</t>
+  </si>
+  <si>
+    <t>The color of this Springtime Mochi will remind you of sweet cherry blossoms and make you feel as if you’ve just spent a fine spring morning perched under a sakura tree.</t>
+  </si>
+  <si>
+    <t>6*pickled*Sakura Leaves,1*tablespoon*Rice Flour (glutinous),0.5*cup*Water,6*tablespoons*Flour,1*tablespoons*Sugar,1*packet*Red Food Colouring,4*ounces*Red Bean Paste,1*splash*Oil,1*heap*Sakura Blossoms</t>
+  </si>
+  <si>
+    <t>1. Soak the sakura leaves in a bowl of water for 10 minutes. Pat dry with paper towels and set aside.||2. In a medium bowl, combine the rice flour and a quarter cup + 2 teaspoons water and whisk until well blended. Sift in the all-purpose flour, add sugar, and whisk again until well combined.||3. Add the red food coloring, just enough to make the mixture pink. Begin with 1 drop, mix well, and add another drop if the cooler seems too light.||4. Divide the bean paste into 6 even portions and roll them into half-inch thick logs.||5. Lightly grease a nonstick frying pan with oil and heat over medium-low heat.||6. Using a spoon, gently pour some of the mochi batter into the pan, spreading the mixture with the spoon to form an oval about 5 inches long and 2 inches wide. Cook for 10 to 15 seconds, until the top surface is dry. Immediately flip and cook for 5 to 10 seconds more. Repeat until you have 6 mochi ovals.||7. Roll each mochi oval around a log of red bean paste. Then roll each in a pickled sakura leaf and top each mochi roll with a sakura blossom if you have them. Arrange on a plate to serve.</t>
+  </si>
+  <si>
+    <t>The sweet taste and vibrant colors are the perfect combination, reminding you to savor the easy summer days before the next big adventure begins.</t>
+  </si>
+  <si>
+    <t>0.5*cup*Rice Flour,0.5*cup*Powdered Sugar,1*cup*Rice Flour (sweet and glutinous),1*cup*Soy Milk (cold),2*tablespoons*Milk,2*drops*Red Food Colouring,0.5*teaspoon*Matcha Powder,5*null*Bamboo Skewers</t>
+  </si>
+  <si>
+    <t>1. Soak the bamboo skewers in cold water for at least 30 minutes.||2. In a large bowl, combine the rice flour, powdered sugar, glutinous rice flour, and soy milk. On a flat surface, knead into a smooth dough. Add 1 to 2 tablespoons of milk or water if the dough feels too dry or falls apart.||3. Divide the dough into 3 equal portions. Add 2 drops red food coloring to 1 portion of dough, add the matcha powder to another portion, and leave the third portion white.||4. Knead each piece of dough, making sure the food coloring and matcha powder are evenly distributed. Then divide each portion into 5 equal pieces and roll them into round balls.||5. Bring a medium pot of water to a boil over high heat. Boil the dango balls over medium heat for about 15 minutes, or until they are floating. (You can do this in one batch—the white dango balls won’t be colored by the other balls.)||6. Fill a large bowl with ice water and use a slotted spoon to transfer the cooked dango balls to the bowl. Let them cool in the water until you’re ready to put them onto the skewers.||7. Insert 3 cooled dango balls onto each bamboo skewer in the order of green, white, and pink. Hand them out and enjoy!</t>
+  </si>
+  <si>
+    <t>Sticky Rice Pudding, with its creamy texture and sweet flavor, will give you that extra boost of stamina you may need as you work on becoming the best adventurer you can be.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5*cups*Water,0.75*cup*White Rice (uncooked),2*cups*Whole Milk,0.3*cup*Sugar,0.25*teaspoon*Salt,1*null*Egg (beaten),1*tablespoon*Unsalted Butter,0.5*teaspoon*Pure Vanilla Extract,1*dash*Ground Cinnamon,1*null*Mango (sliced),1*bits*Fresh Mint </t>
+  </si>
+  <si>
+    <t>1. In a medium saucepan over medium heat, bring the water to a boil. Once boiling, stir in the rice and immediately reduce the heat to low. Cover and let simmer until the liquid is absorbed, about 20 minutes.||2. Add 1 and a half cups milk to the saucepan along with the sugar and salt. Turn the heat back up to medium and stir until well combined. Continue stirring occasionally and cook until the rice mixture becomesthick and creamy, about 15 minutes.||3. Add the remaining half a cup milk and the beaten egg and cook for 2 minutes, stirring constantly. Remove from the heat and stir in the butter and vanilla until well combined.||4. Divide the rice pudding into 4 bowls. Sprinkle with cinnamon and top with mango slices and fresh mint. Serve warm.</t>
+  </si>
+  <si>
+    <t>The subtle hints of rose elevate your typical creamy custard</t>
+  </si>
+  <si>
+    <t>3*cups*Whole Milk,6*tablespoons*Sugar,3*tablespoons*Vanilla Custard Powder,2*teaspoons*Rose Water,0.25*cup*Fresh Strawberries (pureed),1*scoop*Pistachios (chooped and peeled),1*bunch*Edible FLowers</t>
+  </si>
+  <si>
+    <t>1. In a heavy-bottom pan over medium-high heat, bring 2 cups of milk to a boil. Add the sugar, reduce the heat to medium-low, and stir until the sugar is dissolved.||2. Mix the custard powder into the remaining 1 cup milk, whisking until there are no lumps. Pour the mixture into the boiled milk and continue mixing over medium heat for 5 to 6 minutes, or until the mixture thickens.||3. Remove from the heat and, using a rubber spatula, gently fold in the strawberry puree and rose water until well combined. Pour into 2 medium bowls and refrigerate for at least 1 hour before serving.||4. Top with chopped pistachios and edible flowers to serve.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genshin </t>
+  </si>
+  <si>
+    <t>A deep-fried dessert  that celebrates the beauty of the lotus flower.</t>
+  </si>
+  <si>
+    <t>1.5*cups*All Purpose Flour,4.33*tablespoons*Unsalted Butter,1*tablespoon*Sugar,15*teaspoons*Water,1*packet*Red Food Colouring,1*splash*Vegetable Oil,0.75*cup*Almond Flour,10*tablespoons*Powdered Sugar,0.5*teaspoon*Almong Extract</t>
+  </si>
+  <si>
+    <t>1. To make the white dough, in a medium bowl, mix 3 quarters of a cup of the flour with 2 and 2 thirds tablespoons of the butter. Knead until smooth and cover with plastic wrap. Set aside for 30 minutes.||2. To make the red dough, mix another 3 quarters of a cup flour with 1 and 2thirds  tablespoons butter. Work in 1 tablespoon sugar and the red water mixture. Mix well and knead until a smooth dough is formed. Cover with plastic wrap and set aside for 30 minutes.||3. Add all the marzipan ingredients to a medium bowl and mix until well combined.||4. Divide the white dough, the red dough, and the marzipan each into 9 equal-size balls.||5. Using a rolling pin, flatten the red balls into circles. Wrap a white dough ball with a red dough circle, covering it entirely. Repeat with each red dough circle and white dough ball.||6. Squash down each red/white dough ball and use a rolling pin to flatten it into an oval. Roll up into a ball once again and cover with plastic wrap for 15 minutes.||7. Repeat Step 6, flattening the rolled dough into ovals, rolling them back into balls, then letting them rest for 15 minutes, covered with plastic wrap.||8. After the dough has rested, remove the plastic wrap and use your thumb to press each piece of dough into a bowl shape, letting the edges tilt up and onward the middle. Place a marzipan ball in the middle of each dough bowl, then wrap the dough edges around it to seal in the marzipan and form a ball.||9. Place the sealed side of the ball face down, then cut a star shape in the top surface of the ball, cutting only deep enough so you can just see the marzipan filling.||10. Fill a deep saucepan or fryer halfway with vegetable oil and heat to 300 degrees F. Place a lotus ball in a mesh strainer and lower it into the oil to fry. Cook 1 or 2 lotus balls at a time. Use a ladle to pour hot oil onto the balls, letting it bloom and create some layers. Each ball needs to cook around 3 to 4 minutes in the hot oil.||11. Place the cooked lotus flower crisps on a paper towel-lined plate to drain the oil. Allow to cool fully and then enjoy!</t>
   </si>
 </sst>
 </file>
@@ -1905,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4427,6 +4697,512 @@
         <v>12</v>
       </c>
     </row>
+    <row r="110" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="F110" s="12">
+        <v>30</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="F111" s="12">
+        <v>30</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E112" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="F112" s="12">
+        <v>40</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="F113" s="12">
+        <v>10</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="E114" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="F114" s="12">
+        <v>20</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E115" s="10" t="s">
+        <v>496</v>
+      </c>
+      <c r="F115" s="12">
+        <v>105</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="E116" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="F116" s="12">
+        <v>50</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E117" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="F117" s="12">
+        <v>25</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="F118" s="12">
+        <v>45</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="F119" s="12">
+        <v>70</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="F120" s="12">
+        <v>15</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="F121" s="12">
+        <v>30</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="E122" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="F122" s="12">
+        <v>160</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="F123" s="12">
+        <v>150</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>532</v>
+      </c>
+      <c r="F124" s="12">
+        <v>25</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="F125" s="12">
+        <v>30</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="F126" s="12">
+        <v>70</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="F127" s="12">
+        <v>20</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="F128" s="12">
+        <v>50</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="F129" s="12">
+        <v>75</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="F130" s="12">
+        <v>50</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="F131" s="12">
+        <v>30</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the new series
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkish\Downloads\Realm-of-Feasts\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\Downloads\COSC345\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FADF47-F3C9-49E6-B80A-BE6174A05E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90DEA801-EA36-41FF-9430-B1ADED03A9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
   <sheets>
     <sheet name="RecipesTest" sheetId="1" r:id="rId1"/>
@@ -908,9 +908,6 @@
     <t>1*null*Sea Bream Head,1*sheet*Kombu,2*null*turnips,6*null*Asparagus (pencil spears),0.5*null*Lemon,5*cups*Water,2*teaspoons*Salt,1*dash*Soy Sauce</t>
   </si>
   <si>
-    <t>1. Soak the kombu in water for at least 30 minutes. Slice the sea bream head into pieces if necessary and place it in a separate pot of boiling water deep enough to cover the fish head. When the surface becomes white, remove and place in another bowl of cold water, then scrub clean to remove blood and stains ©.||2. Cut turnips into wedges and slice greens finely. Peel the bottom third of asparagus and slice into 2inch (5 cm) pieces. Slice lemon into wheels.|| 3. Pour water from step 1 and sea bream into the same pot and bring to a boil. Skim the scum off the top and lower heat to medium, Add turnip wedges(D) and let simmer, skimming regularly.|| 4. After 10 minutes, add asparagus and simmer for 5 minutes. Add salt, and soy sauce to taste. Transfer to bowls, add lemon slices, and scatter turnip greens on top.</t>
-  </si>
-  <si>
     <t>Pirate Box Lunches for Crossing the Desert</t>
   </si>
   <si>
@@ -941,12 +938,6 @@
     <t>1. Boil eggs whole for 12 minutes until hard-boiled. Let cool. Peel off shells and cut them into thick slices. Tear crab meat by hand. Mince onion, then soak in water, remove, and press the liquid out. Put egg, crab, and onion into a bowl, then mix with mayonnaise (A), Spread butter on the bread slices, then divide the mix to make three sandwiches.</t>
   </si>
   <si>
-    <t>1. Trim fat and sinew from the chicken thighs and cut into bite-size pieces—grate garlic. Put the chicken into a bowl, add mix garlic, salt, pepper and sake then marinate for 20-30 minutes.||2. Sprinkle flour over the thighs. Heat vegetable oil in a pan on medium heat, then fry chicken in batches for 4-5 minutes undisturbed on each side.</t>
-  </si>
-  <si>
-    <t>1. Let the beef sit at room temperature for 30 minutes, and grate onion and garlic for sauce. Just before cooking, rub the other garlic half against meat( C), then rub on salt and pepper. Pour oil on a heated frying pan and cook the meat surface on medium heat (D). Cover and heat on low for 6-8 minutes, then turn over and heat for another 4-5 minutes.||2. Remove from pan, wrap in aluminum foil, and let sit for 15 minutes to heat through (E).||3. Add onions, garlic and saké to the meat juice in the frying pan. Once bubbling, mix in soy sauce and butter. Once mixed in, turn off the heat, add vinegar and mix again.||4. Slice meat thinly and transfer to plate, then drizzle sauce from pan, Add mustard or wasabi as desired.</t>
-  </si>
-  <si>
     <t>Luffy's Favorite Meat on the Bone</t>
   </si>
   <si>
@@ -956,9 +947,6 @@
     <t>4*null*Chicken Drumsticks,4*null*Eggs (hard-boiled),0.25*cup*Breadcrumbs,3*tablespoons*Milk,500*grams*Chicken,1*teaspoon*Salt,1*dash*Black Pepper,1*null*Egg,1*spalsh*Vegetable Oil</t>
   </si>
   <si>
-    <t>1. Make chicken drumstick “tulips.” Use kitchen scissors to cut the meat loose from the handle end of the drumstick (A). Roll the meat down the bone until it is fully inside-out at the end.||2. Soak the breadcrumbs in milk. Knead ground chicken, salt, pepper and egg in a bowl, then add breadcrumbs and knead again.||3.  Fold the meaty end of the drumstick around a hard-boiled egg (B). If the meat doesn't cover well enough, add cuts to loosen it up. Oil hands lightly and cover drumstick and egg with the breadcrumb mixture from the previous step.||4. Bake at 400 degrees Fahrenheit  (200 degrees Celsius) for 15-20 minutes, watching carefully</t>
-  </si>
-  <si>
     <t>Yagara Bull's Favourite Steamed Water-Water Meat</t>
   </si>
   <si>
@@ -1064,9 +1052,6 @@
     <t xml:space="preserve">3*fillets*Salmon,1*dash*Salt,1*dash*White Pepper,0.25*head*Cabbage,0.5*null*Onion,0.5*null*Carrot,1*splash*Vegetable Oil,1*tablespoon*Sake,1.5*tablespoon*Sugar,3*tablespoons*Miso,1.5*tablespoon*Butter,0.5*tablespoon*Soy Sauce </t>
   </si>
   <si>
-    <t>1. Lightly sprinkle salt and white pepper on the salmon. Roughly cut the cabbage, slice the onion into 4-inch (1 cm) pieces, and cut the carrot into short strips.||2.  Pour oil onto a heated frying pan and cook salmon, skin side down, on medium heat for 2-3 minutes, until browned.||3. Turn over the salmon, then add cabbage, onion, and carrot. Swirl in saké, Sprinkle sugar and miso here and there and add dabs of butter on top of the miso clumps (A). Carefully cover with aluminum foil and steam for 6-7 minutes (B).||4. Remove foil, tear salmon into chunks, and mix contents. Add soy sauce and turn off heat.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sliced Octopus </t>
   </si>
   <si>
@@ -1112,10 +1097,6 @@
     <t>6*null*Shiitake Mushrooms,1*pack*Shimeji Mushrooms,2*null*King Oyster Mushrooms,3*pieces*Bacon,1*tablespoon*Vegetable Oil,2*sprigs*Rosemary,1*teaspoon*Salt,1*sprinkle*Black Pepper,1*pat*Butter</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Remove the shiitake mushrooms from their base and cut them into half-inch (1 cm) slices. Remove the shimeji mushrooms from their base and separate them into small bunches. Trim king oyster mushrooms to a length of 1 and a half inches (3cm) and slice thinly. Cut bacon into quarter-inch (7 mm) slices.||2. Put vegetable oil and rosemary into a frying pan and heat on medium. When oil is fragrant, fry bacon briefly, then add all mushrooms and mix. Cover and steam on low heat for 4 minutes.||3. Remove the lid, add salt, and mix again. Cover again and continue steaming for 4-5 minutes, stirring occasionally, until the liquid is gone and the bacon is fried and no longer appears pink. If needed, add more salt and pepper for flavour, then add butter, mix, and turn off heat.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stir-fried Bean Sprouts </t>
   </si>
   <si>
@@ -1137,10 +1118,6 @@
     <t>3*null*Potatoes (peeled),60*grams*Shredded Cheese,1*splash*Vegetable Oil,1*sprinkle*Salt</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Place finely cut shoestring potatoes using a mandoline at a one-third-inch setting if available, and mix with cheese.||2. Pour a generous amount (around a quarter cup) of oil into a frying pan. Pack a quarter of the potatoes tightly and fry on low heat for 7-8 minutes. Turn over and fry another 7-8 minutes, until both sides are crispy. Be careful not to prod too much while frying, as it will come apart. Once cooked, dab dry with paper towels, then sprinkle with salt.||3. Repeat for the other three portions.
-</t>
-  </si>
-  <si>
     <t>Neptunian Penne Gorgonzola</t>
   </si>
   <si>
@@ -1213,10 +1190,6 @@
     <t>2*large*Eggs,1*tablespoon*Parmesan Chees (grated),1*gram*Salt,1*gram*White Pepper</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1. Preheat the oven to 450 degrees F (230 degrees C). Prep a baking sheet with parchment paper.||2. Separate the eggs, placing the whites in a large bowl. Set aside the yolks, keeping them intact.||3. Beat the egg whites until stiff peaks form.||4. Fold in the Parmesan cheese, salt, and white pepper.||5. Spoon the whipped whites into two separate mounds and place them onto the prepped baking sheet.||6. With the back of a spoon, create an indentation in the center of each mound.||7. Bake for 2 minutes. Gently pour the egg yolks into the indentations. Return to the oven and cook for another 3 minutes. Serve immediately.</t>
-  </si>
-  <si>
     <t>Sigh... Pancakes, I guess</t>
   </si>
   <si>
@@ -1238,9 +1211,6 @@
     <t>2*slices*Bacon,1*teaspoon*Light Brown Sugar (packed),2*large*Eggs,1*tablespoon*Unsalted Butter,0.25*teaspoon*Salt,1*gram*Pepper</t>
   </si>
   <si>
-    <t>1. In a nonstick skillet over medium heat, place the bacon and sprinkle the brown sugar on top. Cook until just crisp, about 6 to 8 minutes. Remove from the pan and set aside.||2. Break the eggs that can’t be beat into individual bowls.||3. In the same skillet over medium heat, melt the butter, then slide the eggs into the pan.||4. When the edges start to turn white, cover the pan and lower the heat. Cook 4 to 5 minutes, until the whites firm up. Season with salt and pepper.||5. Lay the bacon blankets over the eggs to serve.</t>
-  </si>
-  <si>
     <t xml:space="preserve">BLTExhausted </t>
   </si>
   <si>
@@ -1250,10 +1220,6 @@
     <t>2*tablespoons*Mayonnaise,1*teaspoon*Pesto,4*slices*Bacon (thick),2*slices* Sourdough Bread,2*slices*Tomato,1*gram*Pepper,3*leaves*Butter Lettuce</t>
   </si>
   <si>
-    <t xml:space="preserve">1. In a small bowl, stir together the mayonnaise and pesto. Set aside.||2. In a skillet over medium-high heat, cook the bacon for 5 to 6 minutes, until crispy. Drain on paper towels.||3. Lightly toast the bread.||4. Spread the mayonnaise mixture onto both sides of the toast. On one slice, layer the bacon, then the tomato.||5. Season with pepper.||6. Place the lettuce on top, then the remaining slice of toast.||7. Slice in half to serve.
-</t>
-  </si>
-  <si>
     <t>Slowly Grilled Cheese</t>
   </si>
   <si>
@@ -1275,9 +1241,6 @@
     <t>A Gudetama Deviled Eggs</t>
   </si>
   <si>
-    <t>1. Place the eggs in a pot and cover with 1 to 2 inches (2.5–5 cm) of water. Turn on the heat to medium-high and bring to a boil.||2. Turn off the heat, cover with a lid, and let sit for 10 to 12 minutes.||3. Place the eggs in an ice bath and let cool completely.||4. Peel and slice the eggs in half. Set aside the whites and place the yolks into a bowl.||5. Stir together the egg yolks, mayonnaise, mustard, onion powder, salt, and pepper.||6. Place the mixture into a piping bag and pipe the filling into the egg white centers.||7. Place an olive half on top of each egg to serve.</t>
-  </si>
-  <si>
     <t>Napping in an Avocado</t>
   </si>
   <si>
@@ -1338,12 +1301,6 @@
     <t>Who Cares about Salmon</t>
   </si>
   <si>
-    <t>1. In a bowl, stir together the graham cracker crumbs, butter, brown sugar, cinnamon, and salt.||2. Press into a 9-inch (23-cm) pie plate, and freeze for 1 hour.||3. Pour in the softened ice cream and spread evenly with a spatula. Place the pie back in the freezer for 4 to 6 hours.||4. In a large bowl, whip together the cream and confectioners’ sugar just until stiff peaks form. Spread onto the pie. Top with fresh strawberries to serve.</t>
-  </si>
-  <si>
-    <t>1. To make the glaze: In a dry skillet over medium-high heat, toast the sesame seeds for 2 to 3 minutes, until fragrant. Use a mortar and pestle or a spice grinder, until it becomes powderlike.||2. In a small bowl, stir together the confectioners’ sugar, the black sesame seed powder, milk, and vanilla. Set aside.||3. To make the doughnuts: Place the biscuits on a cutting board and use a 1-inch (2.5-cm) round cutter to cut holes from the middle of each biscuit.||4. In a Dutch oven, heat the oil to 350 degrees F (177 degrees C). Fry the doughnuts and holes for 1 to 2 minutes on each side, until golden brown. Transfer to a wire rack and let cool.||4. Dip the doughnuts in the glaze and place them back onto the wire rack to let the excess glaze drip off.||5. Once the glaze has set after about 20 minutes, the doughnuts are ready to serve.</t>
-  </si>
-  <si>
     <t>1. To make the cereal mix: Preheat the oven to 250 degrees F (130 degrees C).||2. In an extra-large bowl, toss together the rice and corn cereal, corn chips, pretzels, cheese crackers, and macadamia nuts. Set aside.||3. To make the sauce: In a saucepan over low heat, stir together the butter, Worcestershire sauce, brown sugar, seasoned salt, garlic powder, chili powder, and onion powder. Cook 4 to 6 minutes until melted, stirring constantly.||4. To assemble: Pour the sauce over the cereal mixture and toss to coat.||5. Spread the mixture onto a baking sheet, lined with a silicone baking mat or parchment paper.||6. Bake for 1 hour, making sure to stir every 15 minutes.||7. Remove from the oven and let cool completely.||8. Scoop into an airtight container.</t>
   </si>
   <si>
@@ -1455,9 +1412,6 @@
     <t>1. To make the simple syrup: Combine 1 cup (230 ml) water and the sugars in a small saucepan. Bring to a boil and simmer for 2 minutes, just until the sugar is dissolved. Let cool.||2. To make the boba: In a large saucepan, bring 5 cups (1,180 ml) water to a boil.||3. Add in the boba pearls. When they start to float, turn the heat to low and let them simmer for 25 minutes.||4. Turn off the heat and cover the saucepan. Let sit for 25 minutes.||5. Drain and rinse the boba.||6. In a small bowl, add the cooked boba to the simple syrup and let soak for 30 minutes.||7. Strain the boba and pour it into a tall class.||8. To make the milk tea: Pour the boba over the tea, and then add the milk to serve.</t>
   </si>
   <si>
-    <t>1. To make the cupcakes: Preheat the oven to 350 degrees F (177 degrees C). Prep a cupcake pan with paper liners.||2. In a medium bowl, whisk together the cake flour, baking powder, and salt.||3. In the bowl of an electric mixer, cream the butter and sugar until fluffy.||4. Add the eggs and vanilla, stirring until just combined. Stir in the flour mixture, alternating with buttermilk. Spoon the batter into the prepped cupcake pan.||5. Bake for 16 to 17 minutes, or until a toothpick inserted in the center comes out clean.||6. Let cool on a wire rack.||7. To make the frosting: In a large bowl with a handheld mixer on low, cream the butter while slowly adding the confectioners’ sugar. Stir in the heavy whipping cream, vanilla, and salt.Add food coloring and stir, until the frosting becomes a light pink color.||8. Turn the mixer up to medium-high and whip for 10 to 15 seconds, until light and fluffy.||9. To assemble: Pipe the frosting onto the cupcakes to serve.</t>
-  </si>
-  <si>
     <t>Grilled Chicken Skewers</t>
   </si>
   <si>
@@ -1470,9 +1424,6 @@
     <t>1*tablespoon*Dried Oregano,1*tablespoon*Dijon Mustard,0.5*teaspoon*Dried Thyme,1*null*Lemon Juice,3*cloves*Garlic (minced),2*tablespoons*Olive Oil,1*tablespoon*Smoked Paprika,0.25*cup*Soy Sauce,1*tablespoon*Maple Syrup,3*tablespoons*Orange Juice,0.25*cup*Chicken Stock,0.5*teaspoon*Pepper,2*null*Chicken Breasts (boneless and skinless),1*pound*Cremini Mushrooms (whole)</t>
   </si>
   <si>
-    <t>1.. In a large bowl, mix together all the ingredients except the chicken and mushrooms to create a marinade.||2. Cut the chicken breasts into bite-size pieces. Place the chicken and mushrooms in the bowl of marinade and stir until thoroughly coated. Cover and refrigerate for 4 to 10 hours, stirring occasionally.||3. If you’re using bamboo skewers, soak them in water for a few minutes right before the chicken and mushrooms are done marinating to keep them from burning when it comes time to cook. Then pat dry.||4. Thread the chicken and mushrooms on the skewers, discarding any remaining marinade. Grill on high heat until cooked, 5 to 7 minutes, or bake in the oven at 430 degrees F for 8 to 10 minutes. Enjoy!</t>
-  </si>
-  <si>
     <t>Fried Radish on a Stick</t>
   </si>
   <si>
@@ -1518,9 +1469,6 @@
     <t>8*null*Eggs,2.5*tablepoons*Water,1*tablespoon*Soy Sauce,0.75*teaspoon*Sugar,1*tablespoon*Olive Oil</t>
   </si>
   <si>
-    <t>1. In a medium bowl, combine the eggs, water, soy sauce, and sugar. Using a whisk, beat until well combined.||2. Heat a tamagoyaki pan (rectangular Japanese omelet pan) or a small frying pan over medium heat. Using a pastry brush, lightly coat the bottom of the pan with olive oil.||3. Pour a thin layer of the egg mixture to cover the surface of the pan. When it’s about 80 percent cooked but still wet on the surface, use chopsticks or wooden tongs to start gently rolling in the edges to form a rolled omelet. Move the rolled omelet to one side of the pan.||4. Brush the pan with oil again and pour in another thin layer of the egg mixture. Using a spoon, gently lift the previously made omelet and spread some of the uncooked egg mixture underneath. This willhelp both omelets stick together. When this next layer of eggs is 80 percent cooked but the surface is still wet, start with the previously made omelet and gently roll it up with the new layer. Set to one side of the pan. Repeat this process until the egg mixture is gone. Your omelet will have 3 to 4 layers.||5. Transfer the rolled omelet onto a cutting board and allow to rest for several minutes. Cut into even 2-inch slices and serve.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Loaded Baked Potato </t>
   </si>
   <si>
@@ -1530,18 +1478,12 @@
     <t>3*large*Baking Potatoes,1*teaspoon*Olive Oil,4*tablespoons*Unsalted Butter (cut into cubes),0.5*cup*Green Onions (chopped),5*null*Cremini Mushrooms (chopped),0.5*cup*Half and Half,0.5*cup*Sour Cream,1*sprinkle*Salt,1*spinkle*Pepper,1*cup*Cheddar Cheesew (shredded)</t>
   </si>
   <si>
-    <t>1. Preheat the oven to 400 degrees F. Pierce the potatoes several times with a fork and rub with olive oil. Bake until tender, 50 to 75 minutes. While baking, you can check if the potatoes are done by sticking a skewer or a fork into them; if soft, they are ready.||2. Remove the potatoes from the oven. When cool enough to handle, slice the top off each potato horizontally (about 1 inch). Scoop out the potato pulp and transfer it to a large mixing bowl, leaving thin potato shells. Set the potato skins aside and reduce the oven temperature to 375 degrees F.||3. In a small skillet, melt the butter over medium-high heat, then add the onions and mushrooms and sauté until tender, about 5 minutes.||4. In the mixing bowl, using a potato masher, mash the potato pulp. Stir in the sauteed onions and mushrooms, half-and-half, sour cream, salt, and pepper. Stuff this mixture into the 3 potato shells and top with cheddar cheese.||5. Place the stuffed potatoes on a baking sheet and bake until heated through, about 20 minutes. Top with extra chopped green onions to serve.</t>
-  </si>
-  <si>
     <t>Crispy Baked HashBrowns</t>
   </si>
   <si>
     <t>Crispy Baked Hash Browns</t>
   </si>
   <si>
-    <t>1*package*Hashbrown Potatoes (frozen,shredded and thawed),2*null*Eggs,1*cup*Cheddar Cheese (shredded),1*pinch*Salt,1*pinch*Pepper,1*teaspoon*Ground Cumin,1*teaspoon*Dried Mint,0.5*teaspoon*Garlic Powder,0.5*teaspoon*Onion Powder,0.5*cup*Unsalted Butter (melted)</t>
-  </si>
-  <si>
     <t>1. Preheat the oven to 400 degrees F. Line a baking sheet with parchment paper and set aside.||2. Pour the shredded potatoes into a large bowl. In a small separate bowl, whisk the eggs. Add the eggs to the potatoes along with the shredded cheese and all the seasonings. Toss to coat everything evenly. Pour the melted butter over the top and toss once again to coat.||3. Spread the potato mixture evenly over the parchment-lined baking sheet. Bake for 40 minutes, or until the potatoes turn a light golden-brown color.||4. Remove from the oven. Using a round cookie cutter, cut the potatoes into individual hash brown circles to serve.</t>
   </si>
   <si>
@@ -1566,9 +1508,6 @@
     <t>1*teaspoon*Salt,1*pound*Ground Pork,1*null*Egg (beaten),13*null*Green Onions,1*tablespoon*Ginger (fresh and minced),2*cloves*Garlic (minced),2*tablespoons*Soy Sauce,1*tablespoon*Sesame Oil,0.25*teapoon*Black pepper,1*tablespoon*Paprika,10*large*Cabbage Leaves (root ends trimmed),2*cups*Pork Bone Broth,1*null*Red Chili Pepper (sliced)</t>
   </si>
   <si>
-    <t>1. Fill a large saucepan a third full with water, add a pinch of salt, and bring to a boil over high heat.||2. While the water is coming to a boil, in a large mixing bowl, combine the ground pork, beaten egg, 3 chopped green onions, ginger, garlic, soy sauce, 1 tablespoon toasted sesame oil, crushed red pepper flakes, half a teaspoon salt, pepper, and paprika. Mix to combine thoroughly, then set aside.||3. Place the cabbage leaves and 10 whole green onions in the boiling water for 3 minutes to soften them. Meanwhile, line a baking sheet with paper towels. Transfer the softened leaves and onions to the baking sheet and let cool.||4. Use the paper towels to pat off any excess water. Then spread out a cabbage leaf and place about 1 ½ tablespoons of the pork mixture in the middle of the leaf. Gather the leaf edges together and gently tie with a softened green onion. Repeat until all the cabbage leaves are filled with pork and tied shut.||5. In a pot that can hold a steamer basket, combine the 2 cups broth, the remaining 1 teaspoon sesame oil, and the chili slices. Set the steamer basket on top of the pot. (The pot should be filled to just below your basket so that the broth doesn’t touch the dumplings.)||6. Place the dumplings in the steamer basket and bring the broth to a boil. Then cover with the pot lid and let steam until the pork is cooked through, about 15 minutes. To test, cut a dumpling open and make sure the pork has browned so no pink coloring remains.||7. Using tongs, carefully transfer the dumplings to a serving plate. Pour the chili broth you used for the steaming over the dumplings until they’re sitting in a thin layer of the broth, then serve.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cherry Blossom Tempura </t>
   </si>
   <si>
@@ -1578,9 +1517,6 @@
     <t>1*purple*Eggplant (sliced in rounds),10*null*Okra Pods,10*null*Raw Shrimp (peeled and tails on),4*null*Cauliflower Florets,2*null*Button Mushrooms (sliced),1*cup*Cherry Blossom Petals,4*cups*Vegetable Oil,1*cup*Flour,1*cup*Ice Water,1*null*Egg,1*teaspoon*Salt,1*splash*Soy Sauce,1*dash*Wasabi</t>
   </si>
   <si>
-    <t>1. Pat all the vegetables and shrimp dry with a paper towel and set aside.||2. Add the oil to a deep fryer or a medium pot on the stovetop and heat to 320 degrees F. (Use a thermometer to check the temperature, or dip the tip of a wooden or bamboo chopstick in the oil. If small bubbles appear around the chopstick, the oil is ready.)||3. While the oil is heating, prepare the tempura batter. Place the all-purpose flour in a large bowl. In a smaller bowl, whisk together the ice water and egg until fully combined. Scoop up and discard any surface foam.||4. Slowly pour the egg mixture into the flour while mixing with chopsticks or a wire whisk. Once all the egg mixture is in, continue whisking gently for about 15 seconds. Be careful not to overmix; it’s okay to leave some lumps in your batter. It’s important to keep the tempura batter cold, so set your bowl of batter inside a larger bowl filled with about 1 inch of ice water.||5. When the oil reaches the right temperature, start by dipping an eggplant slice in the cold batter, letting any excess batter drip off for a few seconds before very gently placing the eggplant in the hot oil. Repeat this with each individual ingredient you’re going to deep fry, but make sure you don’t overcrowd the deep fryer or cooking pot. The ingredients should take up only half of the surface area at any time. (Having too many ingredients in the pot at once will cause the oil temperature to drop.)||6. Deep-fry the vegetables and shrimp for 1 to 2 minutes each and the sakura petals or nettle leaves for 15 to 20 seconds, or until golden. Continue frying in batches until all the ingredients have been cooked, transferring each batch to a baking sheet or plate lined with paper towels to absorb excess oil. Between batches, skim any leftover tempura crumbs from the top of the oil so they don’t burn and change the flavor of the oil.||7. Serve the tempura immediately with wasabi and/or soy sauce for dipping.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cold Soba Noodles </t>
   </si>
   <si>
@@ -1602,9 +1538,6 @@
     <t>12*ounce*Boneless Pork Loin (fat trimmed),0.3*cup*Shio Koji Seasoning,2.5*teaspoons*Salt,1*cup*Water,0.5*head*Green Cabbage (core removed and thinly sliced),2*null*Lemons,2*null*Eggs,1*cup*Flour,2*cups*Panko Bread Crumbs,6*cups*Vegetable Oil,2*tablespoons*Japanese Kewpie Mayonnaise,1*splash*Tonkatsu Sauce,8*sliced*Japanaese Milk Bread</t>
   </si>
   <si>
-    <t>1. To prepare the pork cutlets, slice the pork loin into 4 equal pieces. Place each slice in a sealed plastic bag with all the air removed or between 2 sheets of plastic wrap. Using a meat tenderizer, gently pound each slice until it is about 6 inches wide and half aninch thick.||2. In a medium bowl, combine the shio koji, 2 teaspoons salt, and 1 cup water; stir well until the salt is fully dissolved. Add the pork pieces, then cover and chill in the refrigerator for 8 hours or overnight.||3. Just before the pork is done chilling, place the cabbage in a medium bowl. Zest both lemons over the cabbage and then add the juice from the lemons. Season with a half teaspoon salt and toss with your hands until the cabbage is fully coated and slightly wilted. Cover and chill until ready to use.||4. After the pork has chilled, remove it from the refrigerator, drain, and set aside. Line a rimmed baking sheet with paper towels, set a wire rack on top, and place near the stovetop.||5. In a shallow dish, whisk together the eggs and 2 tablespoons water. Place the flour and the bread crumbs in 2 more shallow dishes. Working with a single pork cutlet at a time, first coat it in the flour, shaking off any excess. Then dip it in the eggs and finally in the bread crumbs, pressing firmly into the crumbs on both sides to make sure they stick. Transfer to another rimmed baking sheet or a platter.||6. Pour oil into a medium-deep pot so that it comes about 2 inches up the side. Heat over medium-high heat until an instant-read thermometer reads between 350 degrees F and 365 degrees F. Using chopsticks or tongs, lower a cutlet vertically into the pan, letting it slide away into the oil until it lies flat. Use the chopsticks or tongs to keep the pork fully submerged in the oil until the underside is golden brown, about 1 minute. Gently flip and cook the other side until it is also golden brown, about 1 more minute. Then transfer the cutlet to the prepared wire rack over the paper towel–lined baking sheet. Repeat with the remaining pork cutlets.||7. Drizzle tonkatsu sauce over the cutlets and let rest for a few minutes. Then spread Kewpie mayonnaise on half of the bread slices and add a few cabbage leaves. Top with a pork cutlet and a second slice of bread, then cut each sandwich in half.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Warming Goulash </t>
   </si>
   <si>
@@ -1620,9 +1553,6 @@
     <t>Honey Glazed Roast</t>
   </si>
   <si>
-    <t>Succulent pork roast covered with a sweet-and-savory glaze and accompanied by perfectly seasoned veggies—a superb meal.</t>
-  </si>
-  <si>
     <t>1*cup*Soy Sauce,0.25*cup*Light Brown Sugar (packed),2.5*tablespoons*Garlic (minced),1*teaspoon*Onion Powder,1*teaspoon*Paprika,0.5*teaspoon*Dried Oregano,2*null*Scallions (chopped),2*pounds*Boneless Pork Shoulder (skin on),5*medium*Yukon Gold Potatoes (chopped into half inch chunks),2*null*Carrots (peeled and sliced),10*cloves*Garlic,2*tablespoon*Olive Oil,1*sprinkle*Salt,1*sprinkle*Pepper,1*cup*Dark Brown Sugar (packed),0.5*cup*Honey</t>
   </si>
   <si>
@@ -1635,12 +1565,6 @@
     <t>The springy rice noodles add a balance of texture when paired with pieces of soft, flaky tilapia</t>
   </si>
   <si>
-    <t>1*package*Rice Tagliatelle Noodles,3*tablespoons*Olive Oil,0.5*null*Onion (sliced),1*null*Green Bell Pepper (sliced),1*null*Red Bell Pepper (sliced),3*cloves*Garlic (minced),1*teaspoon*Hoisin sauce,2*tablespoons*Soy sauce,1*Tilapia Filet (cut into 1inch pieces),1*sprinkle*Salt,1*sprinkle*Pepper</t>
-  </si>
-  <si>
-    <t>1. Cook the rice noodles according to the package instructions. Drain and set aside.||2. Add the oil to a wok or large frying pan over medium-high heat. Heat for about 2 minutes and then add the onion and bell peppers slices. Sauté for 3 minutes, stirring frequently.||3. Stir in the garlic, hoisin sauce, and soy sauce and cook for 1 minute.||4. Season the tilapia pieces with salt and pepper and add to the pan. Cook for 2 to 3 minutes, stirring frequently so the fish doesn’t burn.||5. Add the rice noodles and toss gently so the noodles are thoroughly coated and mixed with the veggies. Serve immediately!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grilled Steak </t>
   </si>
   <si>
@@ -1680,9 +1604,6 @@
     <t>1. In a saucepan over medium-low heat, combine the potato starch, sugar, and 3 quarters of cup water. Using a wire whisk, stir frequently until the liquid becomes a translucent jelly, about 5 minutes.||2. Spoon the warm jelly into a silicone or nonstick mini muffin tin until the cups are about 2 thirds full. Add the sliced banana, then spoon more warm jelly on top. Make sure that no parts of the banana are poking up through the jelly.||3. Refrigerate for 1 hour, then gently pop the manju onto a plate to serve.</t>
   </si>
   <si>
-    <t>The color of this Springtime Mochi will remind you of sweet cherry blossoms and make you feel as if you’ve just spent a fine spring morning perched under a sakura tree.</t>
-  </si>
-  <si>
     <t>6*pickled*Sakura Leaves,1*tablespoon*Rice Flour (glutinous),0.5*cup*Water,6*tablespoons*Flour,1*tablespoons*Sugar,1*packet*Red Food Colouring,4*ounces*Red Bean Paste,1*splash*Oil,1*heap*Sakura Blossoms</t>
   </si>
   <si>
@@ -1695,9 +1616,6 @@
     <t>0.5*cup*Rice Flour,0.5*cup*Powdered Sugar,1*cup*Rice Flour (sweet and glutinous),1*cup*Soy Milk (cold),2*tablespoons*Milk,2*drops*Red Food Colouring,0.5*teaspoon*Matcha Powder,5*null*Bamboo Skewers</t>
   </si>
   <si>
-    <t>1. Soak the bamboo skewers in cold water for at least 30 minutes.||2. In a large bowl, combine the rice flour, powdered sugar, glutinous rice flour, and soy milk. On a flat surface, knead into a smooth dough. Add 1 to 2 tablespoons of milk or water if the dough feels too dry or falls apart.||3. Divide the dough into 3 equal portions. Add 2 drops red food coloring to 1 portion of dough, add the matcha powder to another portion, and leave the third portion white.||4. Knead each piece of dough, making sure the food coloring and matcha powder are evenly distributed. Then divide each portion into 5 equal pieces and roll them into round balls.||5. Bring a medium pot of water to a boil over high heat. Boil the dango balls over medium heat for about 15 minutes, or until they are floating. (You can do this in one batch—the white dango balls won’t be colored by the other balls.)||6. Fill a large bowl with ice water and use a slotted spoon to transfer the cooked dango balls to the bowl. Let them cool in the water until you’re ready to put them onto the skewers.||7. Insert 3 cooled dango balls onto each bamboo skewer in the order of green, white, and pink. Hand them out and enjoy!</t>
-  </si>
-  <si>
     <t>Sticky Rice Pudding, with its creamy texture and sweet flavor, will give you that extra boost of stamina you may need as you work on becoming the best adventurer you can be.</t>
   </si>
   <si>
@@ -1726,6 +1644,84 @@
   </si>
   <si>
     <t>1. To make the white dough, in a medium bowl, mix 3 quarters of a cup of the flour with 2 and 2 thirds tablespoons of the butter. Knead until smooth and cover with plastic wrap. Set aside for 30 minutes.||2. To make the red dough, mix another 3 quarters of a cup flour with 1 and 2thirds  tablespoons butter. Work in 1 tablespoon sugar and the red water mixture. Mix well and knead until a smooth dough is formed. Cover with plastic wrap and set aside for 30 minutes.||3. Add all the marzipan ingredients to a medium bowl and mix until well combined.||4. Divide the white dough, the red dough, and the marzipan each into 9 equal-size balls.||5. Using a rolling pin, flatten the red balls into circles. Wrap a white dough ball with a red dough circle, covering it entirely. Repeat with each red dough circle and white dough ball.||6. Squash down each red/white dough ball and use a rolling pin to flatten it into an oval. Roll up into a ball once again and cover with plastic wrap for 15 minutes.||7. Repeat Step 6, flattening the rolled dough into ovals, rolling them back into balls, then letting them rest for 15 minutes, covered with plastic wrap.||8. After the dough has rested, remove the plastic wrap and use your thumb to press each piece of dough into a bowl shape, letting the edges tilt up and onward the middle. Place a marzipan ball in the middle of each dough bowl, then wrap the dough edges around it to seal in the marzipan and form a ball.||9. Place the sealed side of the ball face down, then cut a star shape in the top surface of the ball, cutting only deep enough so you can just see the marzipan filling.||10. Fill a deep saucepan or fryer halfway with vegetable oil and heat to 300 degrees F. Place a lotus ball in a mesh strainer and lower it into the oil to fry. Cook 1 or 2 lotus balls at a time. Use a ladle to pour hot oil onto the balls, letting it bloom and create some layers. Each ball needs to cook around 3 to 4 minutes in the hot oil.||11. Place the cooked lotus flower crisps on a paper towel-lined plate to drain the oil. Allow to cool fully and then enjoy!</t>
+  </si>
+  <si>
+    <t>1. Soak the kombu in water for at least 30 minutes. Slice the sea bream head into pieces if necessary and place it in a separate pot of boiling water deep enough to cover the fish head. When the surface becomes white, remove and place in another bowl of cold water, then scrub clean to remove blood and stains .||2. Cut turnips into wedges and slice greens finely. Peel the bottom third of asparagus and slice into 2inch (5 cm) pieces. Slice lemon into wheels.|| 3. Pour water from step 1 and sea bream into the same pot and bring to a boil. Skim the scum off the top and lower heat to medium, Add turnip wedges(D) and let simmer, skimming regularly.|| 4. After 10 minutes, add asparagus and simmer for 5 minutes. Add salt, and soy sauce to taste. Transfer to bowls, add lemon slices, and scatter turnip greens on top.</t>
+  </si>
+  <si>
+    <t>1. Trim fat and sinew from the chicken thighs and cut into bite-size pieces-grate garlic. Put the chicken into a bowl, add mix garlic, salt, pepper and sake then marinate for 20-30 minutes.||2. Sprinkle flour over the thighs. Heat vegetable oil in a pan on medium heat, then fry chicken in batches for 4-5 minutes undisturbed on each side.</t>
+  </si>
+  <si>
+    <t>Succulent pork roast covered with a sweet-and-savory glaze and accompanied by perfectly seasoned veggies-a superb meal.</t>
+  </si>
+  <si>
+    <t>1. Let the beef sit at room temperature for 30 minutes, and grate onion and garlic for sauce. Just before cooking, rub the other garlic half against meat( C), then rub on salt and pepper. Pour oil on a heated frying pan and cook the meat surface on medium heat (D). Cover and heat on low for 6-8 minutes, then turn over and heat for another 4-5 minutes.||2. Remove from pan, wrap in aluminum foil, and let sit for 15 minutes to heat through (E).||3. Add onions, garlic and sake to the meat juice in the frying pan. Once bubbling, mix in soy sauce and butter. Once mixed in, turn off the heat, add vinegar and mix again.||4. Slice meat thinly and transfer to plate, then drizzle sauce from pan, Add mustard or wasabi as desired.</t>
+  </si>
+  <si>
+    <t>1. Lightly sprinkle salt and white pepper on the salmon. Roughly cut the cabbage, slice the onion into 4-inch (1 cm) pieces, and cut the carrot into short strips.||2.  Pour oil onto a heated frying pan and cook salmon, skin side down, on medium heat for 2-3 minutes, until browned.||3. Turn over the salmon, then add cabbage, onion, and carrot. Swirl in sake, Sprinkle sugar and miso here and there and add dabs of butter on top of the miso clumps (A). Carefully cover with aluminum foil and steam for 6-7 minutes (B).||4. Remove foil, tear salmon into chunks, and mix contents. Add soy sauce and turn off heat.</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 400 degrees F. Pierce the potatoes several times with a fork and rub with olive oil. Bake until tender, 50 to 75 minutes. While baking, you can check if the potatoes are done by sticking a skewer or a fork into them; if soft, they are ready.||2. Remove the potatoes from the oven. When cool enough to handle, slice the top off each potato horizontally (about 1 inch). Scoop out the potato pulp and transfer it to a large mixing bowl, leaving thin potato shells. Set the potato skins aside and reduce the oven temperature to 375 degrees F.||3. In a small skillet, melt the butter over medium-high heat, then add the onions and mushrooms and saute until tender, about 5 minutes.||4. In the mixing bowl, using a potato masher, mash the potato pulp. Stir in the sauteed onions and mushrooms, half-and-half, sour cream, salt, and pepper. Stuff this mixture into the 3 potato shells and top with cheddar cheese.||5. Place the stuffed potatoes on a baking sheet and bake until heated through, about 20 minutes. Top with extra chopped green onions to serve.</t>
+  </si>
+  <si>
+    <t>1. In a nonstick skillet over medium heat, place the bacon and sprinkle the brown sugar on top. Cook until just crisp, about 6 to 8 minutes. Remove from the pan and set aside.||2. Break the eggs that can't be beat into individual bowls.||3. In the same skillet over medium heat, melt the butter, then slide the eggs into the pan.||4. When the edges start to turn white, cover the pan and lower the heat. Cook 4 to 5 minutes, until the whites firm up. Season with salt and pepper.||5. Lay the bacon blankets over the eggs to serve.</t>
+  </si>
+  <si>
+    <t>1. In a bowl, stir together the graham cracker crumbs, butter, brown sugar, cinnamon, and salt.||2. Press into a 9-inch (23-cm) pie plate, and freeze for 1 hour.||3. Pour in the softened ice cream and spread evenly with a spatula. Place the pie back in the freezer for 4 to 6 hours.||4. In a large bowl, whip together the cream and confectioners' sugar just until stiff peaks form. Spread onto the pie. Top with fresh strawberries to serve.</t>
+  </si>
+  <si>
+    <t>1. To make the glaze: In a dry skillet over medium-high heat, toast the sesame seeds for 2 to 3 minutes, until fragrant. Use a mortar and pestle or a spice grinder, until it becomes powderlike.||2. In a small bowl, stir together the confectioners' sugar, the black sesame seed powder, milk, and vanilla. Set aside.||3. To make the doughnuts: Place the biscuits on a cutting board and use a 1-inch (2.5-cm) round cutter to cut holes from the middle of each biscuit.||4. In a Dutch oven, heat the oil to 350 degrees F (177 degrees C). Fry the doughnuts and holes for 1 to 2 minutes on each side, until golden brown. Transfer to a wire rack and let cool.||4. Dip the doughnuts in the glaze and place them back onto the wire rack to let the excess glaze drip off.||5. Once the glaze has set after about 20 minutes, the doughnuts are ready to serve.</t>
+  </si>
+  <si>
+    <t>1. To make the cupcakes: Preheat the oven to 350 degrees F (177 degrees C). Prep a cupcake pan with paper liners.||2. In a medium bowl, whisk together the cake flour, baking powder, and salt.||3. In the bowl of an electric mixer, cream the butter and sugar until fluffy.||4. Add the eggs and vanilla, stirring until just combined. Stir in the flour mixture, alternating with buttermilk. Spoon the batter into the prepped cupcake pan.||5. Bake for 16 to 17 minutes, or until a toothpick inserted in the center comes out clean.||6. Let cool on a wire rack.||7. To make the frosting: In a large bowl with a handheld mixer on low, cream the butter while slowly adding the confectioners' sugar. Stir in the heavy whipping cream, vanilla, and salt.Add food coloring and stir, until the frosting becomes a light pink color.||8. Turn the mixer up to medium-high and whip for 10 to 15 seconds, until light and fluffy.||9. To assemble: Pipe the frosting onto the cupcakes to serve.</t>
+  </si>
+  <si>
+    <t>1.. In a large bowl, mix together all the ingredients except the chicken and mushrooms to create a marinade.||2. Cut the chicken breasts into bite-size pieces. Place the chicken and mushrooms in the bowl of marinade and stir until thoroughly coated. Cover and refrigerate for 4 to 10 hours, stirring occasionally.||3. If you're using bamboo skewers, soak them in water for a few minutes right before the chicken and mushrooms are done marinating to keep them from burning when it comes time to cook. Then pat dry.||4. Thread the chicken and mushrooms on the skewers, discarding any remaining marinade. Grill on high heat until cooked, 5 to 7 minutes, or bake in the oven at 430 degrees F for 8 to 10 minutes. Enjoy!</t>
+  </si>
+  <si>
+    <t>1. In a medium bowl, combine the eggs, water, soy sauce, and sugar. Using a whisk, beat until well combined.||2. Heat a tamagoyaki pan (rectangular Japanese omelet pan) or a small frying pan over medium heat. Using a pastry brush, lightly coat the bottom of the pan with olive oil.||3. Pour a thin layer of the egg mixture to cover the surface of the pan. When it's about 80 percent cooked but still wet on the surface, use chopsticks or wooden tongs to start gently rolling in the edges to form a rolled omelet. Move the rolled omelet to one side of the pan.||4. Brush the pan with oil again and pour in another thin layer of the egg mixture. Using a spoon, gently lift the previously made omelet and spread some of the uncooked egg mixture underneath. This willhelp both omelets stick together. When this next layer of eggs is 80 percent cooked but the surface is still wet, start with the previously made omelet and gently roll it up with the new layer. Set to one side of the pan. Repeat this process until the egg mixture is gone. Your omelet will have 3 to 4 layers.||5. Transfer the rolled omelet onto a cutting board and allow to rest for several minutes. Cut into even 2-inch slices and serve.</t>
+  </si>
+  <si>
+    <t>1. Pat all the vegetables and shrimp dry with a paper towel and set aside.||2. Add the oil to a deep fryer or a medium pot on the stovetop and heat to 320 degrees F. (Use a thermometer to check the temperature, or dip the tip of a wooden or bamboo chopstick in the oil. If small bubbles appear around the chopstick, the oil is ready.)||3. While the oil is heating, prepare the tempura batter. Place the all-purpose flour in a large bowl. In a smaller bowl, whisk together the ice water and egg until fully combined. Scoop up and discard any surface foam.||4. Slowly pour the egg mixture into the flour while mixing with chopsticks or a wire whisk. Once all the egg mixture is in, continue whisking gently for about 15 seconds. Be careful not to overmix; it's okay to leave some lumps in your batter. It's important to keep the tempura batter cold, so set your bowl of batter inside a larger bowl filled with about 1 inch of ice water.||5. When the oil reaches the right temperature, start by dipping an eggplant slice in the cold batter, letting any excess batter drip off for a few seconds before very gently placing the eggplant in the hot oil. Repeat this with each individual ingredient you're going to deep fry, but make sure you don't overcrowd the deep fryer or cooking pot. The ingredients should take up only half of the surface area at any time. (Having too many ingredients in the pot at once will cause the oil temperature to drop.)||6. Deep-fry the vegetables and shrimp for 1 to 2 minutes each and the sakura petals or nettle leaves for 15 to 20 seconds, or until golden. Continue frying in batches until all the ingredients have been cooked, transferring each batch to a baking sheet or plate lined with paper towels to absorb excess oil. Between batches, skim any leftover tempura crumbs from the top of the oil so they don't burn and change the flavor of the oil.||7. Serve the tempura immediately with wasabi and/or soy sauce for dipping.</t>
+  </si>
+  <si>
+    <t>1. Cook the rice noodles according to the package instructions. Drain and set aside.||2. Add the oil to a wok or large frying pan over medium-high heat. Heat for about 2 minutes and then add the onion and bell peppers slices. Saute for 3 minutes, stirring frequently.||3. Stir in the garlic, hoisin sauce, and soy sauce and cook for 1 minute.||4. Season the tilapia pieces with salt and pepper and add to the pan. Cook for 2 to 3 minutes, stirring frequently so the fish doesn't burn.||5. Add the rice noodles and toss gently so the noodles are thoroughly coated and mixed with the veggies. Serve immediately!</t>
+  </si>
+  <si>
+    <t>The color of this Springtime Mochi will remind you of sweet cherry blossoms and make you feel as if you've just spent a fine spring morning perched under a sakura tree.</t>
+  </si>
+  <si>
+    <t>1. Soak the bamboo skewers in cold water for at least 30 minutes.||2. In a large bowl, combine the rice flour, powdered sugar, glutinous rice flour, and soy milk. On a flat surface, knead into a smooth dough. Add 1 to 2 tablespoons of milk or water if the dough feels too dry or falls apart.||3. Divide the dough into 3 equal portions. Add 2 drops red food coloring to 1 portion of dough, add the matcha powder to another portion, and leave the third portion white.||4. Knead each piece of dough, making sure the food coloring and matcha powder are evenly distributed. Then divide each portion into 5 equal pieces and roll them into round balls.||5. Bring a medium pot of water to a boil over high heat. Boil the dango balls over medium heat for about 15 minutes, or until they are floating. (You can do this in one batch-the white dango balls won't be colored by the other balls.)||6. Fill a large bowl with ice water and use a slotted spoon to transfer the cooked dango balls to the bowl. Let them cool in the water until you're ready to put them onto the skewers.||7. Insert 3 cooled dango balls onto each bamboo skewer in the order of green, white, and pink. Hand them out and enjoy!</t>
+  </si>
+  <si>
+    <t>1. Place the eggs in a pot and cover with 1 to 2 inches (2.5-5 cm) of water. Turn on the heat to medium-high and bring to a boil.||2. Turn off the heat, cover with a lid, and let sit for 10 to 12 minutes.||3. Place the eggs in an ice bath and let cool completely.||4. Peel and slice the eggs in half. Set aside the whites and place the yolks into a bowl.||5. Stir together the egg yolks, mayonnaise, mustard, onion powder, salt, and pepper.||6. Place the mixture into a piping bag and pipe the filling into the egg white centers.||7. Place an olive half on top of each egg to serve.</t>
+  </si>
+  <si>
+    <t>1. To prepare the pork cutlets, slice the pork loin into 4 equal pieces. Place each slice in a sealed plastic bag with all the air removed or between 2 sheets of plastic wrap. Using a meat tenderizer, gently pound each slice until it is about 6 inches wide and half aninch thick.||2. In a medium bowl, combine the shio koji, 2 teaspoons salt, and 1 cup water; stir well until the salt is fully dissolved. Add the pork pieces, then cover and chill in the refrigerator for 8 hours or overnight.||3. Just before the pork is done chilling, place the cabbage in a medium bowl. Zest both lemons over the cabbage and then add the juice from the lemons. Season with a half teaspoon salt and toss with your hands until the cabbage is fully coated and slightly wilted. Cover and chill until ready to use.||4. After the pork has chilled, remove it from the refrigerator, drain, and set aside. Line a rimmed baking sheet with paper towels, set a wire rack on top, and place near the stovetop.||5. In a shallow dish, whisk together the eggs and 2 tablespoons water. Place the flour and the bread crumbs in 2 more shallow dishes. Working with a single pork cutlet at a time, first coat it in the flour, shaking off any excess. Then dip it in the eggs and finally in the bread crumbs, pressing firmly into the crumbs on both sides to make sure they stick. Transfer to another rimmed baking sheet or a platter.||6. Pour oil into a medium-deep pot so that it comes about 2 inches up the side. Heat over medium-high heat until an instant-read thermometer reads between 350 degrees F and 365 degrees F. Using chopsticks or tongs, lower a cutlet vertically into the pan, letting it slide away into the oil until it lies flat. Use the chopsticks or tongs to keep the pork fully submerged in the oil until the underside is golden brown, about 1 minute. Gently flip and cook the other side until it is also golden brown, about 1 more minute. Then transfer the cutlet to the prepared wire rack over the paper towel-lined baking sheet. Repeat with the remaining pork cutlets.||7. Drizzle tonkatsu sauce over the cutlets and let rest for a few minutes. Then spread Kewpie mayonnaise on half of the bread slices and add a few cabbage leaves. Top with a pork cutlet and a second slice of bread, then cut each sandwich in half.</t>
+  </si>
+  <si>
+    <t>1. Fill a large saucepan a third full with water, add a pinch of salt, and bring to a boil over high heat.||2. While the water is coming to a boil, in a large mixing bowl, combine the ground pork, beaten egg, 3 chopped green onions, ginger, garlic, soy sauce, 1 tablespoon toasted sesame oil, crushed red pepper flakes, half a teaspoon salt, pepper, and paprika. Mix to combine thoroughly, then set aside.||3. Place the cabbage leaves and 10 whole green onions in the boiling water for 3 minutes to soften them. Meanwhile, line a baking sheet with paper towels. Transfer the softened leaves and onions to the baking sheet and let cool.||4. Use the paper towels to pat off any excess water. Then spread out a cabbage leaf and place about 1 1/2 tablespoons of the pork mixture in the middle of the leaf. Gather the leaf edges together and gently tie with a softened green onion. Repeat until all the cabbage leaves are filled with pork and tied shut.||5. In a pot that can hold a steamer basket, combine the 2 cups broth, the remaining 1 teaspoon sesame oil, and the chili slices. Set the steamer basket on top of the pot. (The pot should be filled to just below your basket so that the broth doesn't touch the dumplings.)||6. Place the dumplings in the steamer basket and bring the broth to a boil. Then cover with the pot lid and let steam until the pork is cooked through, about 15 minutes. To test, cut a dumpling open and make sure the pork has browned so no pink coloring remains.||7. Using tongs, carefully transfer the dumplings to a serving plate. Pour the chili broth you used for the steaming over the dumplings until they're sitting in a thin layer of the broth, then serve.</t>
+  </si>
+  <si>
+    <t>1. Remove the shiitake mushrooms from their base and cut them into half-inch (1 cm) slices. Remove the shimeji mushrooms from their base and separate them into small bunches. Trim king oyster mushrooms to a length of 1 and a half inches (3cm) and slice thinly. Cut bacon into quarter-inch (7 mm) slices.||2. Put vegetable oil and rosemary into a frying pan and heat on medium. When oil is fragrant, fry bacon briefly, then add all mushrooms and mix. Cover and steam on low heat for 4 minutes.||3. Remove the lid, add salt, and mix again. Cover again and continue steaming for 4-5 minutes, stirring occasionally, until the liquid is gone and the bacon is fried and no longer appears pink. If needed, add more salt and pepper for flavour, then add butter, mix, and turn off heat.</t>
+  </si>
+  <si>
+    <t>1. Place finely cut shoestring potatoes using a mandoline at a one-third-inch setting if available, and mix with cheese.||2. Pour a generous amount (around a quarter cup) of oil into a frying pan. Pack a quarter of the potatoes tightly and fry on low heat for 7-8 minutes. Turn over and fry another 7-8 minutes, until both sides are crispy. Be careful not to prod too much while frying, as it will come apart. Once cooked, dab dry with paper towels, then sprinkle with salt.||3. Repeat for the other three portions.</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 450 degrees F (230 degrees C). Prep a baking sheet with parchment paper.||2. Separate the eggs, placing the whites in a large bowl. Set aside the yolks, keeping them intact.||3. Beat the egg whites until stiff peaks form.||4. Fold in the Parmesan cheese, salt, and white pepper.||5. Spoon the whipped whites into two separate mounds and place them onto the prepped baking sheet.||6. With the back of a spoon, create an indentation in the center of each mound.||7. Bake for 2 minutes. Gently pour the egg yolks into the indentations. Return to the oven and cook for another 3 minutes. Serve immediately.</t>
+  </si>
+  <si>
+    <t>1. In a small bowl, stir together the mayonnaise and pesto. Set aside.||2. In a skillet over medium-high heat, cook the bacon for 5 to 6 minutes, until crispy. Drain on paper towels.||3. Lightly toast the bread.||4. Spread the mayonnaise mixture onto both sides of the toast. On one slice, layer the bacon, then the tomato.||5. Season with pepper.||6. Place the lettuce on top, then the remaining slice of toast.||7. Slice in half to serve.</t>
+  </si>
+  <si>
+    <t>1. Make chicken drumstick 'tulips.' Use kitchen scissors to cut the meat loose from the handle end of the drumstick (A). Roll the meat down the bone until it is fully inside-out at the end.||2. Soak the breadcrumbs in milk. Knead ground chicken, salt, pepper and egg in a bowl, then add breadcrumbs and knead again.||3.  Fold the meaty end of the drumstick around a hard-boiled egg (B). If the meat doesn't cover well enough, add cuts to loosen it up. Oil hands lightly and cover drumstick and egg with the breadcrumb mixture from the previous step.||4. Bake at 400 degrees Fahrenheit  (200 degrees Celsius) for 15-20 minutes, watching carefully</t>
+  </si>
+  <si>
+    <t>1*package*Hashbrown Potatoes (frozen and shredded and thawed),2*null*Eggs,1*cup*Cheddar Cheese (shredded),1*pinch*Salt,1*pinch*Pepper,1*teaspoon*Ground Cumin,1*teaspoon*Dried Mint,0.5*teaspoon*Garlic Powder,0.5*teaspoon*Onion Powder,0.5*cup*Unsalted Butter (melted)</t>
+  </si>
+  <si>
+    <t>1*package*Rice Tagliatelle Noodles,3*tablespoons*Olive Oil,0.5*null*Onion (sliced),1*null*Green Bell Pepper (sliced),1*null*Red Bell Pepper (sliced),3*cloves*Garlic (minced),1*teaspoon*Hoisin sauce,2*tablespoons*Soy sauce,1*null*Tilapia Filet (cut into 1inch pieces),1*sprinkle*Salt,1*sprinkle*Pepper</t>
   </si>
 </sst>
 </file>
@@ -2177,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
   <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3653,7 +3649,7 @@
         <v>289</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>290</v>
+        <v>536</v>
       </c>
       <c r="F64" s="1">
         <v>60</v>
@@ -3664,19 +3660,19 @@
     </row>
     <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E65" s="10" t="s">
-        <v>301</v>
+        <v>537</v>
       </c>
       <c r="F65" s="1">
         <v>50</v>
@@ -3687,19 +3683,19 @@
     </row>
     <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="E66" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F66" s="1">
         <v>30</v>
@@ -3710,19 +3706,19 @@
     </row>
     <row r="67" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="E67" s="10" t="s">
-        <v>302</v>
+        <v>539</v>
       </c>
       <c r="F67" s="1">
         <v>70</v>
@@ -3733,19 +3729,19 @@
     </row>
     <row r="68" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>306</v>
+        <v>559</v>
       </c>
       <c r="F68" s="1">
         <v>40</v>
@@ -3756,19 +3752,19 @@
     </row>
     <row r="69" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F69" s="1">
         <v>100</v>
@@ -3779,19 +3775,19 @@
     </row>
     <row r="70" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F70" s="1">
         <v>115</v>
@@ -3802,19 +3798,19 @@
     </row>
     <row r="71" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F71" s="1">
         <v>90</v>
@@ -3825,19 +3821,19 @@
     </row>
     <row r="72" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F72" s="1">
         <v>80</v>
@@ -3848,19 +3844,19 @@
     </row>
     <row r="73" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F73" s="1">
         <v>95</v>
@@ -3871,19 +3867,19 @@
     </row>
     <row r="74" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F74" s="1">
         <v>40</v>
@@ -3894,19 +3890,19 @@
     </row>
     <row r="75" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F75" s="1">
         <v>30</v>
@@ -3917,19 +3913,19 @@
     </row>
     <row r="76" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F76" s="1">
         <v>25</v>
@@ -3940,19 +3936,19 @@
     </row>
     <row r="77" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>342</v>
+        <v>540</v>
       </c>
       <c r="F77" s="1">
         <v>25</v>
@@ -3963,19 +3959,19 @@
     </row>
     <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F78" s="1">
         <v>10</v>
@@ -3986,19 +3982,19 @@
     </row>
     <row r="79" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F79" s="1">
         <v>210</v>
@@ -4009,19 +4005,19 @@
     </row>
     <row r="80" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F80" s="1">
         <v>20</v>
@@ -4030,21 +4026,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>358</v>
+        <v>555</v>
       </c>
       <c r="F81" s="1">
         <v>35</v>
@@ -4055,19 +4051,19 @@
     </row>
     <row r="82" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="F82" s="1">
         <v>10</v>
@@ -4076,21 +4072,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>366</v>
+        <v>556</v>
       </c>
       <c r="F83" s="1">
         <v>80</v>
@@ -4101,19 +4097,19 @@
     </row>
     <row r="84" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="F84" s="1">
         <v>30</v>
@@ -4124,19 +4120,19 @@
     </row>
     <row r="85" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="F85" s="1">
         <v>7</v>
@@ -4147,19 +4143,19 @@
     </row>
     <row r="86" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="F86" s="1">
         <v>35</v>
@@ -4170,19 +4166,19 @@
     </row>
     <row r="87" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="F87" s="1">
         <v>20</v>
@@ -4193,19 +4189,19 @@
     </row>
     <row r="88" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="F88" s="1">
         <v>10</v>
@@ -4214,21 +4210,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>390</v>
-      </c>
       <c r="E89" s="10" t="s">
-        <v>391</v>
+        <v>557</v>
       </c>
       <c r="F89" s="1">
         <v>20</v>
@@ -4239,19 +4235,19 @@
     </row>
     <row r="90" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="F90" s="1">
         <v>45</v>
@@ -4262,19 +4258,19 @@
     </row>
     <row r="91" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>399</v>
+        <v>542</v>
       </c>
       <c r="F91" s="1">
         <v>25</v>
@@ -4283,21 +4279,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>403</v>
+        <v>558</v>
       </c>
       <c r="F92" s="1">
         <v>15</v>
@@ -4308,19 +4304,19 @@
     </row>
     <row r="93" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="F93" s="1">
         <v>10</v>
@@ -4331,19 +4327,19 @@
     </row>
     <row r="94" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>411</v>
+        <v>552</v>
       </c>
       <c r="F94" s="1">
         <v>40</v>
@@ -4354,19 +4350,19 @@
     </row>
     <row r="95" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="F95" s="1">
         <v>30</v>
@@ -4377,19 +4373,19 @@
     </row>
     <row r="96" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="F96" s="1">
         <v>15</v>
@@ -4400,19 +4396,19 @@
     </row>
     <row r="97" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="F97" s="1">
         <v>30</v>
@@ -4423,19 +4419,19 @@
     </row>
     <row r="98" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="F98" s="1">
         <v>220</v>
@@ -4446,19 +4442,19 @@
     </row>
     <row r="99" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="F99" s="1">
         <v>35</v>
@@ -4469,19 +4465,19 @@
     </row>
     <row r="100" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>432</v>
+        <v>543</v>
       </c>
       <c r="F100" s="1">
         <v>420</v>
@@ -4492,19 +4488,19 @@
     </row>
     <row r="101" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>433</v>
+        <v>544</v>
       </c>
       <c r="F101" s="1">
         <v>50</v>
@@ -4515,19 +4511,19 @@
     </row>
     <row r="102" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>471</v>
+        <v>545</v>
       </c>
       <c r="F102" s="12">
         <v>45</v>
@@ -4538,19 +4534,19 @@
     </row>
     <row r="103" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="B103" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C103" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="F103" s="12">
         <v>100</v>
@@ -4561,19 +4557,19 @@
     </row>
     <row r="104" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="D104" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>457</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>470</v>
       </c>
       <c r="F104" s="1">
         <v>95</v>
@@ -4584,19 +4580,19 @@
     </row>
     <row r="105" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="D105" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E105" s="3" t="s">
         <v>456</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>469</v>
       </c>
       <c r="F105" s="12">
         <v>8</v>
@@ -4607,19 +4603,19 @@
     </row>
     <row r="106" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="F106" s="12">
         <v>20</v>
@@ -4630,19 +4626,19 @@
     </row>
     <row r="107" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C107" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="F107" s="12">
         <v>10</v>
@@ -4653,19 +4649,19 @@
     </row>
     <row r="108" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C108" t="s">
+        <v>439</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C108" t="s">
+      <c r="E108" s="3" t="s">
         <v>452</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>465</v>
       </c>
       <c r="F108" s="12">
         <v>7</v>
@@ -4676,19 +4672,19 @@
     </row>
     <row r="109" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="F109" s="12">
         <v>10</v>
@@ -4699,19 +4695,19 @@
     </row>
     <row r="110" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="E110" s="10" t="s">
-        <v>476</v>
+        <v>546</v>
       </c>
       <c r="F110" s="12">
         <v>30</v>
@@ -4722,19 +4718,19 @@
     </row>
     <row r="111" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="E111" s="10" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="F111" s="12">
         <v>30</v>
@@ -4745,19 +4741,19 @@
     </row>
     <row r="112" spans="1:7" ht="288" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="F112" s="12">
         <v>40</v>
@@ -4768,19 +4764,19 @@
     </row>
     <row r="113" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E113" s="10" t="s">
         <v>473</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="E113" s="10" t="s">
-        <v>488</v>
       </c>
       <c r="F113" s="12">
         <v>10</v>
@@ -4791,19 +4787,19 @@
     </row>
     <row r="114" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>492</v>
+        <v>547</v>
       </c>
       <c r="F114" s="12">
         <v>20</v>
@@ -4814,19 +4810,19 @@
     </row>
     <row r="115" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>496</v>
+        <v>541</v>
       </c>
       <c r="F115" s="12">
         <v>105</v>
@@ -4837,19 +4833,19 @@
     </row>
     <row r="116" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>499</v>
+        <v>560</v>
       </c>
       <c r="E116" s="10" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="F116" s="12">
         <v>50</v>
@@ -4860,19 +4856,19 @@
     </row>
     <row r="117" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="F117" s="12">
         <v>25</v>
@@ -4883,19 +4879,19 @@
     </row>
     <row r="118" spans="1:7" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>508</v>
+        <v>554</v>
       </c>
       <c r="F118" s="12">
         <v>45</v>
@@ -4906,19 +4902,19 @@
     </row>
     <row r="119" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>512</v>
+        <v>548</v>
       </c>
       <c r="F119" s="12">
         <v>70</v>
@@ -4929,19 +4925,19 @@
     </row>
     <row r="120" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
       <c r="F120" s="12">
         <v>15</v>
@@ -4952,19 +4948,19 @@
     </row>
     <row r="121" spans="1:7" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>520</v>
+        <v>553</v>
       </c>
       <c r="F121" s="12">
         <v>30</v>
@@ -4975,19 +4971,19 @@
     </row>
     <row r="122" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
       <c r="E122" s="10" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
       <c r="F122" s="12">
         <v>160</v>
@@ -4998,19 +4994,19 @@
     </row>
     <row r="123" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>527</v>
+        <v>505</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>528</v>
+        <v>506</v>
       </c>
       <c r="F123" s="12">
         <v>150</v>
@@ -5021,19 +5017,19 @@
     </row>
     <row r="124" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>529</v>
+        <v>507</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>530</v>
+        <v>508</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>531</v>
+        <v>561</v>
       </c>
       <c r="E124" s="10" t="s">
-        <v>532</v>
+        <v>549</v>
       </c>
       <c r="F124" s="12">
         <v>25</v>
@@ -5044,19 +5040,19 @@
     </row>
     <row r="125" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>534</v>
+        <v>510</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>535</v>
+        <v>511</v>
       </c>
       <c r="E125" s="10" t="s">
-        <v>536</v>
+        <v>512</v>
       </c>
       <c r="F125" s="12">
         <v>30</v>
@@ -5067,19 +5063,19 @@
     </row>
     <row r="126" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>537</v>
+        <v>513</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>543</v>
+        <v>519</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>544</v>
+        <v>520</v>
       </c>
       <c r="E126" s="10" t="s">
-        <v>545</v>
+        <v>521</v>
       </c>
       <c r="F126" s="12">
         <v>70</v>
@@ -5090,19 +5086,19 @@
     </row>
     <row r="127" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>538</v>
+        <v>514</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>547</v>
+        <v>522</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>548</v>
+        <v>523</v>
       </c>
       <c r="F127" s="12">
         <v>20</v>
@@ -5111,18 +5107,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>539</v>
+        <v>515</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>549</v>
+        <v>524</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>550</v>
+        <v>525</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>551</v>
@@ -5136,19 +5132,19 @@
     </row>
     <row r="129" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>540</v>
+        <v>516</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>555</v>
+        <v>529</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>556</v>
+        <v>530</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>557</v>
+        <v>531</v>
       </c>
       <c r="F129" s="12">
         <v>75</v>
@@ -5159,19 +5155,19 @@
     </row>
     <row r="130" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>541</v>
+        <v>517</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>552</v>
+        <v>526</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>553</v>
+        <v>527</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>554</v>
+        <v>528</v>
       </c>
       <c r="F130" s="12">
         <v>50</v>
@@ -5182,19 +5178,19 @@
     </row>
     <row r="131" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>542</v>
+        <v>518</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>558</v>
+        <v>532</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
       <c r="F131" s="12">
         <v>30</v>

</xml_diff>

<commit_message>
Finished the Naruto Recipes
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkish\Downloads\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF571E9-03AF-430E-AADB-967B05C672D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF50B63-D54E-4EB5-8457-4B86CA72A00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="761">
   <si>
     <t>Name</t>
   </si>
@@ -2303,6 +2303,30 @@
   </si>
   <si>
     <t>1. Combine the ice, shochu, vermouth, and yuzu juice in a cocktail shaker and shake well.||2. Strain and pour into a martini glass.||3. Take the lemon peel with both hands and twist it over the glass to express some of the oil, then rub the rim of the glass with it to add extra flavor. Garnish with the lemon peel and serve.</t>
+  </si>
+  <si>
+    <t>Narutomaki Sugar Cookies</t>
+  </si>
+  <si>
+    <t>A naruto inspired sugar cookie.</t>
+  </si>
+  <si>
+    <t>0.25*cup*Butter (softened),0.25*cup*Sugar,1*large*Egg,0.5*teaspoon*Vanilla Extract,0.75*cup*Flour,0.25*teaspoon*Salt,2*tablespoons*Matcha Powder,1*bowl*Coloured Sprinkles</t>
+  </si>
+  <si>
+    <t>1. Place the butter and sugar in a large bowl and stir until combined, then whisk in the egg and vanilla. Sift the flour and salt together, then add to the butter-sugar mixture and stir until well combined.||2. Place a sheet of plastic wrap on your work surface, then spread the mixture evenly on the wrap, making a roughly 9-by-9-inch square. Sprinkle the flavoring over the dough, keeping a 2-inch strip bare on one side.||3. Positioning the rectangle with the bare strip away from you, start at the near side and gently begin rolling up the dough into a cylinder. Use the plastic to guide the dough, and pull it away from the dough as it’s rolled. When the dough is rolled up, wrap it again in the plastic.||4. To create the crinkled narutomaki shape, wrap the dough log in a sushi rolling mat, pressing firmly once it’s fully wrapped to imprint the mat lines in the dough. Unwrap carefully so as to not lose any texture, then place in the freezer to firm up for at least 1 hour.||5. To bake, preheat the oven to 325 degrees Fahrenheit.||6. Unwrap the chilled dough and cut into quarter-inch slices. Arrange the cookies 1 inch apart on parchment-lined baking sheets, then bake for 11 to 14 minutes, until lightly golden.||7. Transfer to wire racks to cool.</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 325 degrees F. Line an 8-by-4-inch loaf pan with parchment paper or grease with oil, then set aside.||2. In a large bowl, beat the eggs with a hand mixer set on high.||3. Add the sugar, and keep mixing at high speed for about 8 to 10 minutes until stiff peaks form in the batter. It will grow in size dramatically—this foam is what gives the cake lift! Take care not to overbeat it once the peaks are achieved, otherwise it could start to collapse. Turn the speed down to low, then mix in 3 tablespoons of honey and the salt.||4. Sift the flour into a separate bowl, then add about one-third of the flour to the egg mixture and beat on low speed until combined. Repeat this twice more until all the flour has been combined.||5. Pour half of the batter into a separate bowl. Add the cocoa powder to the second bowl and stir until combined.||6. To create the marble effect, first pour some of the plain batter into the prepared baking pan. Top it with some of the chocolate batter, then more of the plain. Repeat this process until you have about half a cup of each batter left. Draw a knife through the poured batter to create swirls in the cake, then carefully pour the remaining plain batter on top, smoothing it out over the center of the surface. To create the curse marks, pour three circles of the remaining chocolate batter, arranged in a small triangle, in the middle of the cake, then draw the knife through each circle in an outward motion, creating a comma shape with each one.||7. Bake on the middle rack for 40 minutes, until a skewer inserted into the center comes out clean. If not, continue baking for 5-minute intervals until the correct doneness is achieved.||8. Flip the cake over on the counter to remove from the pan, then immediately cover with plastic wrap. When cooled, remove the wrap and trim off the sides of the cake, exposing the marbled cake underneath.||9. Just before serving, mix the remaining 1 tablespoon of honey with 1 tablespoon of water and brush on the top.</t>
+  </si>
+  <si>
+    <t>4*large*Eggs (room temperature),0.5*cup*Sugar,4*tablespoons*Honey,0.125*teaspoon*Salt,0.6*cup*Bread Flour,1*tablespoon*Unsweetened Cocoa Powder</t>
+  </si>
+  <si>
+    <t>This honeyed sponge cake has a long history in Japan as well as in Konoha village. They’re traditionally served plain, but the chocolate marble in this variation serves to mimic Sasuke’s curse marks—though with a sweeter result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sasuke's Curse Mark Castella </t>
   </si>
 </sst>
 </file>
@@ -2770,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
-  <dimension ref="A1:M195"/>
+  <dimension ref="A1:M197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E193" zoomScale="95" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="E195" sqref="E195"/>
+    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="95" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7348,20 +7372,168 @@
         <v>11</v>
       </c>
     </row>
+    <row r="196" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A196" s="14" t="s">
+        <v>753</v>
+      </c>
+      <c r="B196" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D196" s="14" t="s">
+        <v>755</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="F196" s="14">
+        <v>95</v>
+      </c>
+      <c r="G196" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A197" s="14" t="s">
+        <v>760</v>
+      </c>
+      <c r="B197" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="C197" s="13" t="s">
+        <v>759</v>
+      </c>
+      <c r="D197" s="14" t="s">
+        <v>758</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="F197" s="14">
+        <v>75</v>
+      </c>
+      <c r="G197" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="150">
-    <mergeCell ref="H134:H135"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="J134:J135"/>
-    <mergeCell ref="K134:K135"/>
-    <mergeCell ref="L134:L135"/>
-    <mergeCell ref="M134:M135"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="J169:J171"/>
+    <mergeCell ref="K169:K171"/>
+    <mergeCell ref="L169:L171"/>
+    <mergeCell ref="M169:M171"/>
+    <mergeCell ref="J166:J168"/>
+    <mergeCell ref="K166:K168"/>
+    <mergeCell ref="L166:L168"/>
+    <mergeCell ref="M166:M168"/>
+    <mergeCell ref="A169:A171"/>
+    <mergeCell ref="B169:B171"/>
+    <mergeCell ref="C169:C171"/>
+    <mergeCell ref="D169:D171"/>
+    <mergeCell ref="F169:F171"/>
+    <mergeCell ref="G169:G171"/>
+    <mergeCell ref="M163:M165"/>
+    <mergeCell ref="A166:A168"/>
+    <mergeCell ref="B166:B168"/>
+    <mergeCell ref="C166:C168"/>
+    <mergeCell ref="D166:D168"/>
+    <mergeCell ref="E166:E168"/>
+    <mergeCell ref="F166:F168"/>
+    <mergeCell ref="G166:G168"/>
+    <mergeCell ref="H166:H168"/>
+    <mergeCell ref="I166:I168"/>
+    <mergeCell ref="G163:G165"/>
+    <mergeCell ref="H163:H165"/>
+    <mergeCell ref="I163:I165"/>
+    <mergeCell ref="J163:J165"/>
+    <mergeCell ref="K163:K165"/>
+    <mergeCell ref="L163:L165"/>
+    <mergeCell ref="H169:H171"/>
+    <mergeCell ref="I169:I171"/>
+    <mergeCell ref="J159:J161"/>
+    <mergeCell ref="K159:K161"/>
+    <mergeCell ref="L159:L161"/>
+    <mergeCell ref="M159:M161"/>
+    <mergeCell ref="A163:A165"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="C163:C165"/>
+    <mergeCell ref="D163:D165"/>
+    <mergeCell ref="E163:E165"/>
+    <mergeCell ref="F163:F165"/>
+    <mergeCell ref="L151:L152"/>
+    <mergeCell ref="M151:M152"/>
+    <mergeCell ref="M156:M158"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="B159:B161"/>
+    <mergeCell ref="C159:C161"/>
+    <mergeCell ref="D159:D161"/>
+    <mergeCell ref="E159:E161"/>
+    <mergeCell ref="F159:F161"/>
+    <mergeCell ref="G159:G161"/>
+    <mergeCell ref="H159:H161"/>
+    <mergeCell ref="I159:I161"/>
+    <mergeCell ref="G156:G158"/>
+    <mergeCell ref="H156:H158"/>
+    <mergeCell ref="I156:I158"/>
+    <mergeCell ref="J156:J158"/>
+    <mergeCell ref="K156:K158"/>
+    <mergeCell ref="L156:L158"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="B156:B158"/>
+    <mergeCell ref="C156:C158"/>
+    <mergeCell ref="D156:D158"/>
+    <mergeCell ref="E156:E158"/>
+    <mergeCell ref="F156:F158"/>
+    <mergeCell ref="G153:G155"/>
+    <mergeCell ref="M147:M148"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="C151:C152"/>
+    <mergeCell ref="D151:D152"/>
+    <mergeCell ref="F151:F152"/>
+    <mergeCell ref="G151:G152"/>
+    <mergeCell ref="H151:H152"/>
+    <mergeCell ref="I151:I152"/>
+    <mergeCell ref="J151:J152"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="H147:H148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="J147:J148"/>
+    <mergeCell ref="K147:K148"/>
+    <mergeCell ref="L147:L148"/>
+    <mergeCell ref="H153:H155"/>
+    <mergeCell ref="I153:I155"/>
+    <mergeCell ref="J153:J155"/>
+    <mergeCell ref="K153:K155"/>
+    <mergeCell ref="L153:L155"/>
+    <mergeCell ref="M153:M155"/>
+    <mergeCell ref="K151:K152"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="D153:D155"/>
+    <mergeCell ref="E153:E155"/>
+    <mergeCell ref="F153:F155"/>
+    <mergeCell ref="M142:M143"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="H145:H146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="J145:J146"/>
+    <mergeCell ref="K145:K146"/>
+    <mergeCell ref="L145:L146"/>
+    <mergeCell ref="M145:M146"/>
     <mergeCell ref="M138:M140"/>
     <mergeCell ref="A142:A143"/>
     <mergeCell ref="B142:B143"/>
@@ -7386,120 +7558,18 @@
     <mergeCell ref="F138:F140"/>
     <mergeCell ref="K142:K143"/>
     <mergeCell ref="L142:L143"/>
-    <mergeCell ref="M142:M143"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="H145:H146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="J145:J146"/>
-    <mergeCell ref="K145:K146"/>
-    <mergeCell ref="L145:L146"/>
-    <mergeCell ref="M145:M146"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="D153:D155"/>
-    <mergeCell ref="E153:E155"/>
-    <mergeCell ref="F153:F155"/>
-    <mergeCell ref="G153:G155"/>
-    <mergeCell ref="M147:M148"/>
-    <mergeCell ref="A151:A152"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="C151:C152"/>
-    <mergeCell ref="D151:D152"/>
-    <mergeCell ref="F151:F152"/>
-    <mergeCell ref="G151:G152"/>
-    <mergeCell ref="H151:H152"/>
-    <mergeCell ref="I151:I152"/>
-    <mergeCell ref="J151:J152"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="H147:H148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="J147:J148"/>
-    <mergeCell ref="K147:K148"/>
-    <mergeCell ref="L147:L148"/>
-    <mergeCell ref="H153:H155"/>
-    <mergeCell ref="I153:I155"/>
-    <mergeCell ref="J153:J155"/>
-    <mergeCell ref="K153:K155"/>
-    <mergeCell ref="L153:L155"/>
-    <mergeCell ref="M153:M155"/>
-    <mergeCell ref="K151:K152"/>
-    <mergeCell ref="L151:L152"/>
-    <mergeCell ref="M151:M152"/>
-    <mergeCell ref="M156:M158"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="B159:B161"/>
-    <mergeCell ref="C159:C161"/>
-    <mergeCell ref="D159:D161"/>
-    <mergeCell ref="E159:E161"/>
-    <mergeCell ref="F159:F161"/>
-    <mergeCell ref="G159:G161"/>
-    <mergeCell ref="H159:H161"/>
-    <mergeCell ref="I159:I161"/>
-    <mergeCell ref="G156:G158"/>
-    <mergeCell ref="H156:H158"/>
-    <mergeCell ref="I156:I158"/>
-    <mergeCell ref="J156:J158"/>
-    <mergeCell ref="K156:K158"/>
-    <mergeCell ref="L156:L158"/>
-    <mergeCell ref="A156:A158"/>
-    <mergeCell ref="B156:B158"/>
-    <mergeCell ref="C156:C158"/>
-    <mergeCell ref="D156:D158"/>
-    <mergeCell ref="E156:E158"/>
-    <mergeCell ref="F156:F158"/>
-    <mergeCell ref="J159:J161"/>
-    <mergeCell ref="K159:K161"/>
-    <mergeCell ref="L159:L161"/>
-    <mergeCell ref="M159:M161"/>
-    <mergeCell ref="A163:A165"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="C163:C165"/>
-    <mergeCell ref="D163:D165"/>
-    <mergeCell ref="E163:E165"/>
-    <mergeCell ref="F163:F165"/>
-    <mergeCell ref="A169:A171"/>
-    <mergeCell ref="B169:B171"/>
-    <mergeCell ref="C169:C171"/>
-    <mergeCell ref="D169:D171"/>
-    <mergeCell ref="F169:F171"/>
-    <mergeCell ref="G169:G171"/>
-    <mergeCell ref="M163:M165"/>
-    <mergeCell ref="A166:A168"/>
-    <mergeCell ref="B166:B168"/>
-    <mergeCell ref="C166:C168"/>
-    <mergeCell ref="D166:D168"/>
-    <mergeCell ref="E166:E168"/>
-    <mergeCell ref="F166:F168"/>
-    <mergeCell ref="G166:G168"/>
-    <mergeCell ref="H166:H168"/>
-    <mergeCell ref="I166:I168"/>
-    <mergeCell ref="G163:G165"/>
-    <mergeCell ref="H163:H165"/>
-    <mergeCell ref="I163:I165"/>
-    <mergeCell ref="J163:J165"/>
-    <mergeCell ref="K163:K165"/>
-    <mergeCell ref="L163:L165"/>
-    <mergeCell ref="H169:H171"/>
-    <mergeCell ref="I169:I171"/>
-    <mergeCell ref="J169:J171"/>
-    <mergeCell ref="K169:K171"/>
-    <mergeCell ref="L169:L171"/>
-    <mergeCell ref="M169:M171"/>
-    <mergeCell ref="J166:J168"/>
-    <mergeCell ref="K166:K168"/>
-    <mergeCell ref="L166:L168"/>
-    <mergeCell ref="M166:M168"/>
+    <mergeCell ref="H134:H135"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="J134:J135"/>
+    <mergeCell ref="K134:K135"/>
+    <mergeCell ref="L134:L135"/>
+    <mergeCell ref="M134:M135"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="G134:G135"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed the database with a total of 215 Recipes!
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkish\Downloads\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF50B63-D54E-4EB5-8457-4B86CA72A00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714913DF-813E-4B11-B28A-80CD90992704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
   <sheets>
     <sheet name="RecipesTest" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="834">
   <si>
     <t>Name</t>
   </si>
@@ -2327,6 +2327,229 @@
   </si>
   <si>
     <t xml:space="preserve">Sasuke's Curse Mark Castella </t>
+  </si>
+  <si>
+    <t>Minecraft</t>
+  </si>
+  <si>
+    <t>2.25*teaspoons*Active Dry Yeast,1.5*cups*Warm Water,3.5*cups*Flour,2*tablespoons*Salted Butter (melted),1*teaspoon*Kosher Salt,0.5*cup*Salted Butter (melted for topping),1*bunch*Assorted Toppings</t>
+  </si>
+  <si>
+    <t>Inventory Bread</t>
+  </si>
+  <si>
+    <t>Hoglins and Lava</t>
+  </si>
+  <si>
+    <t>Dragon's Breath</t>
+  </si>
+  <si>
+    <t>Smelted Nuggets</t>
+  </si>
+  <si>
+    <t>This recipe takes the concept of monkey bread, a delicious pull-apart dish perfect for parties, and turns it into a colorful collection of edible Minecraft blocks, a reminder of the great things we can craft from humble components.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> These real-life puff pastry sausage herds , topped with poppy seeds and a Buffalo sauce–inspired lava.</t>
+  </si>
+  <si>
+    <t>It’s a multiuse condiment that enhances salad, meats, veggies, and breads.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Combine the yeast and ¼ cup warm water in the bowl of a stand mixer fitted with a dough hook. Let stand 10 minutes or until foamy.||2. Add the rest of the water, flour, butter, and kosher salt to the bowl. Mix with a dough hook attachment, slowly at first, then on medium speed once the flour is incorporated. Mix for 5 minutes or until a sticky dough forms. If you don’t have a mixer, mix the dough together by hand, then knead it on a floured surface for 5 minutes.||3. Move the dough into a large oiled bowl and cover with a damp towel. Let sit in a warm location for 1 hour, or until the dough has doubled in size.||4. While waiting for the dough to rise, prep your ingredients. Put each block’s seasoning mix on its own flat plate.||5. Transfer the dough to a floured surface, punch it down, and using a sharp knife or a pizza cutter, divide the dough into 32 separate cubes.||6. Dip each cube in melted butter (with the exception of the lava and moss stone variations), then roll in the seasonings of choice to create whatever block types you want. Place each cube in a greased 8-by-8-inch square pan so they’re lightly stacked on top of each other. Cover the pan with plastic wrap and let rise for 30 minutes or until doubled in size.||7. While waiting for the dough to rise, preheat your oven to 400 degrees Fahrenheit. Once risen, place the pan in the oven for 30 minutes or until the bread is golden brown.||8. Remove the pan from the oven and let cool for 5 minutes.||9. Take a spatula or butter knife and run it along the edges to loosen the bread, and remove. Serve with the top side up. The individual cubes will be stuck together into a larger block but can be pulled apart evenly.</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 425 degrees Fahrenheit and cover a baking sheet with parchment paper. Set aside.||2. Sprinkle flour over a flat surface and roll out the thawed puff pastry sheet to a 10-by-14-inch rectangle.||3. Using a sharp knife or a pizza cutter, cut the pastry into 24 equally sized rectangles. Place one sausage at the base of each pastry rectangle (long side of the rectangle up) and roll up the sausage in the pastry. Pinch the seam closed.||4. Whisk the egg and water together and brush the top of each puff pastry sausage. Sprinkle a small line of poppy seeds in the centre of each top.||5. Bake for 20 to 25 minutes or until the puff pastry is golden brown and flaky.||6. While baking, make the lava dip: Combine the hot sauce, butter, vinegar, Worcestershire sauce, cayenne pepper, garlic powder, and paprika in a saucepan over medium heat. Whisk continuously until the mixture starts to boil (about 3 minutes). Mix together the cornstarch and water in a small bowl and add the slurry into the saucepan. Reduce heat to medium-low, cover, and let simmer for 5 minutes or until sauce has thickened.||7. Stir, remove from heat, and let cool for 5 minutes before serving.||8. Once the hoglins have finished baking, place them on a platter with a small bowl of the lava dip on the side.</t>
+  </si>
+  <si>
+    <t>1. Place the vinegar, sugar, and salt in a small saucepan over medium heat and stir while cooking until the sugar and salt dissolve, about 1 minute.||2. Remove the saucepan from the heat and add the onion. Set aside to pickle for 1 hour.||3. Place the olive oil, lemon juice, garlic cloves, red pepper, and black pepper in a 10-ounce mason jar, then add the pickled onions and vinegar. Seal the jar and shake for 20 seconds or until emulsified. Refrigerate and shake quickly before using.</t>
+  </si>
+  <si>
+    <t>1. Heat oil on high in a large saucepan or Dutch oven until it reaches 375 degrees Fahrenheit. Adjust the stove’s heat to medium and monitor the temperature of the oil, keeping it consistently at 375 degrees Fahrenheit.||2. Mix together the flour, baking soda, salt, pepper, and garlic powder in a large bowl, then add the buttermilk and egg. Whisk together until fully combined.||3. Place the cheese curds in the batter mixture, fully coating the curds, and fish them out with a slotted spoon.||4. Place 8 to 10 of the cheese curds in the hot oil at a time, being careful not to crowd.||5. Fry for 1 minute, flipping over halfway through, then remove, placing on a paper towel–lined plate to drain and cool.||6. Bring the oil back to 375 degrees Fahrenheit and fry the next batch. Continue with the rest of the cheese curds.</t>
+  </si>
+  <si>
+    <t>2*tablespoons*Flour,1*packet*Frozen Puff Pastry Sheet (thawed),24*mini*Cocktail Sausages,1*null*Egg,1*tablespoon*Water,1*packet*Poppy Seeds,1*cup*Cayenne Hot Sauce,0.5*cup*Unsalted Butter,2*tablespoons*White Vinegar,0.5*teaspoon*Worcestershire Sauce,0.5*teaspoon*Cayenne Pepper,0.5*teaspoon*Garlic Powder,0.25*teaspoon*Paprika,1*tablespoon*Cornstarch,1*tablespoon*Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25*cup*Red Wine Vinegar,1*tablespoon*Sugar,0.75*teaspoon*Kosher Salt,0.25*null*Red Onion (sliced thin),0.3*cup*Extra Virgin OilveOil,0.25*cup*Lemon Juice,10*cloves*Garlic,025*teaspoon*Red Pepper Flakes,0.25*teaspoon*Black Pepper </t>
+  </si>
+  <si>
+    <t>18*ounces*Vegetable Oil,1*cup*Flour,1*teaspoon*Baking Soda,0.5*teaspoon*Black Pepper,0.5*teaspoon*Garlic Powder,1*cup*Buttermilk,1*null*Egg,1*pound*Cheese Curds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warped Forest Flatbread Pizza </t>
+  </si>
+  <si>
+    <t>28*ounce*Can of Whole Peeled Tomatoes (San Marzano if possible),0.5*teaspoon*Kosher Salt,0.25*cup*Olive Oil,1*dash*Red Pepper Flakes,1.5*cups*Flour,0.5*teaspoon*Salt,0.5*teaspoon*Dried Rosemary,0.5*cup*Water,1.5*tablespoons*Olive Oil (dough),1*sprinkle*Cornmeal,6*ounces*Whole Milk Mozzarella (low moisture and cut into half-inch cubes),1.5*tablespoons*Sun-dried Tomatoes,2*null*Cremini Mushrooms (sliced thin),0.25*cup*Baby Arugula,1*bowl*Parmesan (grated)</t>
+  </si>
+  <si>
+    <t>1. Pour the contents of the can of tomatoes into a bowl and crush the tomatoes by hand until a chunky sauce forms. Whisk in the salt and olive oil until the olive oil and tomato sauce are fully emulsified, and incorporate red pepper flakes if you’d like the sauce to be spicy. Refrigerate until you’re ready to use. (You’ll have some sauce left over after this recipe.|| For the Flatbread: 1. Preheat the oven as high as it will go (most likely 500 degrees Fahrenheit to 550 degrees Fahrenheit). Place a baking sheet in the oven while it preheats.||2. Combine the flour, salt, and rosemary in a large bowl.||3. Add the water and the olive oil, mixing with your hands until fully combined.||4. Move the dough to a floured surface and knead for 1 minute, until the dough is smooth and elastic. (Add more flour 1 tablespoon at a time if the dough is too sticky.)||5. Roll the dough into a long, flat oval (about 16 by 8 inches).||6. Using oven mitts, remove the baking sheet and sprinkle with cornmeal. Place the dough oval on the baking sheet and set back in the oven, baking for 5 to 7 minutes or until the edges are starting to turn golden brown, but it’s not fully cooked. (You’ll continue baking after adding the toppings.)||7. Remove from the oven. Place 3 quarters of a cup of sauce in the middle of the flatbread and use the back of a spoon to lightly spread it around the rest of the crust, leaving a half-inch border around the edge. Sprinkle the mozzarella evenly on top of the sauce and top with the sun-dried tomatoes and mushrooms. Brush the crust edges with olive oil.||8. Bake for an additional 6 minutes, or until the crust is brown and the cheese is melted and beginning to brown.||9. Remove the flatbread from the oven and onto a cutting board. Let sit for a few minutes, then top with arugula. Shake grated Parmesan, some red pepper flakes, and a dash of oregano on top.||10. Cut into squares to serve.</t>
+  </si>
+  <si>
+    <t>Chicken Jockey Sandwich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Here’s a satisfying pesto and bacon-covered chicken sandwich, inspired by the rare but unforgettable sight of a zombified piglin on a chicken</t>
+  </si>
+  <si>
+    <t>4*slices*Bacon (thick-cut),1*null*Chicken Breast (boneless and skinless),0.25*teaspoon*Salt,0.25*teaspoon*Pepper,2*slice*Provolone Cheese,2*null*Brioche Buns (split),2*tablespoons*Mayonnaise,2*tablespoons*Pesto,2*slices*Tomato,2*pieces*Lettuce</t>
+  </si>
+  <si>
+    <t>1. Place the bacon slices in a large skillet on medium-high heat and cook for 3 minutes on each side, or until bacon is crispy. Remove the bacon and place on a paper towel–lined plate, leaving the bacon grease in the skillet.||2. Cut the chicken breast in half lengthwise, cover with parchment paper, and pound with a mallet (or another heavy, blunt utensil, like a rolling pin) until both pieces are of even thickness, about half inch. Salt and pepper both sides of the breast pieces and place them in the large skillet on medium-high heat. Cook the chicken for 3 to 4 minutes on each side, or until chicken is cooked through. (The chicken should feel firm to the touch and have an internal temperature of 165 degrees Fahrenheit.)||3. In the last minute of cooking, add the provolone cheese to the top of each chicken breast piece and let melt.||4. Toast brioche buns, then spread a light layer of mayo on the inside of each bun.||5. Place the chicken on the bottom buns, then spread a layer of pesto on top of the melted cheese.||6. Top with 2 slices of bacon for each sandwich, then tomato, lettuce, and the top bun.</t>
+  </si>
+  <si>
+    <t>Farmland Smorgastarta</t>
+  </si>
+  <si>
+    <t>4*null*Eggs (hard-boiled and minced),0.3*cup*Mayonnaise,1*null*Green Onion (minced),0.5*tablespoon*Dijon Mustard,0.5*teaspoon*Lemon Juice,0.25*teaspoon*Paprika,1*cup*Rotisserie Chicken (chopped),0.25*cup*Mayonnaise (chicken salad),1*stalk*Celery (chopped),1*null*Green Onion (minced for the chicken salad),0.5*teaspoon*Dijon Mustard (chicken salad),0.5*teaspoon*Dill,0.25*teaspoon*Salt,1*dash*Pepper,6*ounces*Cream Cheese,0.6*cup*Sour Cream,0.25*cup*Mayonnaise (smorgastarta),0.5*teaspoon*Dill (smorgastarta),1*dash*Salt (smorgastarta),1*dash*Pepper (smorgastarta),10*slices*White Bread,1*null*Cucumber,1*null*Radish</t>
+  </si>
+  <si>
+    <t>1. To make the individual salads: For the egg salad combine the eggs, mayonnaise, green onion, dijon mustard, lemon juice and paprika in a bowl and refrigerate until ready to use. For the chicken salad combine the chicken, mayonnaise, celery, green onion, dijon mustard, dill, salt and pepper in a bowl.||2. To make the smörgåstårta: Combine the cream cheese, sour cream, mayonnaise, dill, salt, and pepper in a bowl and mix until smooth.||3. Cut the crusts off of the bread slices, then place 2 slices side by side on a serving plate. Top one slice with egg salad, spread evenly and place a slice of bread on top.||4. Top the other slice with chicken salad, spread evenly, and place a slice of bread on top.||5. Repeat, this time putting egg salad atop the chicken salad side and vice versa. Top with bread and continue alternating salads and bread slices until you have a rectangular cake that’s 5 slices of bread and salad high and 2 slices wide.||6. Frost the bread cake’s top and sides with the cream cheese mixture. Slice the cucumber and radish thinly with a mandoline or a sharp knife, then decorate the sides and top of the cake with the sliced vegetables. Refrigerate for at least 30 minutes. Cut and serve just like you would cake!</t>
+  </si>
+  <si>
+    <t>1. Mix all ingredients together and place in a jar.||2. When time to prep meat, sprinkle on 2 tablespoons per pound of meat or vegetables and rub it in with your hands, making sure to cover the meat or vegetables evenly. Let rest for at least 15 minutes, then cook the meat as you would otherwise.</t>
+  </si>
+  <si>
+    <t>Redstone Dust Rub</t>
+  </si>
+  <si>
+    <t>A spicy, smoky, and sweet flavor—perfect for chicken, ribs, or anything you want to put on a grill.</t>
+  </si>
+  <si>
+    <t>Decorate the outside to look like your farmland and favorite plants, then cut into delicious slices of satisfying, layered sandwiches.</t>
+  </si>
+  <si>
+    <t>A fast flatbread pizza. Mushrooms, sun-dried tomatoes, and arugula represent crimson fungus, crimson roots, and warped nylium.</t>
+  </si>
+  <si>
+    <t>Breaded, melted cheese</t>
+  </si>
+  <si>
+    <t>0.25*cup*Dark Bronw Sugar,2*tablespoons*Smoked Paprika,2*tablespoons*Kosher Salt,1*tablespoons*Garlic Powder,1*tablespoon*Chili Powder,2*teaspoons*Black Pepper,1*teaspoon*Onion Powder,1*teaspoon*Cayenne Pepper,1*teaspoon*Cumin</t>
+  </si>
+  <si>
+    <t>Buried Treasure Pie</t>
+  </si>
+  <si>
+    <t>Cut through the flaky crust of this “treasure chest,” and you’ll be rewarded with deliciously cooked salmon. And although it’s not the heart of the sea, the salmon is sitting on a bed of spinach, which is good for your heart.</t>
+  </si>
+  <si>
+    <t>2*tablespoons*Salted Butter,1*null*Yellow Onion,6*cups*Baby Spinach,2*cloves*Garlic (minced),0.6*cup*Cream Cheese,0.25*cup*Dried Bread crumbs,0.25*cup*Parmesan (grated),0.75*teaspoon*Kosher Salt,0.5*teaspoon*Black Pepper,2*tablespoon*Flour,2*sheets*Frozen Puff Pastry (thawed),4*null*6 ounce Salmon Fillets (skin removed),0.5*null*Lemon Juice ,1*null*Egg,1*tablespoon*Water</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 400 degrees Fahrenheit and line a baking sheet with parchment paper. Set aside.||2. Melt the butter in a large saucepan over medium heat and add the diced onion. Saute for 3 to 5 minutes or until the onions are soft and translucent.||3. Add the spinach and garlic and cook for 1 minute, or until the spinach begins to wilt. Add the cream cheese, and once it melts, add the bread crumbs, Parmesan, and a quarter teaspoon each of salt and pepper. Mix together and remove from heat.||4. Flour a cutting board, then unfold the pastry sheets and cut both sheets in half. Using a rolling pin, flatten each sheet to half its thickness. Season both sides of the salmon fillets with salt and pepper, then place one fillet, top side down, in the middle of each pastry sheet. Squeeze a small amount of lemon juice on each fillet.||5. Top the salmon with a quarter of the spinach mixture and spread so it covers the fillet evenly.||6. Fold up the edges of the puff pastry like you’re wrapping a present, then place the pastry packets on the parchment paper–covered baking sheet, seam side down.||7. Using a sharp knife, cut slits in the shape of an x in the middle of the pastry packets.||8. Make an egg wash by whisking the egg and water, then brush on the top of each pastry packet.||9. Bake for 30 minutes or until the pastry is golden and flaky.</t>
+  </si>
+  <si>
+    <t>Potion of Night Vision</t>
+  </si>
+  <si>
+    <t>The vitamins in this carrot cake–inspired smoothie improve your night vision</t>
+  </si>
+  <si>
+    <t>1*cup*Coconut Milk,0.5*cup*Frozen Carrots,1*null*Banana (frozen),0.25*cup*Vanilla Greek Yogurt,0.5*teaspoon*Vanilla Extract,0.25*teaspoon*Cinnamon,1*dash*Ginger,1*dash*Nutmeg</t>
+  </si>
+  <si>
+    <t>1. Place all ingredients in a blender and blend on high for 1 minute or until smooth.||2. Pour into a glass and top with another dash of nutmeg.</t>
+  </si>
+  <si>
+    <t>1. Muddle the blueberries and mint leaves at the bottom of a shaker.||2. Add ice, simple syrup, and lime juice, and shake until the shaker is frosted.||3. Strain into a glass with ice and pour the sparkling water on top.||4. Give a gentle stir and garnish with blueberries and mint on a skewer.</t>
+  </si>
+  <si>
+    <t>15*null*Blueberries,5*null*Mint Leaves (fresh),1*packet*Ice,1*ounce*Simple Syrup,1*ounce*Lime Juice,4*ounces*Sparkling Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The recipe uses blueberries instead of the namesake fruit and includes a bit of sparkling water to put a spring in your step—whether you want it there or not.</t>
+  </si>
+  <si>
+    <t>Chorus Fruit Spritzer</t>
+  </si>
+  <si>
+    <t>TNTea</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brew a cup of this sweet and cinnamony black tea</t>
+  </si>
+  <si>
+    <t>1*teaspoon*Black Tea,0.25*teaspoon*Sparkling Sugar,0.25*teaspoon*Popping Candy,1*dash*Cinnamon</t>
+  </si>
+  <si>
+    <t>1. Mix together all ingredients in a small bowl, then place in a tea sachet. (If making more than one serving at a time, multiply the ingredient list accordingly, then scoop 1 and half  teaspoons of the mixture into each sachet.)||2. Place the sachet in hot water and steep for 3 to 5 minutes or until your desired strength is achieved.</t>
+  </si>
+  <si>
+    <t>Creeper Cleanse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banish that creeper vibe from your mind with this green lemonade-like concoction, full of electrolytes, antioxidants, fruits, and veggies.</t>
+  </si>
+  <si>
+    <t>1*cup*Coconut Water,0.25*cup*Lemon Juice,1*cup*Packed Spinach,1*null*Green Apple (cored and sliced),1*stalk*Celery (trimmed and cut into 4 large pieces),1*small*Ginger Root Knob (peeled),1*tablespoon*Honey,5*null*Ice Cubes</t>
+  </si>
+  <si>
+    <t>1. Place all ingredients except for ice in a blender and blend for 2 minutes or until smooth.||2. Strain through a sieve and into an ice-filled glass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torch Shooter </t>
+  </si>
+  <si>
+    <t>7*large*Egg Yolks,0.6*cup*Sugar,3*cups*Heavy Whipping Cream,1*teaspoon*Vanilla Extract,0.5*cup*Semisweet Chocolate Chips,1*jug*Hot Water</t>
+  </si>
+  <si>
+    <t>1. Preheat the oven to 300 degrees Fahrenheit.||2. Whisk the egg yolks with half a cup of sugar until light and fluffy.||3. Heat cream in a large saucepan for 3 minutes or until bubbles start to form along the edges. Remove from heat.||4. Incorporate a quarter cup of the hot cream into the egg yolk mixture, then transfer the yolk mixture into the large saucepan with the rest of the cream. Add in the vanilla and stir.||5. Place a third of the mixture into a separate bowl and set aside. Add the chocolate chips to the remaining custard in the saucepan. Stir until fully melted and combined.||6. Pour the chocolate custard mixture into the dessert shooters, filling each shooter halfway.||7. Pour the vanilla custard slowly over the back of a spoon to layer on top of the chocolate. Fill until the shooters are 3 quarters full.||8. Place the shooters in a tall-rimmed baking dish and fill the dish with hot water at least halfway up the sides of the shooters.||9. Place in the oven and bake for 35 minutes or until the creme brulee is set but still jiggly. Remove the shooters from the pan and let cool at room temperature for 15 minutes.||10. Move to the fridge and let chill for at least 1 hour.||11. Sprinkle a teaspoon of sugar on the top of each shooter and torch the sugar using a culinary torch until it is fully melted and caramelized.</t>
+  </si>
+  <si>
+    <t>A chocolate-and-vanilla-layered creme brulee is topped with sugar and flambéed with fire</t>
+  </si>
+  <si>
+    <t>Blocks of Clay Fudge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Although these look just like clay blocks, they taste more like your favorite cookies and cream ice cream.</t>
+  </si>
+  <si>
+    <t>4*cups*cream-filled Sandwich Cookies,14*ounce*Can Sweetened Condensed Milk,0.125*teaspoon*Salt,18*ounces*White Chocolate Chips,1*teaspoon*Vanilla Extract</t>
+  </si>
+  <si>
+    <t>1. Place half of the cookies in a blender or food processor and process for 10 seconds or until they make a fine crumb. Add the other half and pulse until the second half is coarsely chopped. Set aside.||2. Line an 8-by-8-inch square pan with parchment or wax paper and set aside.||3. Place the sweetened condensed milk and salt in a medium saucepan over medium-low heat until it begins to simmer, stirring often. Adjust the heat to low and add the white chocolate chips and vanilla extract, stirring until just starting to melt. Turn off the heat and continue to stir until fully melted.||4. Once fully melted and combined, stir in the cookie crumbs.||5. Place the fudge mixture in the parchment paper–lined square pan and spread evenly.||6. Chill in the refrigerator for at least 2 hours or until firm.
+7. Cut the fudge into 64 squares, about half an inch each.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheep's Wool </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The pulled sugar makes thin strands reminiscent of wool, and much like the in-game sheep, you can dye this treat an assortment of colors.</t>
+  </si>
+  <si>
+    <t>1*cup*Water,5*drops*Food Colouring (of choice),2*drops*Flavouring (optional),2*cups*White Sugar,0.25*cup*Corn Starch,0.5*teaspoon*White Vinegar,1*cup*Cornstarch</t>
+  </si>
+  <si>
+    <t>1. Line a 9-by-9-inch baking dish with parchment paper and set aside.||2. Combine the sugar, honey, and water in a medium pot over high heat. Bring the mixture to a boil, stirring constantly.||3. Reduce the heat to medium-high and cook for 5 to 7 minutes, stirring often, until the mixture darkens and the candy thermometer reaches 300 degrees Fahrenheit.||4. Remove from heat and whisk in the baking soda. It will bubble up very quickly.||5. Pour the mixture into the baking dish, scraping it all out with a spatula. Slowly tilt the dish to even out the mixture if needed, but do not stir, or you will deflate the bubbles.||6. Let cool for 30 minutes or until the honey block has hardened. Cut into blocks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glazed Terracotta Cookies </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Some preplanning and rolling of various colored doughs will give you artful cookies that almost look too good to eat.</t>
+  </si>
+  <si>
+    <t>1*cup*Unsalted Butter,1*cup*Granulated Sugar,1*null*Egg,1*teaspoon*Vanilla,3*cups*Flour,2*teaspoons*Baking Powder,0.5*teaspoon*Kosher Salt,1*packet*Gel Food Colouring (of choice)</t>
+  </si>
+  <si>
+    <t>1. Mix the butter and sugar in a mixer until it is light and creamy.||2. Add in the egg and vanilla, mixing fully in between each addition.||3. Mix the flour, baking powder, and salt together in a separate bowl, then slowly add into the wet mixture until everything is fully mixed.||4. Divide the dough into separate small bowls, one for each color you want to include in your tile. You might want to sketch out the design of your tile to guide you through the next steps. Or improvise and see what happens!||5. Place a few drops of gel food coloring into each bowl and mix with the dough until it reaches your desired color. (You may want to wear gloves to prevent your hands from getting stained!)||6. Roll each batch of colored dough into a long cylinder. You’re going to stack them together to form a single, thicker cylinder; slices of the cylinder will become your tiles. Consult your sketch, if you have one, and stack the tubes of dough on top of each other lengthwise so the colors line up where you want them. Look at the end of tube to see what the cross section will look like.||7. If you want your tile to include a specific shape in the center, you can roll one of the colored dough batches flat and cut out shapes with a cookie cutter. Stack the shapes on top of each other. Roll the other dough batches into long cylinders and use them to fill in the spaces around the cutout stack, creating a log with the cutout shape inside.||8. With the colors arranged correctly, press the dough together and form everything into a single cylinder.||9. Take the full log of dough and flatten it on four sides, creating a squared column. Wrap with plastic wrap and refrigerate for at least 1 hour.||10. Preheat the oven to 350 degrees Fahrenheit and line two baking sheets with parchment paper.||11. Take the log from the refrigerator and slice it into half-inch tiles. Place them on the baking sheets. Bake for 8 to 10 minutes or until set and barely golden on the edges. Let cool on the baking sheets for 5 minutes, then transfer to a wire rack to cool completely.</t>
+  </si>
+  <si>
+    <t>Cocoa Chunk Cookies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> These are large treats with crispy edges, a gooey middle, and flakes of salty crunch to complement the sugar and chocolate—everything the perfect cookie should be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1*cup*Salted Butter,1*cup*Brown Sugar,0.5*cup*Sugar,2*null*Eggs,1*teaspoon*Vanilla,2.5*cups*Flour,1*teaspoon*Salt,0.75*teaspoon*Baking Soda,1.5*cups*Dark Chocolate Chunks,0.5*cup*Chopped Walnuts,1*dash*Flake Salt </t>
+  </si>
+  <si>
+    <t>1. Mix the butter in a mixer until it is light and creamy, then mix in both sugars.||2. Add in each egg one at a time, mixing in between each addition. Add the vanilla, and mix fully.||3. Mix the flour, salt, and baking soda together in a separate bowl, then slowly add into the wet mixture until everything is fully mixed.||4. Stir in the chocolate chunks. You may also add chopped walnuts.||5. Cover the top of the bowl of cookie dough with plastic wrap and refrigerate for 1 hour.||6. Preheat the oven to 375 degrees F, 15 minutes before removing the cookie dough from the fridge. Cover the cookie sheets with parchment paper.||7. Using the cookie scoop, drop round balls of cookie dough onto the cookie sheets, 2 inches apart from each other. Top each cookie with a small sprinkling of flake salt, lightly pressing into the tops.||8. Bake for 13 to 15 minutes, or until the edges of the cookies are light brown.|| 9. Cool for 5 minutes, then transfer to a wire rack to finish cooling.</t>
   </si>
 </sst>
 </file>
@@ -2794,10 +3017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
-  <dimension ref="A1:M197"/>
+  <dimension ref="A1:M584"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="95" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="C206" sqref="C206"/>
+    <sheetView tabSelected="1" topLeftCell="B214" zoomScale="95" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="E222" sqref="E222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7303,14 +7526,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A193" s="14" t="s">
         <v>741</v>
       </c>
       <c r="B193" s="14" t="s">
         <v>550</v>
       </c>
-      <c r="C193" s="13" t="s">
+      <c r="C193" s="1" t="s">
         <v>742</v>
       </c>
       <c r="D193" s="14" t="s">
@@ -7326,14 +7549,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A194" s="14" t="s">
         <v>745</v>
       </c>
       <c r="B194" s="14" t="s">
         <v>550</v>
       </c>
-      <c r="C194" s="13" t="s">
+      <c r="C194" s="1" t="s">
         <v>746</v>
       </c>
       <c r="D194" s="14" t="s">
@@ -7349,14 +7572,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
         <v>749</v>
       </c>
       <c r="B195" s="14" t="s">
         <v>550</v>
       </c>
-      <c r="C195" s="13" t="s">
+      <c r="C195" s="1" t="s">
         <v>750</v>
       </c>
       <c r="D195" s="14" t="s">
@@ -7372,7 +7595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A196" s="14" t="s">
         <v>753</v>
       </c>
@@ -7395,14 +7618,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A197" s="14" t="s">
         <v>760</v>
       </c>
       <c r="B197" s="14" t="s">
         <v>550</v>
       </c>
-      <c r="C197" s="13" t="s">
+      <c r="C197" s="1" t="s">
         <v>759</v>
       </c>
       <c r="D197" s="14" t="s">
@@ -7417,6 +7640,2838 @@
       <c r="G197" s="14" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="198" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A198" s="14" t="s">
+        <v>763</v>
+      </c>
+      <c r="B198" s="14" t="s">
+        <v>761</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D198" s="14" t="s">
+        <v>762</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="F198" s="14">
+        <v>150</v>
+      </c>
+      <c r="G198" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A199" s="14" t="s">
+        <v>764</v>
+      </c>
+      <c r="B199" s="14" t="s">
+        <v>761</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="F199" s="14">
+        <v>30</v>
+      </c>
+      <c r="G199" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A200" s="14" t="s">
+        <v>765</v>
+      </c>
+      <c r="B200" s="14" t="s">
+        <v>761</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="F200" s="14">
+        <v>65</v>
+      </c>
+      <c r="G200" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A201" s="14" t="s">
+        <v>766</v>
+      </c>
+      <c r="B201" s="14" t="s">
+        <v>761</v>
+      </c>
+      <c r="C201" s="12" t="s">
+        <v>792</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="F201" s="14">
+        <v>10</v>
+      </c>
+      <c r="G201" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="F202" s="1">
+        <v>25</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H202" s="12"/>
+      <c r="I202" s="12"/>
+    </row>
+    <row r="203" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="F203" s="1">
+        <v>20</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H203" s="12"/>
+      <c r="I203" s="12"/>
+    </row>
+    <row r="204" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F204" s="1">
+        <v>30</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H204" s="12"/>
+      <c r="I204" s="12"/>
+    </row>
+    <row r="205" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="F205" s="1">
+        <v>5</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H205" s="12"/>
+      <c r="I205" s="12"/>
+    </row>
+    <row r="206" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="F206" s="1">
+        <v>50</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H206" s="12"/>
+      <c r="I206" s="12"/>
+    </row>
+    <row r="207" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A207" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="F207" s="1">
+        <v>5</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H207" s="12"/>
+      <c r="I207" s="12"/>
+    </row>
+    <row r="208" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="F208" s="1">
+        <v>5</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H208" s="12"/>
+      <c r="I208" s="12"/>
+    </row>
+    <row r="209" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="F209" s="1">
+        <v>5</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H209" s="12"/>
+      <c r="I209" s="12"/>
+    </row>
+    <row r="210" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F210" s="1">
+        <v>5</v>
+      </c>
+      <c r="G210" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H210" s="12"/>
+      <c r="I210" s="12"/>
+    </row>
+    <row r="211" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A211" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="F211" s="1">
+        <v>130</v>
+      </c>
+      <c r="G211" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H211" s="12"/>
+      <c r="I211" s="12"/>
+    </row>
+    <row r="212" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="F212" s="1">
+        <v>10</v>
+      </c>
+      <c r="G212" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H212" s="12"/>
+      <c r="I212" s="12"/>
+    </row>
+    <row r="213" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="F213" s="1">
+        <v>150</v>
+      </c>
+      <c r="G213" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H213" s="12"/>
+      <c r="I213" s="12"/>
+    </row>
+    <row r="214" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="F214" s="1">
+        <v>100</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H214" s="12"/>
+      <c r="I214" s="12"/>
+    </row>
+    <row r="215" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="F215" s="1">
+        <v>90</v>
+      </c>
+      <c r="G215" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H215" s="12"/>
+      <c r="I215" s="12"/>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A216" s="1"/>
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="1"/>
+      <c r="F216" s="1"/>
+      <c r="G216" s="1"/>
+      <c r="H216" s="12"/>
+      <c r="I216" s="12"/>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1"/>
+      <c r="D217" s="1"/>
+      <c r="F217" s="1"/>
+      <c r="G217" s="1"/>
+      <c r="H217" s="12"/>
+      <c r="I217" s="12"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A218" s="1"/>
+      <c r="B218" s="1"/>
+      <c r="C218" s="1"/>
+      <c r="D218" s="1"/>
+      <c r="F218" s="1"/>
+      <c r="G218" s="1"/>
+      <c r="H218" s="12"/>
+      <c r="I218" s="12"/>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A219" s="1"/>
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="1"/>
+      <c r="F219" s="1"/>
+      <c r="G219" s="1"/>
+      <c r="H219" s="12"/>
+      <c r="I219" s="12"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="F220" s="1"/>
+      <c r="G220" s="1"/>
+      <c r="H220" s="12"/>
+      <c r="I220" s="12"/>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
+      <c r="D221" s="1"/>
+      <c r="F221" s="1"/>
+      <c r="G221" s="1"/>
+      <c r="H221" s="12"/>
+      <c r="I221" s="12"/>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A222" s="1"/>
+      <c r="B222" s="1"/>
+      <c r="C222" s="1"/>
+      <c r="D222" s="1"/>
+      <c r="F222" s="1"/>
+      <c r="G222" s="1"/>
+      <c r="H222" s="12"/>
+      <c r="I222" s="12"/>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="1"/>
+      <c r="F223" s="1"/>
+      <c r="G223" s="1"/>
+      <c r="H223" s="12"/>
+      <c r="I223" s="12"/>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A224" s="1"/>
+      <c r="B224" s="1"/>
+      <c r="C224" s="1"/>
+      <c r="D224" s="1"/>
+      <c r="F224" s="1"/>
+      <c r="G224" s="1"/>
+      <c r="H224" s="12"/>
+      <c r="I224" s="12"/>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A225" s="1"/>
+      <c r="B225" s="1"/>
+      <c r="C225" s="1"/>
+      <c r="D225" s="1"/>
+      <c r="F225" s="1"/>
+      <c r="G225" s="1"/>
+      <c r="H225" s="12"/>
+      <c r="I225" s="12"/>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A226" s="1"/>
+      <c r="B226" s="1"/>
+      <c r="C226" s="1"/>
+      <c r="D226" s="1"/>
+      <c r="F226" s="1"/>
+      <c r="G226" s="1"/>
+      <c r="H226" s="12"/>
+      <c r="I226" s="12"/>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A227" s="1"/>
+      <c r="B227" s="1"/>
+      <c r="C227" s="1"/>
+      <c r="D227" s="1"/>
+      <c r="F227" s="1"/>
+      <c r="G227" s="1"/>
+      <c r="H227" s="12"/>
+      <c r="I227" s="12"/>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A228" s="1"/>
+      <c r="B228" s="1"/>
+      <c r="C228" s="1"/>
+      <c r="D228" s="1"/>
+      <c r="F228" s="1"/>
+      <c r="G228" s="1"/>
+      <c r="H228" s="12"/>
+      <c r="I228" s="12"/>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A229" s="1"/>
+      <c r="B229" s="1"/>
+      <c r="C229" s="1"/>
+      <c r="D229" s="1"/>
+      <c r="F229" s="1"/>
+      <c r="G229" s="1"/>
+      <c r="H229" s="12"/>
+      <c r="I229" s="12"/>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A230" s="1"/>
+      <c r="B230" s="1"/>
+      <c r="C230" s="1"/>
+      <c r="D230" s="1"/>
+      <c r="F230" s="1"/>
+      <c r="G230" s="1"/>
+      <c r="H230" s="12"/>
+      <c r="I230" s="12"/>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A231" s="1"/>
+      <c r="B231" s="1"/>
+      <c r="C231" s="1"/>
+      <c r="D231" s="1"/>
+      <c r="F231" s="1"/>
+      <c r="G231" s="1"/>
+      <c r="H231" s="12"/>
+      <c r="I231" s="12"/>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A232" s="1"/>
+      <c r="B232" s="1"/>
+      <c r="C232" s="1"/>
+      <c r="D232" s="1"/>
+      <c r="F232" s="1"/>
+      <c r="G232" s="1"/>
+      <c r="H232" s="12"/>
+      <c r="I232" s="12"/>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A233" s="1"/>
+      <c r="B233" s="1"/>
+      <c r="C233" s="1"/>
+      <c r="D233" s="1"/>
+      <c r="F233" s="1"/>
+      <c r="G233" s="1"/>
+      <c r="H233" s="12"/>
+      <c r="I233" s="12"/>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A234" s="1"/>
+      <c r="B234" s="1"/>
+      <c r="C234" s="1"/>
+      <c r="D234" s="1"/>
+      <c r="F234" s="1"/>
+      <c r="G234" s="1"/>
+      <c r="H234" s="12"/>
+      <c r="I234" s="12"/>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A235" s="1"/>
+      <c r="B235" s="1"/>
+      <c r="C235" s="1"/>
+      <c r="D235" s="1"/>
+      <c r="F235" s="1"/>
+      <c r="G235" s="1"/>
+      <c r="H235" s="12"/>
+      <c r="I235" s="12"/>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A236" s="1"/>
+      <c r="B236" s="1"/>
+      <c r="C236" s="1"/>
+      <c r="D236" s="1"/>
+      <c r="F236" s="1"/>
+      <c r="G236" s="1"/>
+      <c r="H236" s="12"/>
+      <c r="I236" s="12"/>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A237" s="1"/>
+      <c r="B237" s="1"/>
+      <c r="C237" s="1"/>
+      <c r="D237" s="1"/>
+      <c r="F237" s="1"/>
+      <c r="G237" s="1"/>
+      <c r="H237" s="12"/>
+      <c r="I237" s="12"/>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A238" s="1"/>
+      <c r="B238" s="1"/>
+      <c r="C238" s="1"/>
+      <c r="D238" s="1"/>
+      <c r="F238" s="1"/>
+      <c r="G238" s="1"/>
+      <c r="H238" s="12"/>
+      <c r="I238" s="12"/>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A239" s="1"/>
+      <c r="B239" s="1"/>
+      <c r="C239" s="1"/>
+      <c r="D239" s="1"/>
+      <c r="F239" s="1"/>
+      <c r="G239" s="1"/>
+      <c r="H239" s="12"/>
+      <c r="I239" s="12"/>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A240" s="1"/>
+      <c r="B240" s="1"/>
+      <c r="C240" s="1"/>
+      <c r="D240" s="1"/>
+      <c r="F240" s="1"/>
+      <c r="G240" s="1"/>
+      <c r="H240" s="12"/>
+      <c r="I240" s="12"/>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A241" s="1"/>
+      <c r="B241" s="1"/>
+      <c r="C241" s="1"/>
+      <c r="D241" s="1"/>
+      <c r="F241" s="1"/>
+      <c r="G241" s="1"/>
+      <c r="H241" s="12"/>
+      <c r="I241" s="12"/>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="1"/>
+      <c r="F242" s="1"/>
+      <c r="G242" s="1"/>
+      <c r="H242" s="12"/>
+      <c r="I242" s="12"/>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
+      <c r="C243" s="1"/>
+      <c r="D243" s="1"/>
+      <c r="F243" s="1"/>
+      <c r="G243" s="1"/>
+      <c r="H243" s="12"/>
+      <c r="I243" s="12"/>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="1"/>
+      <c r="F244" s="1"/>
+      <c r="G244" s="1"/>
+      <c r="H244" s="12"/>
+      <c r="I244" s="12"/>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="1"/>
+      <c r="F245" s="1"/>
+      <c r="G245" s="1"/>
+      <c r="H245" s="12"/>
+      <c r="I245" s="12"/>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A246" s="1"/>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
+      <c r="D246" s="1"/>
+      <c r="F246" s="13"/>
+      <c r="G246" s="13"/>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
+      <c r="D247" s="1"/>
+      <c r="F247" s="13"/>
+      <c r="G247" s="13"/>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="1"/>
+      <c r="F248" s="13"/>
+      <c r="G248" s="13"/>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="1"/>
+      <c r="F249" s="13"/>
+      <c r="G249" s="13"/>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="1"/>
+      <c r="F250" s="13"/>
+      <c r="G250" s="13"/>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A251" s="1"/>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="1"/>
+      <c r="F251" s="13"/>
+      <c r="G251" s="13"/>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A252" s="1"/>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="1"/>
+      <c r="F252" s="13"/>
+      <c r="G252" s="13"/>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A253" s="1"/>
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
+      <c r="D253" s="1"/>
+      <c r="F253" s="13"/>
+      <c r="G253" s="13"/>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A254" s="1"/>
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
+      <c r="D254" s="1"/>
+      <c r="F254" s="13"/>
+      <c r="G254" s="13"/>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A255" s="1"/>
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
+      <c r="D255" s="1"/>
+      <c r="F255" s="13"/>
+      <c r="G255" s="13"/>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A256" s="1"/>
+      <c r="B256" s="1"/>
+      <c r="C256" s="1"/>
+      <c r="D256" s="1"/>
+      <c r="F256" s="13"/>
+      <c r="G256" s="13"/>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A257" s="1"/>
+      <c r="B257" s="1"/>
+      <c r="C257" s="1"/>
+      <c r="D257" s="1"/>
+      <c r="F257" s="13"/>
+      <c r="G257" s="13"/>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A258" s="1"/>
+      <c r="B258" s="1"/>
+      <c r="C258" s="1"/>
+      <c r="D258" s="1"/>
+      <c r="F258" s="13"/>
+      <c r="G258" s="13"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A259" s="1"/>
+      <c r="B259" s="1"/>
+      <c r="C259" s="1"/>
+      <c r="D259" s="1"/>
+      <c r="F259" s="13"/>
+      <c r="G259" s="13"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A260" s="1"/>
+      <c r="B260" s="1"/>
+      <c r="C260" s="1"/>
+      <c r="D260" s="1"/>
+      <c r="F260" s="13"/>
+      <c r="G260" s="13"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A261" s="1"/>
+      <c r="B261" s="1"/>
+      <c r="C261" s="1"/>
+      <c r="D261" s="1"/>
+      <c r="F261" s="13"/>
+      <c r="G261" s="13"/>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A262" s="1"/>
+      <c r="B262" s="1"/>
+      <c r="C262" s="1"/>
+      <c r="D262" s="1"/>
+      <c r="F262" s="13"/>
+      <c r="G262" s="13"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A263" s="1"/>
+      <c r="B263" s="1"/>
+      <c r="C263" s="1"/>
+      <c r="D263" s="1"/>
+      <c r="F263" s="13"/>
+      <c r="G263" s="13"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A264" s="1"/>
+      <c r="B264" s="1"/>
+      <c r="C264" s="1"/>
+      <c r="D264" s="1"/>
+      <c r="F264" s="13"/>
+      <c r="G264" s="13"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A265" s="1"/>
+      <c r="B265" s="1"/>
+      <c r="C265" s="1"/>
+      <c r="D265" s="1"/>
+      <c r="F265" s="13"/>
+      <c r="G265" s="13"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A266" s="1"/>
+      <c r="B266" s="1"/>
+      <c r="C266" s="1"/>
+      <c r="D266" s="1"/>
+      <c r="F266" s="13"/>
+      <c r="G266" s="13"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A267" s="1"/>
+      <c r="B267" s="1"/>
+      <c r="C267" s="1"/>
+      <c r="D267" s="1"/>
+      <c r="F267" s="13"/>
+      <c r="G267" s="13"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A268" s="1"/>
+      <c r="B268" s="1"/>
+      <c r="C268" s="1"/>
+      <c r="D268" s="1"/>
+      <c r="F268" s="13"/>
+      <c r="G268" s="13"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A269" s="1"/>
+      <c r="B269" s="1"/>
+      <c r="C269" s="1"/>
+      <c r="D269" s="1"/>
+      <c r="F269" s="13"/>
+      <c r="G269" s="13"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A270" s="1"/>
+      <c r="B270" s="1"/>
+      <c r="C270" s="1"/>
+      <c r="D270" s="1"/>
+      <c r="F270" s="13"/>
+      <c r="G270" s="13"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A271" s="1"/>
+      <c r="B271" s="1"/>
+      <c r="C271" s="1"/>
+      <c r="D271" s="1"/>
+      <c r="F271" s="13"/>
+      <c r="G271" s="13"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A272" s="1"/>
+      <c r="B272" s="1"/>
+      <c r="C272" s="1"/>
+      <c r="D272" s="1"/>
+      <c r="F272" s="13"/>
+      <c r="G272" s="13"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A273" s="1"/>
+      <c r="B273" s="1"/>
+      <c r="C273" s="1"/>
+      <c r="D273" s="1"/>
+      <c r="F273" s="13"/>
+      <c r="G273" s="13"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A274" s="12"/>
+      <c r="B274" s="12"/>
+      <c r="C274" s="12"/>
+      <c r="D274" s="12"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A275" s="12"/>
+      <c r="B275" s="12"/>
+      <c r="C275" s="12"/>
+      <c r="D275" s="12"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A276" s="12"/>
+      <c r="B276" s="12"/>
+      <c r="C276" s="12"/>
+      <c r="D276" s="12"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A277" s="12"/>
+      <c r="B277" s="12"/>
+      <c r="C277" s="12"/>
+      <c r="D277" s="12"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A278" s="12"/>
+      <c r="B278" s="12"/>
+      <c r="C278" s="12"/>
+      <c r="D278" s="12"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A279" s="12"/>
+      <c r="B279" s="12"/>
+      <c r="C279" s="12"/>
+      <c r="D279" s="12"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A280" s="12"/>
+      <c r="B280" s="12"/>
+      <c r="C280" s="12"/>
+      <c r="D280" s="12"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A281" s="12"/>
+      <c r="B281" s="12"/>
+      <c r="C281" s="12"/>
+      <c r="D281" s="12"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A282" s="12"/>
+      <c r="B282" s="12"/>
+      <c r="C282" s="12"/>
+      <c r="D282" s="12"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A283" s="12"/>
+      <c r="B283" s="12"/>
+      <c r="C283" s="12"/>
+      <c r="D283" s="12"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A284" s="12"/>
+      <c r="B284" s="12"/>
+      <c r="C284" s="12"/>
+      <c r="D284" s="12"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A285" s="12"/>
+      <c r="B285" s="12"/>
+      <c r="C285" s="12"/>
+      <c r="D285" s="12"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A286" s="12"/>
+      <c r="B286" s="12"/>
+      <c r="C286" s="12"/>
+      <c r="D286" s="12"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A287" s="12"/>
+      <c r="B287" s="12"/>
+      <c r="C287" s="12"/>
+      <c r="D287" s="12"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A288" s="12"/>
+      <c r="B288" s="12"/>
+      <c r="C288" s="12"/>
+      <c r="D288" s="12"/>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A289" s="12"/>
+      <c r="B289" s="12"/>
+      <c r="C289" s="12"/>
+      <c r="D289" s="12"/>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A290" s="12"/>
+      <c r="B290" s="12"/>
+      <c r="C290" s="12"/>
+      <c r="D290" s="12"/>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A291" s="12"/>
+      <c r="B291" s="12"/>
+      <c r="C291" s="12"/>
+      <c r="D291" s="12"/>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A292" s="12"/>
+      <c r="B292" s="12"/>
+      <c r="C292" s="12"/>
+      <c r="D292" s="12"/>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A293" s="12"/>
+      <c r="B293" s="12"/>
+      <c r="C293" s="12"/>
+      <c r="D293" s="12"/>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A294" s="12"/>
+      <c r="B294" s="12"/>
+      <c r="C294" s="12"/>
+      <c r="D294" s="12"/>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A295" s="12"/>
+      <c r="B295" s="12"/>
+      <c r="C295" s="12"/>
+      <c r="D295" s="12"/>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A296" s="12"/>
+      <c r="B296" s="12"/>
+      <c r="C296" s="12"/>
+      <c r="D296" s="12"/>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A297" s="12"/>
+      <c r="B297" s="12"/>
+      <c r="C297" s="12"/>
+      <c r="D297" s="12"/>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A298" s="12"/>
+      <c r="B298" s="12"/>
+      <c r="C298" s="12"/>
+      <c r="D298" s="12"/>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A299" s="12"/>
+      <c r="B299" s="12"/>
+      <c r="C299" s="12"/>
+      <c r="D299" s="12"/>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A300" s="12"/>
+      <c r="B300" s="12"/>
+      <c r="C300" s="12"/>
+      <c r="D300" s="12"/>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A301" s="12"/>
+      <c r="B301" s="12"/>
+      <c r="C301" s="12"/>
+      <c r="D301" s="12"/>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A302" s="12"/>
+      <c r="B302" s="12"/>
+      <c r="C302" s="12"/>
+      <c r="D302" s="12"/>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A303" s="12"/>
+      <c r="B303" s="12"/>
+      <c r="C303" s="12"/>
+      <c r="D303" s="12"/>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A304" s="12"/>
+      <c r="B304" s="12"/>
+      <c r="C304" s="12"/>
+      <c r="D304" s="12"/>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A305" s="12"/>
+      <c r="B305" s="12"/>
+      <c r="C305" s="12"/>
+      <c r="D305" s="12"/>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A306" s="12"/>
+      <c r="B306" s="12"/>
+      <c r="C306" s="12"/>
+      <c r="D306" s="12"/>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A307" s="12"/>
+      <c r="B307" s="12"/>
+      <c r="C307" s="12"/>
+      <c r="D307" s="12"/>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A308" s="12"/>
+      <c r="B308" s="12"/>
+      <c r="C308" s="12"/>
+      <c r="D308" s="12"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A309" s="12"/>
+      <c r="B309" s="12"/>
+      <c r="C309" s="12"/>
+      <c r="D309" s="12"/>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A310" s="12"/>
+      <c r="B310" s="12"/>
+      <c r="C310" s="12"/>
+      <c r="D310" s="12"/>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A311" s="12"/>
+      <c r="B311" s="12"/>
+      <c r="C311" s="12"/>
+      <c r="D311" s="12"/>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A312" s="12"/>
+      <c r="B312" s="12"/>
+      <c r="C312" s="12"/>
+      <c r="D312" s="12"/>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A313" s="12"/>
+      <c r="B313" s="12"/>
+      <c r="C313" s="12"/>
+      <c r="D313" s="12"/>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A314" s="12"/>
+      <c r="B314" s="12"/>
+      <c r="C314" s="12"/>
+      <c r="D314" s="12"/>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A315" s="12"/>
+      <c r="B315" s="12"/>
+      <c r="C315" s="12"/>
+      <c r="D315" s="12"/>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A316" s="12"/>
+      <c r="B316" s="12"/>
+      <c r="C316" s="12"/>
+      <c r="D316" s="12"/>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A317" s="12"/>
+      <c r="B317" s="12"/>
+      <c r="C317" s="12"/>
+      <c r="D317" s="12"/>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A318" s="12"/>
+      <c r="B318" s="12"/>
+      <c r="C318" s="12"/>
+      <c r="D318" s="12"/>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A319" s="12"/>
+      <c r="B319" s="12"/>
+      <c r="C319" s="12"/>
+      <c r="D319" s="12"/>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A320" s="12"/>
+      <c r="B320" s="12"/>
+      <c r="C320" s="12"/>
+      <c r="D320" s="12"/>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A321" s="12"/>
+      <c r="B321" s="12"/>
+      <c r="C321" s="12"/>
+      <c r="D321" s="12"/>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A322" s="12"/>
+      <c r="B322" s="12"/>
+      <c r="C322" s="12"/>
+      <c r="D322" s="12"/>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A323" s="12"/>
+      <c r="B323" s="12"/>
+      <c r="C323" s="12"/>
+      <c r="D323" s="12"/>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A324" s="12"/>
+      <c r="B324" s="12"/>
+      <c r="C324" s="12"/>
+      <c r="D324" s="12"/>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A325" s="12"/>
+      <c r="B325" s="12"/>
+      <c r="C325" s="12"/>
+      <c r="D325" s="12"/>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A326" s="12"/>
+      <c r="B326" s="12"/>
+      <c r="C326" s="12"/>
+      <c r="D326" s="12"/>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A327" s="12"/>
+      <c r="B327" s="12"/>
+      <c r="C327" s="12"/>
+      <c r="D327" s="12"/>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A328" s="12"/>
+      <c r="B328" s="12"/>
+      <c r="C328" s="12"/>
+      <c r="D328" s="12"/>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A329" s="12"/>
+      <c r="B329" s="12"/>
+      <c r="C329" s="12"/>
+      <c r="D329" s="12"/>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A330" s="12"/>
+      <c r="B330" s="12"/>
+      <c r="C330" s="12"/>
+      <c r="D330" s="12"/>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A331" s="12"/>
+      <c r="B331" s="12"/>
+      <c r="C331" s="12"/>
+      <c r="D331" s="12"/>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A332" s="12"/>
+      <c r="B332" s="12"/>
+      <c r="C332" s="12"/>
+      <c r="D332" s="12"/>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A333" s="12"/>
+      <c r="B333" s="12"/>
+      <c r="C333" s="12"/>
+      <c r="D333" s="12"/>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A334" s="12"/>
+      <c r="B334" s="12"/>
+      <c r="C334" s="12"/>
+      <c r="D334" s="12"/>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A335" s="12"/>
+      <c r="B335" s="12"/>
+      <c r="C335" s="12"/>
+      <c r="D335" s="12"/>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A336" s="12"/>
+      <c r="B336" s="12"/>
+      <c r="C336" s="12"/>
+      <c r="D336" s="12"/>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A337" s="12"/>
+      <c r="B337" s="12"/>
+      <c r="C337" s="12"/>
+      <c r="D337" s="12"/>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A338" s="12"/>
+      <c r="B338" s="12"/>
+      <c r="C338" s="12"/>
+      <c r="D338" s="12"/>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A339" s="12"/>
+      <c r="B339" s="12"/>
+      <c r="C339" s="12"/>
+      <c r="D339" s="12"/>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A340" s="12"/>
+      <c r="B340" s="12"/>
+      <c r="C340" s="12"/>
+      <c r="D340" s="12"/>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A341" s="12"/>
+      <c r="B341" s="12"/>
+      <c r="C341" s="12"/>
+      <c r="D341" s="12"/>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A342" s="12"/>
+      <c r="B342" s="12"/>
+      <c r="C342" s="12"/>
+      <c r="D342" s="12"/>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A343" s="12"/>
+      <c r="B343" s="12"/>
+      <c r="C343" s="12"/>
+      <c r="D343" s="12"/>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A344" s="12"/>
+      <c r="B344" s="12"/>
+      <c r="C344" s="12"/>
+      <c r="D344" s="12"/>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A345" s="12"/>
+      <c r="B345" s="12"/>
+      <c r="C345" s="12"/>
+      <c r="D345" s="12"/>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A346" s="12"/>
+      <c r="B346" s="12"/>
+      <c r="C346" s="12"/>
+      <c r="D346" s="12"/>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A347" s="12"/>
+      <c r="B347" s="12"/>
+      <c r="C347" s="12"/>
+      <c r="D347" s="12"/>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A348" s="12"/>
+      <c r="B348" s="12"/>
+      <c r="C348" s="12"/>
+      <c r="D348" s="12"/>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A349" s="12"/>
+      <c r="B349" s="12"/>
+      <c r="C349" s="12"/>
+      <c r="D349" s="12"/>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A350" s="12"/>
+      <c r="B350" s="12"/>
+      <c r="C350" s="12"/>
+      <c r="D350" s="12"/>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A351" s="12"/>
+      <c r="B351" s="12"/>
+      <c r="C351" s="12"/>
+      <c r="D351" s="12"/>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A352" s="12"/>
+      <c r="B352" s="12"/>
+      <c r="C352" s="12"/>
+      <c r="D352" s="12"/>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A353" s="12"/>
+      <c r="B353" s="12"/>
+      <c r="C353" s="12"/>
+      <c r="D353" s="12"/>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A354" s="12"/>
+      <c r="B354" s="12"/>
+      <c r="C354" s="12"/>
+      <c r="D354" s="12"/>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A355" s="12"/>
+      <c r="B355" s="12"/>
+      <c r="C355" s="12"/>
+      <c r="D355" s="12"/>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A356" s="12"/>
+      <c r="B356" s="12"/>
+      <c r="C356" s="12"/>
+      <c r="D356" s="12"/>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A357" s="12"/>
+      <c r="B357" s="12"/>
+      <c r="C357" s="12"/>
+      <c r="D357" s="12"/>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A358" s="12"/>
+      <c r="B358" s="12"/>
+      <c r="C358" s="12"/>
+      <c r="D358" s="12"/>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A359" s="12"/>
+      <c r="B359" s="12"/>
+      <c r="C359" s="12"/>
+      <c r="D359" s="12"/>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A360" s="12"/>
+      <c r="B360" s="12"/>
+      <c r="C360" s="12"/>
+      <c r="D360" s="12"/>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A361" s="12"/>
+      <c r="B361" s="12"/>
+      <c r="C361" s="12"/>
+      <c r="D361" s="12"/>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A362" s="12"/>
+      <c r="B362" s="12"/>
+      <c r="C362" s="12"/>
+      <c r="D362" s="12"/>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A363" s="12"/>
+      <c r="B363" s="12"/>
+      <c r="C363" s="12"/>
+      <c r="D363" s="12"/>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A364" s="12"/>
+      <c r="B364" s="12"/>
+      <c r="C364" s="12"/>
+      <c r="D364" s="12"/>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A365" s="12"/>
+      <c r="B365" s="12"/>
+      <c r="C365" s="12"/>
+      <c r="D365" s="12"/>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A366" s="12"/>
+      <c r="B366" s="12"/>
+      <c r="C366" s="12"/>
+      <c r="D366" s="12"/>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A367" s="12"/>
+      <c r="B367" s="12"/>
+      <c r="C367" s="12"/>
+      <c r="D367" s="12"/>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A368" s="12"/>
+      <c r="B368" s="12"/>
+      <c r="C368" s="12"/>
+      <c r="D368" s="12"/>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A369" s="12"/>
+      <c r="B369" s="12"/>
+      <c r="C369" s="12"/>
+      <c r="D369" s="12"/>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A370" s="12"/>
+      <c r="B370" s="12"/>
+      <c r="C370" s="12"/>
+      <c r="D370" s="12"/>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A371" s="12"/>
+      <c r="B371" s="12"/>
+      <c r="C371" s="12"/>
+      <c r="D371" s="12"/>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A372" s="12"/>
+      <c r="B372" s="12"/>
+      <c r="C372" s="12"/>
+      <c r="D372" s="12"/>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A373" s="12"/>
+      <c r="B373" s="12"/>
+      <c r="C373" s="12"/>
+      <c r="D373" s="12"/>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A374" s="12"/>
+      <c r="B374" s="12"/>
+      <c r="C374" s="12"/>
+      <c r="D374" s="12"/>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A375" s="12"/>
+      <c r="B375" s="12"/>
+      <c r="C375" s="12"/>
+      <c r="D375" s="12"/>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A376" s="12"/>
+      <c r="B376" s="12"/>
+      <c r="C376" s="12"/>
+      <c r="D376" s="12"/>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A377" s="12"/>
+      <c r="B377" s="12"/>
+      <c r="C377" s="12"/>
+      <c r="D377" s="12"/>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A378" s="12"/>
+      <c r="B378" s="12"/>
+      <c r="C378" s="12"/>
+      <c r="D378" s="12"/>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A379" s="12"/>
+      <c r="B379" s="12"/>
+      <c r="C379" s="12"/>
+      <c r="D379" s="12"/>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A380" s="12"/>
+      <c r="B380" s="12"/>
+      <c r="C380" s="12"/>
+      <c r="D380" s="12"/>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A381" s="12"/>
+      <c r="B381" s="12"/>
+      <c r="C381" s="12"/>
+      <c r="D381" s="12"/>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A382" s="12"/>
+      <c r="B382" s="12"/>
+      <c r="C382" s="12"/>
+      <c r="D382" s="12"/>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A383" s="12"/>
+      <c r="B383" s="12"/>
+      <c r="C383" s="12"/>
+      <c r="D383" s="12"/>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A384" s="12"/>
+      <c r="B384" s="12"/>
+      <c r="C384" s="12"/>
+      <c r="D384" s="12"/>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A385" s="12"/>
+      <c r="B385" s="12"/>
+      <c r="C385" s="12"/>
+      <c r="D385" s="12"/>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A386" s="12"/>
+      <c r="B386" s="12"/>
+      <c r="C386" s="12"/>
+      <c r="D386" s="12"/>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A387" s="12"/>
+      <c r="B387" s="12"/>
+      <c r="C387" s="12"/>
+      <c r="D387" s="12"/>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A388" s="12"/>
+      <c r="B388" s="12"/>
+      <c r="C388" s="12"/>
+      <c r="D388" s="12"/>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A389" s="12"/>
+      <c r="B389" s="12"/>
+      <c r="C389" s="12"/>
+      <c r="D389" s="12"/>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A390" s="12"/>
+      <c r="B390" s="12"/>
+      <c r="C390" s="12"/>
+      <c r="D390" s="12"/>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A391" s="12"/>
+      <c r="B391" s="12"/>
+      <c r="C391" s="12"/>
+      <c r="D391" s="12"/>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A392" s="12"/>
+      <c r="B392" s="12"/>
+      <c r="C392" s="12"/>
+      <c r="D392" s="12"/>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A393" s="12"/>
+      <c r="B393" s="12"/>
+      <c r="C393" s="12"/>
+      <c r="D393" s="12"/>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A394" s="12"/>
+      <c r="B394" s="12"/>
+      <c r="C394" s="12"/>
+      <c r="D394" s="12"/>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A395" s="12"/>
+      <c r="B395" s="12"/>
+      <c r="C395" s="12"/>
+      <c r="D395" s="12"/>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A396" s="12"/>
+      <c r="B396" s="12"/>
+      <c r="C396" s="12"/>
+      <c r="D396" s="12"/>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A397" s="12"/>
+      <c r="B397" s="12"/>
+      <c r="C397" s="12"/>
+      <c r="D397" s="12"/>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A398" s="12"/>
+      <c r="B398" s="12"/>
+      <c r="C398" s="12"/>
+      <c r="D398" s="12"/>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A399" s="12"/>
+      <c r="B399" s="12"/>
+      <c r="C399" s="12"/>
+      <c r="D399" s="12"/>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A400" s="12"/>
+      <c r="B400" s="12"/>
+      <c r="C400" s="12"/>
+      <c r="D400" s="12"/>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A401" s="12"/>
+      <c r="B401" s="12"/>
+      <c r="C401" s="12"/>
+      <c r="D401" s="12"/>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A402" s="12"/>
+      <c r="B402" s="12"/>
+      <c r="C402" s="12"/>
+      <c r="D402" s="12"/>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A403" s="12"/>
+      <c r="B403" s="12"/>
+      <c r="C403" s="12"/>
+      <c r="D403" s="12"/>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A404" s="12"/>
+      <c r="B404" s="12"/>
+      <c r="C404" s="12"/>
+      <c r="D404" s="12"/>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A405" s="12"/>
+      <c r="B405" s="12"/>
+      <c r="C405" s="12"/>
+      <c r="D405" s="12"/>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A406" s="12"/>
+      <c r="B406" s="12"/>
+      <c r="C406" s="12"/>
+      <c r="D406" s="12"/>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A407" s="12"/>
+      <c r="B407" s="12"/>
+      <c r="C407" s="12"/>
+      <c r="D407" s="12"/>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A408" s="12"/>
+      <c r="B408" s="12"/>
+      <c r="C408" s="12"/>
+      <c r="D408" s="12"/>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A409" s="12"/>
+      <c r="B409" s="12"/>
+      <c r="C409" s="12"/>
+      <c r="D409" s="12"/>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A410" s="12"/>
+      <c r="B410" s="12"/>
+      <c r="C410" s="12"/>
+      <c r="D410" s="12"/>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A411" s="12"/>
+      <c r="B411" s="12"/>
+      <c r="C411" s="12"/>
+      <c r="D411" s="12"/>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A412" s="12"/>
+      <c r="B412" s="12"/>
+      <c r="C412" s="12"/>
+      <c r="D412" s="12"/>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A413" s="12"/>
+      <c r="B413" s="12"/>
+      <c r="C413" s="12"/>
+      <c r="D413" s="12"/>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A414" s="12"/>
+      <c r="B414" s="12"/>
+      <c r="C414" s="12"/>
+      <c r="D414" s="12"/>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A415" s="12"/>
+      <c r="B415" s="12"/>
+      <c r="C415" s="12"/>
+      <c r="D415" s="12"/>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A416" s="12"/>
+      <c r="B416" s="12"/>
+      <c r="C416" s="12"/>
+      <c r="D416" s="12"/>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A417" s="12"/>
+      <c r="B417" s="12"/>
+      <c r="C417" s="12"/>
+      <c r="D417" s="12"/>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A418" s="12"/>
+      <c r="B418" s="12"/>
+      <c r="C418" s="12"/>
+      <c r="D418" s="12"/>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A419" s="12"/>
+      <c r="B419" s="12"/>
+      <c r="C419" s="12"/>
+      <c r="D419" s="12"/>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A420" s="12"/>
+      <c r="B420" s="12"/>
+      <c r="C420" s="12"/>
+      <c r="D420" s="12"/>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A421" s="12"/>
+      <c r="B421" s="12"/>
+      <c r="C421" s="12"/>
+      <c r="D421" s="12"/>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A422" s="12"/>
+      <c r="B422" s="12"/>
+      <c r="C422" s="12"/>
+      <c r="D422" s="12"/>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A423" s="12"/>
+      <c r="B423" s="12"/>
+      <c r="C423" s="12"/>
+      <c r="D423" s="12"/>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A424" s="12"/>
+      <c r="B424" s="12"/>
+      <c r="C424" s="12"/>
+      <c r="D424" s="12"/>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A425" s="12"/>
+      <c r="B425" s="12"/>
+      <c r="C425" s="12"/>
+      <c r="D425" s="12"/>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A426" s="12"/>
+      <c r="B426" s="12"/>
+      <c r="C426" s="12"/>
+      <c r="D426" s="12"/>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A427" s="12"/>
+      <c r="B427" s="12"/>
+      <c r="C427" s="12"/>
+      <c r="D427" s="12"/>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A428" s="12"/>
+      <c r="B428" s="12"/>
+      <c r="C428" s="12"/>
+      <c r="D428" s="12"/>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A429" s="12"/>
+      <c r="B429" s="12"/>
+      <c r="C429" s="12"/>
+      <c r="D429" s="12"/>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A430" s="12"/>
+      <c r="B430" s="12"/>
+      <c r="C430" s="12"/>
+      <c r="D430" s="12"/>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A431" s="12"/>
+      <c r="B431" s="12"/>
+      <c r="C431" s="12"/>
+      <c r="D431" s="12"/>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A432" s="12"/>
+      <c r="B432" s="12"/>
+      <c r="C432" s="12"/>
+      <c r="D432" s="12"/>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A433" s="12"/>
+      <c r="B433" s="12"/>
+      <c r="C433" s="12"/>
+      <c r="D433" s="12"/>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A434" s="12"/>
+      <c r="B434" s="12"/>
+      <c r="C434" s="12"/>
+      <c r="D434" s="12"/>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A435" s="12"/>
+      <c r="B435" s="12"/>
+      <c r="C435" s="12"/>
+      <c r="D435" s="12"/>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A436" s="12"/>
+      <c r="B436" s="12"/>
+      <c r="C436" s="12"/>
+      <c r="D436" s="12"/>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A437" s="12"/>
+      <c r="B437" s="12"/>
+      <c r="C437" s="12"/>
+      <c r="D437" s="12"/>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A438" s="12"/>
+      <c r="B438" s="12"/>
+      <c r="C438" s="12"/>
+      <c r="D438" s="12"/>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A439" s="12"/>
+      <c r="B439" s="12"/>
+      <c r="C439" s="12"/>
+      <c r="D439" s="12"/>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A440" s="12"/>
+      <c r="B440" s="12"/>
+      <c r="C440" s="12"/>
+      <c r="D440" s="12"/>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A441" s="12"/>
+      <c r="B441" s="12"/>
+      <c r="C441" s="12"/>
+      <c r="D441" s="12"/>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A442" s="12"/>
+      <c r="B442" s="12"/>
+      <c r="C442" s="12"/>
+      <c r="D442" s="12"/>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A443" s="12"/>
+      <c r="B443" s="12"/>
+      <c r="C443" s="12"/>
+      <c r="D443" s="12"/>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A444" s="12"/>
+      <c r="B444" s="12"/>
+      <c r="C444" s="12"/>
+      <c r="D444" s="12"/>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A445" s="12"/>
+      <c r="B445" s="12"/>
+      <c r="C445" s="12"/>
+      <c r="D445" s="12"/>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A446" s="12"/>
+      <c r="B446" s="12"/>
+      <c r="C446" s="12"/>
+      <c r="D446" s="12"/>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A447" s="12"/>
+      <c r="B447" s="12"/>
+      <c r="C447" s="12"/>
+      <c r="D447" s="12"/>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A448" s="12"/>
+      <c r="B448" s="12"/>
+      <c r="C448" s="12"/>
+      <c r="D448" s="12"/>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A449" s="12"/>
+      <c r="B449" s="12"/>
+      <c r="C449" s="12"/>
+      <c r="D449" s="12"/>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A450" s="12"/>
+      <c r="B450" s="12"/>
+      <c r="C450" s="12"/>
+      <c r="D450" s="12"/>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A451" s="12"/>
+      <c r="B451" s="12"/>
+      <c r="C451" s="12"/>
+      <c r="D451" s="12"/>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A452" s="12"/>
+      <c r="B452" s="12"/>
+      <c r="C452" s="12"/>
+      <c r="D452" s="12"/>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A453" s="12"/>
+      <c r="B453" s="12"/>
+      <c r="C453" s="12"/>
+      <c r="D453" s="12"/>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A454" s="12"/>
+      <c r="B454" s="12"/>
+      <c r="C454" s="12"/>
+      <c r="D454" s="12"/>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A455" s="12"/>
+      <c r="B455" s="12"/>
+      <c r="C455" s="12"/>
+      <c r="D455" s="12"/>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A456" s="12"/>
+      <c r="B456" s="12"/>
+      <c r="C456" s="12"/>
+      <c r="D456" s="12"/>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A457" s="12"/>
+      <c r="B457" s="12"/>
+      <c r="C457" s="12"/>
+      <c r="D457" s="12"/>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A458" s="12"/>
+      <c r="B458" s="12"/>
+      <c r="C458" s="12"/>
+      <c r="D458" s="12"/>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A459" s="12"/>
+      <c r="B459" s="12"/>
+      <c r="C459" s="12"/>
+      <c r="D459" s="12"/>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A460" s="12"/>
+      <c r="B460" s="12"/>
+      <c r="C460" s="12"/>
+      <c r="D460" s="12"/>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A461" s="12"/>
+      <c r="B461" s="12"/>
+      <c r="C461" s="12"/>
+      <c r="D461" s="12"/>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A462" s="12"/>
+      <c r="B462" s="12"/>
+      <c r="C462" s="12"/>
+      <c r="D462" s="12"/>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A463" s="12"/>
+      <c r="B463" s="12"/>
+      <c r="C463" s="12"/>
+      <c r="D463" s="12"/>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A464" s="12"/>
+      <c r="B464" s="12"/>
+      <c r="C464" s="12"/>
+      <c r="D464" s="12"/>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A465" s="12"/>
+      <c r="B465" s="12"/>
+      <c r="C465" s="12"/>
+      <c r="D465" s="12"/>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A466" s="12"/>
+      <c r="B466" s="12"/>
+      <c r="C466" s="12"/>
+      <c r="D466" s="12"/>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A467" s="12"/>
+      <c r="B467" s="12"/>
+      <c r="C467" s="12"/>
+      <c r="D467" s="12"/>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A468" s="12"/>
+      <c r="B468" s="12"/>
+      <c r="C468" s="12"/>
+      <c r="D468" s="12"/>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A469" s="12"/>
+      <c r="B469" s="12"/>
+      <c r="C469" s="12"/>
+      <c r="D469" s="12"/>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A470" s="12"/>
+      <c r="B470" s="12"/>
+      <c r="C470" s="12"/>
+      <c r="D470" s="12"/>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A471" s="12"/>
+      <c r="B471" s="12"/>
+      <c r="C471" s="12"/>
+      <c r="D471" s="12"/>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A472" s="12"/>
+      <c r="B472" s="12"/>
+      <c r="C472" s="12"/>
+      <c r="D472" s="12"/>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A473" s="12"/>
+      <c r="B473" s="12"/>
+      <c r="C473" s="12"/>
+      <c r="D473" s="12"/>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A474" s="12"/>
+      <c r="B474" s="12"/>
+      <c r="C474" s="12"/>
+      <c r="D474" s="12"/>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A475" s="12"/>
+      <c r="B475" s="12"/>
+      <c r="C475" s="12"/>
+      <c r="D475" s="12"/>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A476" s="12"/>
+      <c r="B476" s="12"/>
+      <c r="C476" s="12"/>
+      <c r="D476" s="12"/>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A477" s="12"/>
+      <c r="B477" s="12"/>
+      <c r="C477" s="12"/>
+      <c r="D477" s="12"/>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A478" s="12"/>
+      <c r="B478" s="12"/>
+      <c r="C478" s="12"/>
+      <c r="D478" s="12"/>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A479" s="12"/>
+      <c r="B479" s="12"/>
+      <c r="C479" s="12"/>
+      <c r="D479" s="12"/>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A480" s="12"/>
+      <c r="B480" s="12"/>
+      <c r="C480" s="12"/>
+      <c r="D480" s="12"/>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A481" s="12"/>
+      <c r="B481" s="12"/>
+      <c r="C481" s="12"/>
+      <c r="D481" s="12"/>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A482" s="12"/>
+      <c r="B482" s="12"/>
+      <c r="C482" s="12"/>
+      <c r="D482" s="12"/>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A483" s="12"/>
+      <c r="B483" s="12"/>
+      <c r="C483" s="12"/>
+      <c r="D483" s="12"/>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A484" s="12"/>
+      <c r="B484" s="12"/>
+      <c r="C484" s="12"/>
+      <c r="D484" s="12"/>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A485" s="12"/>
+      <c r="B485" s="12"/>
+      <c r="C485" s="12"/>
+      <c r="D485" s="12"/>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A486" s="12"/>
+      <c r="B486" s="12"/>
+      <c r="C486" s="12"/>
+      <c r="D486" s="12"/>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A487" s="12"/>
+      <c r="B487" s="12"/>
+      <c r="C487" s="12"/>
+      <c r="D487" s="12"/>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A488" s="12"/>
+      <c r="B488" s="12"/>
+      <c r="C488" s="12"/>
+      <c r="D488" s="12"/>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A489" s="12"/>
+      <c r="B489" s="12"/>
+      <c r="C489" s="12"/>
+      <c r="D489" s="12"/>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A490" s="12"/>
+      <c r="B490" s="12"/>
+      <c r="C490" s="12"/>
+      <c r="D490" s="12"/>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A491" s="12"/>
+      <c r="B491" s="12"/>
+      <c r="C491" s="12"/>
+      <c r="D491" s="12"/>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A492" s="12"/>
+      <c r="B492" s="12"/>
+      <c r="C492" s="12"/>
+      <c r="D492" s="12"/>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A493" s="12"/>
+      <c r="B493" s="12"/>
+      <c r="C493" s="12"/>
+      <c r="D493" s="12"/>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A494" s="12"/>
+      <c r="B494" s="12"/>
+      <c r="C494" s="12"/>
+      <c r="D494" s="12"/>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A495" s="12"/>
+      <c r="B495" s="12"/>
+      <c r="C495" s="12"/>
+      <c r="D495" s="12"/>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A496" s="12"/>
+      <c r="B496" s="12"/>
+      <c r="C496" s="12"/>
+      <c r="D496" s="12"/>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A497" s="12"/>
+      <c r="B497" s="12"/>
+      <c r="C497" s="12"/>
+      <c r="D497" s="12"/>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A498" s="12"/>
+      <c r="B498" s="12"/>
+      <c r="C498" s="12"/>
+      <c r="D498" s="12"/>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A499" s="12"/>
+      <c r="B499" s="12"/>
+      <c r="C499" s="12"/>
+      <c r="D499" s="12"/>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A500" s="12"/>
+      <c r="B500" s="12"/>
+      <c r="C500" s="12"/>
+      <c r="D500" s="12"/>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A501" s="12"/>
+      <c r="B501" s="12"/>
+      <c r="C501" s="12"/>
+      <c r="D501" s="12"/>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A502" s="12"/>
+      <c r="B502" s="12"/>
+      <c r="C502" s="12"/>
+      <c r="D502" s="12"/>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A503" s="12"/>
+      <c r="B503" s="12"/>
+      <c r="C503" s="12"/>
+      <c r="D503" s="12"/>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A504" s="12"/>
+      <c r="B504" s="12"/>
+      <c r="C504" s="12"/>
+      <c r="D504" s="12"/>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A505" s="12"/>
+      <c r="B505" s="12"/>
+      <c r="C505" s="12"/>
+      <c r="D505" s="12"/>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A506" s="12"/>
+      <c r="B506" s="12"/>
+      <c r="C506" s="12"/>
+      <c r="D506" s="12"/>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A507" s="12"/>
+      <c r="B507" s="12"/>
+      <c r="C507" s="12"/>
+      <c r="D507" s="12"/>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A508" s="12"/>
+      <c r="B508" s="12"/>
+      <c r="C508" s="12"/>
+      <c r="D508" s="12"/>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A509" s="12"/>
+      <c r="B509" s="12"/>
+      <c r="C509" s="12"/>
+      <c r="D509" s="12"/>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A510" s="12"/>
+      <c r="B510" s="12"/>
+      <c r="C510" s="12"/>
+      <c r="D510" s="12"/>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A511" s="12"/>
+      <c r="B511" s="12"/>
+      <c r="C511" s="12"/>
+      <c r="D511" s="12"/>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A512" s="12"/>
+      <c r="B512" s="12"/>
+      <c r="C512" s="12"/>
+      <c r="D512" s="12"/>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A513" s="12"/>
+      <c r="B513" s="12"/>
+      <c r="C513" s="12"/>
+      <c r="D513" s="12"/>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A514" s="12"/>
+      <c r="B514" s="12"/>
+      <c r="C514" s="12"/>
+      <c r="D514" s="12"/>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A515" s="12"/>
+      <c r="B515" s="12"/>
+      <c r="C515" s="12"/>
+      <c r="D515" s="12"/>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A516" s="12"/>
+      <c r="B516" s="12"/>
+      <c r="C516" s="12"/>
+      <c r="D516" s="12"/>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A517" s="12"/>
+      <c r="B517" s="12"/>
+      <c r="C517" s="12"/>
+      <c r="D517" s="12"/>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A518" s="12"/>
+      <c r="B518" s="12"/>
+      <c r="C518" s="12"/>
+      <c r="D518" s="12"/>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A519" s="12"/>
+      <c r="B519" s="12"/>
+      <c r="C519" s="12"/>
+      <c r="D519" s="12"/>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A520" s="12"/>
+      <c r="B520" s="12"/>
+      <c r="C520" s="12"/>
+      <c r="D520" s="12"/>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A521" s="12"/>
+      <c r="B521" s="12"/>
+      <c r="C521" s="12"/>
+      <c r="D521" s="12"/>
+    </row>
+    <row r="522" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A522" s="12"/>
+      <c r="B522" s="12"/>
+      <c r="C522" s="12"/>
+      <c r="D522" s="12"/>
+    </row>
+    <row r="523" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A523" s="12"/>
+      <c r="B523" s="12"/>
+      <c r="C523" s="12"/>
+      <c r="D523" s="12"/>
+    </row>
+    <row r="524" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A524" s="12"/>
+      <c r="B524" s="12"/>
+      <c r="C524" s="12"/>
+      <c r="D524" s="12"/>
+    </row>
+    <row r="525" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A525" s="12"/>
+      <c r="B525" s="12"/>
+      <c r="C525" s="12"/>
+      <c r="D525" s="12"/>
+    </row>
+    <row r="526" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A526" s="12"/>
+      <c r="B526" s="12"/>
+      <c r="C526" s="12"/>
+      <c r="D526" s="12"/>
+    </row>
+    <row r="527" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A527" s="12"/>
+      <c r="B527" s="12"/>
+      <c r="C527" s="12"/>
+      <c r="D527" s="12"/>
+    </row>
+    <row r="528" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A528" s="12"/>
+      <c r="B528" s="12"/>
+      <c r="C528" s="12"/>
+      <c r="D528" s="12"/>
+    </row>
+    <row r="529" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A529" s="12"/>
+      <c r="B529" s="12"/>
+      <c r="C529" s="12"/>
+      <c r="D529" s="12"/>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A530" s="12"/>
+      <c r="B530" s="12"/>
+      <c r="C530" s="12"/>
+      <c r="D530" s="12"/>
+    </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A531" s="12"/>
+      <c r="B531" s="12"/>
+      <c r="C531" s="12"/>
+      <c r="D531" s="12"/>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A532" s="12"/>
+      <c r="B532" s="12"/>
+      <c r="C532" s="12"/>
+      <c r="D532" s="12"/>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A533" s="12"/>
+      <c r="B533" s="12"/>
+      <c r="C533" s="12"/>
+      <c r="D533" s="12"/>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A534" s="12"/>
+      <c r="B534" s="12"/>
+      <c r="C534" s="12"/>
+      <c r="D534" s="12"/>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A535" s="12"/>
+      <c r="B535" s="12"/>
+      <c r="C535" s="12"/>
+      <c r="D535" s="12"/>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A536" s="12"/>
+      <c r="B536" s="12"/>
+      <c r="C536" s="12"/>
+      <c r="D536" s="12"/>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A537" s="12"/>
+      <c r="B537" s="12"/>
+      <c r="C537" s="12"/>
+      <c r="D537" s="12"/>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A538" s="12"/>
+      <c r="B538" s="12"/>
+      <c r="C538" s="12"/>
+      <c r="D538" s="12"/>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A539" s="12"/>
+      <c r="B539" s="12"/>
+      <c r="C539" s="12"/>
+      <c r="D539" s="12"/>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A540" s="12"/>
+      <c r="B540" s="12"/>
+      <c r="C540" s="12"/>
+      <c r="D540" s="12"/>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A541" s="12"/>
+      <c r="B541" s="12"/>
+      <c r="C541" s="12"/>
+      <c r="D541" s="12"/>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A542" s="12"/>
+      <c r="B542" s="12"/>
+      <c r="C542" s="12"/>
+      <c r="D542" s="12"/>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A543" s="12"/>
+      <c r="B543" s="12"/>
+      <c r="C543" s="12"/>
+      <c r="D543" s="12"/>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A544" s="12"/>
+      <c r="B544" s="12"/>
+      <c r="C544" s="12"/>
+      <c r="D544" s="12"/>
+    </row>
+    <row r="545" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A545" s="12"/>
+      <c r="B545" s="12"/>
+      <c r="C545" s="12"/>
+      <c r="D545" s="12"/>
+    </row>
+    <row r="546" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A546" s="12"/>
+      <c r="B546" s="12"/>
+      <c r="C546" s="12"/>
+      <c r="D546" s="12"/>
+    </row>
+    <row r="547" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A547" s="12"/>
+      <c r="B547" s="12"/>
+      <c r="C547" s="12"/>
+      <c r="D547" s="12"/>
+    </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A548" s="12"/>
+      <c r="B548" s="12"/>
+      <c r="C548" s="12"/>
+      <c r="D548" s="12"/>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A549" s="12"/>
+      <c r="B549" s="12"/>
+      <c r="C549" s="12"/>
+      <c r="D549" s="12"/>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A550" s="12"/>
+      <c r="B550" s="12"/>
+      <c r="C550" s="12"/>
+      <c r="D550" s="12"/>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A551" s="12"/>
+      <c r="B551" s="12"/>
+      <c r="C551" s="12"/>
+      <c r="D551" s="12"/>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A552" s="12"/>
+      <c r="B552" s="12"/>
+      <c r="C552" s="12"/>
+      <c r="D552" s="12"/>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A553" s="12"/>
+      <c r="B553" s="12"/>
+      <c r="C553" s="12"/>
+      <c r="D553" s="12"/>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A554" s="12"/>
+      <c r="B554" s="12"/>
+      <c r="C554" s="12"/>
+      <c r="D554" s="12"/>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A555" s="12"/>
+      <c r="B555" s="12"/>
+      <c r="C555" s="12"/>
+      <c r="D555" s="12"/>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A556" s="12"/>
+      <c r="B556" s="12"/>
+      <c r="C556" s="12"/>
+      <c r="D556" s="12"/>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A557" s="12"/>
+      <c r="B557" s="12"/>
+      <c r="C557" s="12"/>
+      <c r="D557" s="12"/>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A558" s="12"/>
+      <c r="B558" s="12"/>
+      <c r="C558" s="12"/>
+      <c r="D558" s="12"/>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A559" s="12"/>
+      <c r="B559" s="12"/>
+      <c r="C559" s="12"/>
+      <c r="D559" s="12"/>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A560" s="12"/>
+      <c r="B560" s="12"/>
+      <c r="C560" s="12"/>
+      <c r="D560" s="12"/>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A561" s="12"/>
+      <c r="B561" s="12"/>
+      <c r="C561" s="12"/>
+      <c r="D561" s="12"/>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A562" s="12"/>
+      <c r="B562" s="12"/>
+      <c r="C562" s="12"/>
+      <c r="D562" s="12"/>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A563" s="12"/>
+      <c r="B563" s="12"/>
+      <c r="C563" s="12"/>
+      <c r="D563" s="12"/>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A564" s="12"/>
+      <c r="B564" s="12"/>
+      <c r="C564" s="12"/>
+      <c r="D564" s="12"/>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A565" s="12"/>
+      <c r="B565" s="12"/>
+      <c r="C565" s="12"/>
+      <c r="D565" s="12"/>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A566" s="12"/>
+      <c r="B566" s="12"/>
+      <c r="C566" s="12"/>
+      <c r="D566" s="12"/>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A567" s="12"/>
+      <c r="B567" s="12"/>
+      <c r="C567" s="12"/>
+      <c r="D567" s="12"/>
+    </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A568" s="12"/>
+      <c r="B568" s="12"/>
+      <c r="C568" s="12"/>
+      <c r="D568" s="12"/>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A569" s="12"/>
+      <c r="B569" s="12"/>
+      <c r="C569" s="12"/>
+      <c r="D569" s="12"/>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A570" s="12"/>
+      <c r="B570" s="12"/>
+      <c r="C570" s="12"/>
+      <c r="D570" s="12"/>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A571" s="12"/>
+      <c r="B571" s="12"/>
+      <c r="C571" s="12"/>
+      <c r="D571" s="12"/>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A572" s="12"/>
+      <c r="B572" s="12"/>
+      <c r="C572" s="12"/>
+      <c r="D572" s="12"/>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A573" s="12"/>
+      <c r="B573" s="12"/>
+      <c r="C573" s="12"/>
+      <c r="D573" s="12"/>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A574" s="12"/>
+      <c r="B574" s="12"/>
+      <c r="C574" s="12"/>
+      <c r="D574" s="12"/>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A575" s="12"/>
+      <c r="B575" s="12"/>
+      <c r="C575" s="12"/>
+      <c r="D575" s="12"/>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A576" s="12"/>
+      <c r="B576" s="12"/>
+      <c r="C576" s="12"/>
+      <c r="D576" s="12"/>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A577" s="12"/>
+      <c r="B577" s="12"/>
+      <c r="C577" s="12"/>
+      <c r="D577" s="12"/>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A578" s="12"/>
+      <c r="B578" s="12"/>
+      <c r="C578" s="12"/>
+      <c r="D578" s="12"/>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A579" s="12"/>
+      <c r="B579" s="12"/>
+      <c r="C579" s="12"/>
+      <c r="D579" s="12"/>
+    </row>
+    <row r="580" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A580" s="12"/>
+      <c r="B580" s="12"/>
+      <c r="C580" s="12"/>
+      <c r="D580" s="12"/>
+    </row>
+    <row r="581" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A581" s="12"/>
+      <c r="B581" s="12"/>
+      <c r="C581" s="12"/>
+      <c r="D581" s="12"/>
+    </row>
+    <row r="582" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A582" s="12"/>
+      <c r="B582" s="12"/>
+      <c r="C582" s="12"/>
+      <c r="D582" s="12"/>
+    </row>
+    <row r="583" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A583" s="12"/>
+      <c r="B583" s="12"/>
+      <c r="C583" s="12"/>
+      <c r="D583" s="12"/>
+    </row>
+    <row r="584" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A584" s="12"/>
+      <c r="B584" s="12"/>
+      <c r="C584" s="12"/>
+      <c r="D584" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="150">
@@ -7434,7 +10489,8 @@
     <mergeCell ref="D169:D171"/>
     <mergeCell ref="F169:F171"/>
     <mergeCell ref="G169:G171"/>
-    <mergeCell ref="M163:M165"/>
+    <mergeCell ref="H169:H171"/>
+    <mergeCell ref="I169:I171"/>
     <mergeCell ref="A166:A168"/>
     <mergeCell ref="B166:B168"/>
     <mergeCell ref="C166:C168"/>
@@ -7444,14 +10500,6 @@
     <mergeCell ref="G166:G168"/>
     <mergeCell ref="H166:H168"/>
     <mergeCell ref="I166:I168"/>
-    <mergeCell ref="G163:G165"/>
-    <mergeCell ref="H163:H165"/>
-    <mergeCell ref="I163:I165"/>
-    <mergeCell ref="J163:J165"/>
-    <mergeCell ref="K163:K165"/>
-    <mergeCell ref="L163:L165"/>
-    <mergeCell ref="H169:H171"/>
-    <mergeCell ref="I169:I171"/>
     <mergeCell ref="J159:J161"/>
     <mergeCell ref="K159:K161"/>
     <mergeCell ref="L159:L161"/>
@@ -7462,6 +10510,13 @@
     <mergeCell ref="D163:D165"/>
     <mergeCell ref="E163:E165"/>
     <mergeCell ref="F163:F165"/>
+    <mergeCell ref="M163:M165"/>
+    <mergeCell ref="G163:G165"/>
+    <mergeCell ref="H163:H165"/>
+    <mergeCell ref="I163:I165"/>
+    <mergeCell ref="J163:J165"/>
+    <mergeCell ref="K163:K165"/>
+    <mergeCell ref="L163:L165"/>
     <mergeCell ref="L151:L152"/>
     <mergeCell ref="M151:M152"/>
     <mergeCell ref="M156:M158"/>

</xml_diff>

<commit_message>
Final debugging and fixing things up
</commit_message>
<xml_diff>
--- a/database/COSC345_Recipes.xlsx
+++ b/database/COSC345_Recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\Downloads\COSC345\Realm-of-Feasts\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{869F6E1F-D6DE-4737-8782-AE8B06CA0C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8D6CBD0E-4F00-48EA-BB8A-946A946E69B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
@@ -1775,9 +1775,6 @@
     <t xml:space="preserve">Chocolate Cake Delicacy </t>
   </si>
   <si>
-    <t>2*ounces*Bittersweet Chocolate (chopped),1*tablespoon*Instant Coffee,1.25*cups*Boiling Water,2.75*cups*Flour,2,75*cups*Granulated Sugar,0.75*cup*Unsweetened Cocoa Powder,0.5*teaspoon*Salt,2*teaspoons*Baking Soda,1*teaspoon*Baking Powder,1*cup*Vegetable Oil,1.25*cups*Buttermilk,4*large*Eggs,2*teaspoons*Pure Vanilla Extract</t>
-  </si>
-  <si>
     <t>Paddington Burgers</t>
   </si>
   <si>
@@ -1835,9 +1832,6 @@
     <t>Stewed beef with a side of dumpling</t>
   </si>
   <si>
-    <t>1*cup*FLour,0.25*teaspoon*Salt,1*teaspoon*Baking Powder,0.25*teaspoon*Freshly Ground Black Pepper,0.25*teaspoon*Ground Sage,0.25*teaspoon*Ground Thyme,0.25*teaspoon*Dried Marjoram,2*tablespoons*Fresh Parsley (chopped),4*tablespoons*Butter (chilled and cut into small pieces),2*tablespoons*Milk,1*null*Egg,3*tablespoons*Vegetable Oil,1.5*pounds*Chuck Steak (trimmed and cut into half inch cubes),1*null*Onion (chopped),1*tablespoon*Flour,1*14ounce*Chicken Broth Can,1*sprinkle*Salt,1*sprinkle*Freshly Ground Black Pepper,2*null*Carrots (cut into 1 inch pieces),2*null*Celery Ribs (cut into 1 inch pieces),4*null*Red Skinned Potatoes (unpeeled, scrubbed, and cut into 1 inch cubes)</t>
-  </si>
-  <si>
     <t>1. To make the dumplings, whisk together the flour, salt, baking powder, black pepper, and herbs. Add the pieces of butter and rub with your fingertips until the mixture resembles a coarse meal and no powdery bits remain.||2. Whisk the milk and egg together and add to the flour mixture. Toss with a rubber spatula until the mixture begins to clump together. Press plastic wrap down on top of the dough and refrigerate until needed.||3. To make the stew, heat 1 tablespoon of the oil in a Dutch oven or wide pot and add the meat in batches, searing on both sides over high heat for 4 to 5 minutes until crusty brown, and transferring each batch to a dinner plate. Add the remaining 2 tablespoons of oil to the skillet. Add the chopped onion and cook over medium-low heat until softened, scraping up the fond (browned bits) from the bottom of the pot with a wooden spoon.||4. Add the flour to the pot and stir until combined. Pour in the chicken broth and stir until well combined. Add the salt and pepper and the meat along with its accumulated juices to the pot and cook over medium-high heat, stirring occasionally, until thickened and bubbling. Reduce to a simmer and simmer the meat for 1 and half hours.||5. Add the carrots, celery, and potatoes to the pot and simmer for 1 hour, stirring occasionally. Remove the dumpling dough from the refrigerator. Wet your hands and form the dumplings into 1-inch balls, dropping them onto the hot stew in the pot as you form them. Wet your hands as needed to prevent sticking. Cover the pot and simmer another 30 minutes until the dumplings have puffed up and feel set when pressed lightly with the fingertips, though they will be very soft.</t>
   </si>
   <si>
@@ -1979,9 +1973,6 @@
     <t xml:space="preserve"> A classic rice soup, a Japanese version of chicken noodle soup</t>
   </si>
   <si>
-    <t>6*null*Radishes (sliced and simmered),3.5*cups*Dashi (divided),2*null*Chicken Thighs ( boneless, skinless and chopped),1*null*Carrot (sliced),3*null*Shiitake Mushrooms (chopped),1.5*cups*Japanese Rice (cooked),1*tablespoon*Soy Sauce,1*large*Egg,3*null*Green Onions (chopped),1*teaspoon*Sesame Seeds ( toasted),0.25*teaspoon*Pepper</t>
-  </si>
-  <si>
     <t>Chojis Chips</t>
   </si>
   <si>
@@ -2084,9 +2075,6 @@
     <t>An octopus dish</t>
   </si>
   <si>
-    <t>3*tablespoons*Rice Vinegar,1*tablespoon*Sugar,1*tablespoon*Soy Sauce,0.25*inch*Ginger (fresh and grated),0.5*tablespoon*Dried Wakame,1*small*Cucumber,1*teaspoon*Salt,0.25*pound*Octopus (boiled, precooked and sliced)</t>
-  </si>
-  <si>
     <t>1. Combine the rice vinegar, sugar, soy sauce, and ginger in a small bowl and stir to combine, then set aside.||2. Place the wakame in a small bowl of water and let sit for 15 minutes to allow the wakame to rehydrate.||3. Slice the cucumber thinly and place in a small bowl. Stir in the salt, and let it sit for 15 minutes.||4. Gently squeeze out the water from the cucumbers with your hands, taking a handful at a time and squeezing it between your palms, then place in a large bowl.||5. Add the sliced octopus, wakame, and seasoning and stir well to combine.||6. Serve chilled.</t>
   </si>
   <si>
@@ -2514,6 +2502,18 @@
   </si>
   <si>
     <t>1. To make the stock, combine all the stock ingredients in a heavy saucepan. Bring to a boil. Cover and reduce to a simmer for 1 hour. Strain the solids and return the liquid to the pan. Bring to a boil and reduce the total volume to 1 and a quarter cups. Set aside to cool.||2. To make the pastry, combine the flour and salt in a large mixing bowl. Place the lard or vegetable shortening in a saucepan along with the milk and water; set the saucepan over high heat until the fat melts. Bring to a boil. Stir the fat and liquids together and pour into the bowl with the flour. Mix well. Turn the dough out onto a flour dusted work surface. Form the dough into a ball and dust it with flour. Knead for 5 minutes. Wrap in plastic wrap and let rest for 30 minutes.||3. For the filling, dice the pork into quarter-inch pieces or place chunks of pork into a food processor and pulse to coarsely chop. Place the pork in a large mixing bowl with the diced bacon, sage, minced anchovy or anchovy oil, and allspice. Add a quarter cup of the stock and mix well. Test the seasoning by heating a small amount of water in a saute pan to a boil and cook a small amount of the pork mixture (1 teaspoon) in it. Taste the filling and adjust the salt and pepper as desired.||4. To assemble the pies, preheat the oven to 400 degrees Fahrenheit, then decide on the size of the finished pies desired. This recipe can be made in a muffin pan, popover pan, or 4-ounce ceramic ramekins. Cut off 3 quarters of the dough and place on a flour-dusted work surface. Roll it out 1/8-inch thick. To make the bottom crust, cut 4-inch circles for a muffin or popover pan and 41/2-inch circles for the ramekins. Place the dough circles in the cups or ramekins and press the dough into the bottom and sides of each.|5. Fill the pastry-lined moulds up to the rim. Fold any excess dough from the sides onto the top of the filling. Roll out the remaining dough and cut 3-inch circles to fit into the tops of the muffin or popover pan or ramekins. Place the tops onto the filling and press down lightly to seal. Cut a small hole in the centre of each top. Reroll any excess dough. Using small pastry cutters, cut out shapes and decorate the tops. Brush the top of each pie with the beaten egg. Bake the pies for 20 minutes. Reduce the heat to 350 degrees Fahrenheit and bake for 2 hours.||6. Remove the pies from the oven, brush with the beaten egg again, and bake for 10 minutes longer. Remove and let cool in the pan.||7. Bring the reduced stock back to a boil, remove from the heat, add the gelatin, and stir to dissolve. Using a funnel, spoon the stock mixture into the hole at the top of each pie, dividing the stock evenly among the pies. This is a slow process, and all of the liquid should be used. Chill overnight.||8. To serve, remove from the pan and serve with good English mustard.</t>
+  </si>
+  <si>
+    <t>2*ounces*Bittersweet Chocolate (chopped),1*tablespoon*Instant Coffee,1.25*cups*Boiling Water,2.75*cups*Flour,2.75*cups*Granulated Sugar,0.75*cup*Unsweetened Cocoa Powder,0.5*teaspoon*Salt,2*teaspoons*Baking Soda,1*teaspoon*Baking Powder,1*cup*Vegetable Oil,1.25*cups*Buttermilk,4*large*Eggs,2*teaspoons*Pure Vanilla Extract</t>
+  </si>
+  <si>
+    <t>1*cup*FLour,0.25*teaspoon*Salt,1*teaspoon*Baking Powder,0.25*teaspoon*Freshly Ground Black Pepper,0.25*teaspoon*Ground Sage,0.25*teaspoon*Ground Thyme,0.25*teaspoon*Dried Marjoram,2*tablespoons*Fresh Parsley (chopped),4*tablespoons*Butter (chilled and cut into small pieces),2*tablespoons*Milk,1*null*Egg,3*tablespoons*Vegetable Oil,1.5*pounds*Chuck Steak (trimmed and cut into half inch cubes),1*null*Onion (chopped),1*tablespoon*Flour,1*14ounce*Chicken Broth Can,1*sprinkle*Salt,1*sprinkle*Freshly Ground Black Pepper,2*null*Carrots (cut into 1 inch pieces),2*null*Celery Ribs (cut into 1 inch pieces),4*null*Red Skinned Potatoes (unpeeled - scrubbed - and cut into 1 inch cubes)</t>
+  </si>
+  <si>
+    <t>3*tablespoons*Rice Vinegar,1*tablespoon*Sugar,1*tablespoon*Soy Sauce,0.25*inch*Ginger (fresh and grated),0.5*tablespoon*Dried Wakame,1*small*Cucumber,1*teaspoon*Salt,0.25*pound*Octopus (boiled - precooked and sliced)</t>
+  </si>
+  <si>
+    <t>6*null*Radishes (sliced and simmered),3.5*cups*Dashi (divided),2*null*Chicken Thighs ( boneless - skinless and chopped),1*null*Carrot (sliced),3*null*Shiitake Mushrooms (chopped),1.5*cups*Japanese Rice (cooked),1*tablespoon*Soy Sauce,1*large*Egg,3*null*Green Onions (chopped),1*teaspoon*Sesame Seeds ( toasted),0.25*teaspoon*Pepper</t>
   </si>
 </sst>
 </file>
@@ -2980,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
   <dimension ref="A1:G196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3021,7 +3021,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -3044,7 +3044,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -3067,7 +3067,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>18</v>
@@ -3090,7 +3090,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>22</v>
@@ -3113,7 +3113,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>26</v>
@@ -3136,7 +3136,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>30</v>
@@ -3159,7 +3159,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>34</v>
@@ -3182,7 +3182,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>38</v>
@@ -3205,7 +3205,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>41</v>
@@ -3228,7 +3228,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>45</v>
@@ -3251,7 +3251,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>49</v>
@@ -3274,7 +3274,7 @@
         <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>53</v>
@@ -3297,7 +3297,7 @@
         <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>57</v>
@@ -3320,7 +3320,7 @@
         <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>61</v>
@@ -3343,7 +3343,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>65</v>
@@ -3366,7 +3366,7 @@
         <v>69</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>70</v>
@@ -3412,7 +3412,7 @@
         <v>78</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>79</v>
@@ -3435,7 +3435,7 @@
         <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>83</v>
@@ -3458,7 +3458,7 @@
         <v>86</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>87</v>
@@ -3481,7 +3481,7 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>91</v>
@@ -6014,13 +6014,13 @@
         <v>550</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>551</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="F132" s="12">
         <v>25</v>
@@ -6066,7 +6066,7 @@
         <v>559</v>
       </c>
       <c r="E134" s="14" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="F134" s="14">
         <v>30</v>
@@ -6112,7 +6112,7 @@
         <v>566</v>
       </c>
       <c r="E136" s="14" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="F136" s="14">
         <v>15</v>
@@ -6158,7 +6158,7 @@
         <v>573</v>
       </c>
       <c r="E138" s="14" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="F138" s="14">
         <v>20</v>
@@ -6181,7 +6181,7 @@
         <v>576</v>
       </c>
       <c r="E139" s="14" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="F139" s="14">
         <v>10</v>
@@ -6201,10 +6201,10 @@
         <v>578</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>579</v>
+        <v>822</v>
       </c>
       <c r="E140" s="14" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="F140" s="14">
         <v>60</v>
@@ -6215,19 +6215,19 @@
     </row>
     <row r="141" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B141" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C141" s="14" t="s">
+        <v>580</v>
+      </c>
+      <c r="D141" s="14" t="s">
         <v>581</v>
       </c>
-      <c r="D141" s="14" t="s">
-        <v>582</v>
-      </c>
       <c r="E141" s="14" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="F141" s="14">
         <v>30</v>
@@ -6238,19 +6238,19 @@
     </row>
     <row r="142" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B142" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C142" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="D142" s="14" t="s">
         <v>584</v>
       </c>
-      <c r="D142" s="14" t="s">
-        <v>585</v>
-      </c>
       <c r="E142" s="14" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="F142" s="14">
         <v>115</v>
@@ -6261,19 +6261,19 @@
     </row>
     <row r="143" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B143" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C143" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="D143" s="14" t="s">
         <v>587</v>
       </c>
-      <c r="D143" s="14" t="s">
+      <c r="E143" s="14" t="s">
         <v>588</v>
-      </c>
-      <c r="E143" s="14" t="s">
-        <v>589</v>
       </c>
       <c r="F143" s="14">
         <v>80</v>
@@ -6284,19 +6284,19 @@
     </row>
     <row r="144" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B144" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C144" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="D144" s="14" t="s">
         <v>591</v>
       </c>
-      <c r="D144" s="14" t="s">
+      <c r="E144" s="14" t="s">
         <v>592</v>
-      </c>
-      <c r="E144" s="14" t="s">
-        <v>593</v>
       </c>
       <c r="F144" s="14">
         <v>35</v>
@@ -6307,19 +6307,19 @@
     </row>
     <row r="145" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="15" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B145" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C145" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="D145" s="14" t="s">
         <v>595</v>
       </c>
-      <c r="D145" s="14" t="s">
-        <v>596</v>
-      </c>
       <c r="E145" s="14" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="F145" s="14">
         <v>70</v>
@@ -6330,19 +6330,19 @@
     </row>
     <row r="146" spans="1:7" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B146" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C146" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="D146" s="14" t="s">
+        <v>823</v>
+      </c>
+      <c r="E146" s="14" t="s">
         <v>598</v>
-      </c>
-      <c r="D146" s="14" t="s">
-        <v>599</v>
-      </c>
-      <c r="E146" s="14" t="s">
-        <v>600</v>
       </c>
       <c r="F146" s="14">
         <v>210</v>
@@ -6353,19 +6353,19 @@
     </row>
     <row r="147" spans="1:7" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B147" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C147" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="D147" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="E147" s="14" t="s">
         <v>602</v>
-      </c>
-      <c r="D147" s="14" t="s">
-        <v>603</v>
-      </c>
-      <c r="E147" s="14" t="s">
-        <v>604</v>
       </c>
       <c r="F147" s="14">
         <v>90</v>
@@ -6376,19 +6376,19 @@
     </row>
     <row r="148" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B148" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C148" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="D148" s="14" t="s">
+        <v>605</v>
+      </c>
+      <c r="E148" s="14" t="s">
         <v>606</v>
-      </c>
-      <c r="D148" s="14" t="s">
-        <v>607</v>
-      </c>
-      <c r="E148" s="14" t="s">
-        <v>608</v>
       </c>
       <c r="F148" s="14">
         <v>55</v>
@@ -6399,19 +6399,19 @@
     </row>
     <row r="149" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A149" s="14" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B149" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C149" s="14" t="s">
+        <v>608</v>
+      </c>
+      <c r="D149" s="14" t="s">
+        <v>609</v>
+      </c>
+      <c r="E149" s="14" t="s">
         <v>610</v>
-      </c>
-      <c r="D149" s="14" t="s">
-        <v>611</v>
-      </c>
-      <c r="E149" s="14" t="s">
-        <v>612</v>
       </c>
       <c r="F149" s="14">
         <v>40</v>
@@ -6422,19 +6422,19 @@
     </row>
     <row r="150" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B150" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C150" s="14" t="s">
+        <v>612</v>
+      </c>
+      <c r="D150" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="E150" s="14" t="s">
         <v>614</v>
-      </c>
-      <c r="D150" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="E150" s="14" t="s">
-        <v>616</v>
       </c>
       <c r="F150" s="14">
         <v>20</v>
@@ -6445,19 +6445,19 @@
     </row>
     <row r="151" spans="1:7" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="14" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B151" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E151" s="14" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="F151" s="14">
         <v>140</v>
@@ -6468,19 +6468,19 @@
     </row>
     <row r="152" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B152" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E152" s="14" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="F152" s="14">
         <v>340</v>
@@ -6491,19 +6491,19 @@
     </row>
     <row r="153" spans="1:7" ht="244.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="14" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B153" s="14" t="s">
         <v>553</v>
       </c>
       <c r="C153" s="14" t="s">
+        <v>622</v>
+      </c>
+      <c r="D153" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="E153" s="14" t="s">
         <v>624</v>
-      </c>
-      <c r="D153" s="14" t="s">
-        <v>625</v>
-      </c>
-      <c r="E153" s="14" t="s">
-        <v>626</v>
       </c>
       <c r="F153" s="14">
         <v>10</v>
@@ -6514,19 +6514,19 @@
     </row>
     <row r="154" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A154" s="14" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B154" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C154" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="D154" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="E154" s="14" t="s">
         <v>628</v>
-      </c>
-      <c r="D154" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="E154" s="14" t="s">
-        <v>630</v>
       </c>
       <c r="F154" s="14">
         <v>155</v>
@@ -6537,19 +6537,19 @@
     </row>
     <row r="155" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A155" s="14" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B155" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>647</v>
+        <v>825</v>
       </c>
       <c r="E155" s="14" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F155" s="14">
         <v>35</v>
@@ -6560,19 +6560,19 @@
     </row>
     <row r="156" spans="1:7" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="14" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B156" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="E156" s="14" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="F156" s="14">
         <v>50</v>
@@ -6583,19 +6583,19 @@
     </row>
     <row r="157" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A157" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B157" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="E157" s="14" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="F157" s="14">
         <v>45</v>
@@ -6606,19 +6606,19 @@
     </row>
     <row r="158" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A158" s="14" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B158" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="E158" s="14" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="F158" s="14">
         <v>15</v>
@@ -6629,19 +6629,19 @@
     </row>
     <row r="159" spans="1:7" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="14" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B159" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="E159" s="14" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="F159" s="14">
         <v>330</v>
@@ -6652,19 +6652,19 @@
     </row>
     <row r="160" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A160" s="14" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="B160" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="E160" s="14" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="F160" s="14">
         <v>740</v>
@@ -6675,19 +6675,19 @@
     </row>
     <row r="161" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A161" s="14" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B161" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E161" s="14" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="F161" s="14">
         <v>300</v>
@@ -6698,19 +6698,19 @@
     </row>
     <row r="162" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A162" s="14" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B162" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E162" s="14" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="F162" s="14">
         <v>20</v>
@@ -6721,19 +6721,19 @@
     </row>
     <row r="163" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="14" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="B163" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="E163" s="14" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="F163" s="14">
         <v>40</v>
@@ -6744,19 +6744,19 @@
     </row>
     <row r="164" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A164" s="14" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="B164" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="E164" s="14" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="F164" s="14">
         <v>35</v>
@@ -6767,19 +6767,19 @@
     </row>
     <row r="165" spans="1:7" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A165" s="14" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B165" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E165" s="14" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="F165" s="14">
         <v>30</v>
@@ -6790,19 +6790,19 @@
     </row>
     <row r="166" spans="1:7" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="14" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="B166" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>682</v>
+        <v>824</v>
       </c>
       <c r="E166" s="14" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="F166" s="14">
         <v>15</v>
@@ -6813,19 +6813,19 @@
     </row>
     <row r="167" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A167" s="14" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="B167" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="E167" s="14" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="F167" s="14">
         <v>50</v>
@@ -6836,19 +6836,19 @@
     </row>
     <row r="168" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A168" s="14" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B168" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E168" s="14" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="F168" s="14">
         <v>40</v>
@@ -6859,19 +6859,19 @@
     </row>
     <row r="169" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="14" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="B169" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="F169" s="14">
         <v>15</v>
@@ -6882,19 +6882,19 @@
     </row>
     <row r="170" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A170" s="14" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B170" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="F170" s="14">
         <v>20</v>
@@ -6905,19 +6905,19 @@
     </row>
     <row r="171" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A171" s="14" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B171" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="F171" s="14">
         <v>25</v>
@@ -6928,19 +6928,19 @@
     </row>
     <row r="172" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A172" s="14" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="B172" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="F172" s="14">
         <v>10</v>
@@ -6951,19 +6951,19 @@
     </row>
     <row r="173" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A173" s="14" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B173" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="F173" s="14">
         <v>5</v>
@@ -6974,19 +6974,19 @@
     </row>
     <row r="174" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A174" s="14" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B174" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D174" s="14" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F174" s="14">
         <v>5</v>
@@ -6997,19 +6997,19 @@
     </row>
     <row r="175" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="14" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B175" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="D175" s="14" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="F175" s="14">
         <v>5</v>
@@ -7020,19 +7020,19 @@
     </row>
     <row r="176" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A176" s="14" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B176" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="D176" s="14" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="F176" s="14">
         <v>5</v>
@@ -7043,19 +7043,19 @@
     </row>
     <row r="177" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A177" s="14" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B177" s="14" t="s">
         <v>550</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D177" s="14" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F177" s="14">
         <v>95</v>
@@ -7066,19 +7066,19 @@
     </row>
     <row r="178" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A178" s="14" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D178" s="14" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="F178" s="14">
         <v>75</v>
@@ -7089,19 +7089,19 @@
     </row>
     <row r="179" spans="1:7" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A179" s="14" t="s">
+        <v>722</v>
+      </c>
+      <c r="B179" s="14" t="s">
+        <v>720</v>
+      </c>
+      <c r="C179" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="B179" s="14" t="s">
-        <v>724</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>730</v>
-      </c>
       <c r="D179" s="14" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="F179" s="14">
         <v>150</v>
@@ -7112,19 +7112,19 @@
     </row>
     <row r="180" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A180" s="14" t="s">
+        <v>723</v>
+      </c>
+      <c r="B180" s="14" t="s">
+        <v>720</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="E180" s="3" t="s">
         <v>727</v>
-      </c>
-      <c r="B180" s="14" t="s">
-        <v>724</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="E180" s="3" t="s">
-        <v>731</v>
       </c>
       <c r="F180" s="14">
         <v>30</v>
@@ -7135,19 +7135,19 @@
     </row>
     <row r="181" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A181" s="14" t="s">
+        <v>724</v>
+      </c>
+      <c r="B181" s="14" t="s">
+        <v>720</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="E181" s="3" t="s">
         <v>728</v>
-      </c>
-      <c r="B181" s="14" t="s">
-        <v>724</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="E181" s="3" t="s">
-        <v>732</v>
       </c>
       <c r="F181" s="14">
         <v>65</v>
@@ -7158,19 +7158,19 @@
     </row>
     <row r="182" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A182" s="14" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="F182" s="14">
         <v>10</v>
@@ -7181,19 +7181,19 @@
     </row>
     <row r="183" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="F183" s="1">
         <v>25</v>
@@ -7204,19 +7204,19 @@
     </row>
     <row r="184" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="F184" s="1">
         <v>20</v>
@@ -7227,19 +7227,19 @@
     </row>
     <row r="185" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C185" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>744</v>
-      </c>
       <c r="D185" s="1" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="F185" s="1">
         <v>30</v>
@@ -7250,19 +7250,19 @@
     </row>
     <row r="186" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D186" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C186" s="1" t="s">
-        <v>791</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="E186" s="3" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="F186" s="1">
         <v>5</v>
@@ -7273,19 +7273,19 @@
     </row>
     <row r="187" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="F187" s="1">
         <v>50</v>
@@ -7296,19 +7296,19 @@
     </row>
     <row r="188" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="F188" s="1">
         <v>5</v>
@@ -7319,19 +7319,19 @@
     </row>
     <row r="189" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="F189" s="1">
         <v>5</v>
@@ -7342,19 +7342,19 @@
     </row>
     <row r="190" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="F190" s="1">
         <v>5</v>
@@ -7365,19 +7365,19 @@
     </row>
     <row r="191" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="F191" s="1">
         <v>5</v>
@@ -7388,19 +7388,19 @@
     </row>
     <row r="192" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="F192" s="1">
         <v>130</v>
@@ -7411,19 +7411,19 @@
     </row>
     <row r="193" spans="1:7" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="F193" s="1">
         <v>10</v>
@@ -7434,19 +7434,19 @@
     </row>
     <row r="194" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F194" s="1">
         <v>150</v>
@@ -7457,19 +7457,19 @@
     </row>
     <row r="195" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="F195" s="1">
         <v>100</v>
@@ -7480,19 +7480,19 @@
     </row>
     <row r="196" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="F196" s="1">
         <v>90</v>

</xml_diff>